<commit_message>
added styling, fixed users seeing all posts.
</commit_message>
<xml_diff>
--- a/rptTerminalStatusCassetteBalances.xlsx
+++ b/rptTerminalStatusCassetteBalances.xlsx
@@ -478,34 +478,34 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>LK644532</v>
+        <v>L474792</v>
       </c>
       <c r="C5" t="str">
-        <v>SCL ENTERPRISES LAUNDRY</v>
+        <v>NICK SHELL SERVICE</v>
       </c>
       <c r="E5">
-        <v>1260</v>
+        <v>560</v>
       </c>
       <c r="F5" t="str">
         <v>T</v>
       </c>
       <c r="H5">
-        <v>45115.04184097222</v>
+        <v>45095.04187195602</v>
       </c>
       <c r="J5" t="str">
-        <v>06/05/23 19:53</v>
+        <v>06/13/23 11:00</v>
       </c>
       <c r="K5" t="str">
-        <v>06/05/23 19:53</v>
+        <v>06/13/23 11:00</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="M5" t="str">
-        <v>$1,260 as of 6/5/2023 5:53:05 PM</v>
+        <v>$560 as of 6/13/2023 9:00:01 AM</v>
       </c>
       <c r="N5">
-        <v>1300</v>
+        <v>700</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -519,31 +519,34 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>L682801</v>
+        <v>LK644532</v>
       </c>
       <c r="C6" t="str">
-        <v>SB#5</v>
+        <v>SCL ENTERPRISES LAUNDRY</v>
       </c>
       <c r="E6">
-        <v>1380</v>
+        <v>880</v>
       </c>
       <c r="F6" t="str">
         <v>T</v>
       </c>
+      <c r="H6">
+        <v>45106.04187195602</v>
+      </c>
       <c r="J6" t="str">
-        <v>06/06/23 18:58</v>
+        <v>06/12/23 19:34</v>
       </c>
       <c r="K6" t="str">
-        <v>06/06/23 18:58</v>
+        <v>06/12/23 19:34</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6" t="str">
-        <v>$1,880 as of 6/5/2023 4:37:14 PM</v>
+        <v>$880 as of 6/12/2023 5:34:00 PM</v>
       </c>
       <c r="N6">
-        <v>1580</v>
+        <v>920</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -557,34 +560,34 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>L488595</v>
+        <v>L647934</v>
       </c>
       <c r="C7" t="str">
-        <v>N S MART</v>
+        <v>SB #6</v>
       </c>
       <c r="E7">
-        <v>1640</v>
+        <v>1940</v>
       </c>
       <c r="F7" t="str">
         <v>T</v>
       </c>
-      <c r="H7">
-        <v>45101.04184097222</v>
+      <c r="I7" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J7" t="str">
-        <v>06/06/23 13:48</v>
+        <v>04/06/23 22:10</v>
       </c>
       <c r="K7" t="str">
-        <v>06/06/23 13:48</v>
+        <v>04/06/23 22:05</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M7" t="str">
-        <v>$1,640 as of 6/6/2023 11:48:14 AM</v>
+        <v>$1,940 as of 4/6/2023 8:05:45 PM</v>
       </c>
       <c r="N7">
-        <v>1660</v>
+        <v>1960</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -598,34 +601,37 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>L474761</v>
+        <v>L688961</v>
       </c>
       <c r="C8" t="str">
-        <v>BABS MARKET</v>
+        <v>MONA MART</v>
       </c>
       <c r="E8">
-        <v>1780</v>
+        <v>2640</v>
       </c>
       <c r="F8" t="str">
         <v>T</v>
       </c>
       <c r="H8">
-        <v>45090.04184097222</v>
+        <v>45167.04187195602</v>
+      </c>
+      <c r="I8" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J8" t="str">
-        <v>06/05/23 23:14</v>
+        <v>06/13/23 14:33</v>
       </c>
       <c r="K8" t="str">
-        <v>06/05/23 23:14</v>
+        <v>06/09/23 16:00</v>
       </c>
       <c r="L8">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M8" t="str">
-        <v>$1,780 as of 6/5/2023 9:14:39 PM</v>
+        <v>$2,640 as of 6/9/2023 2:00:40 PM</v>
       </c>
       <c r="N8">
-        <v>1880</v>
+        <v>2640</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -639,34 +645,34 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>L647934</v>
+        <v>LK561655</v>
       </c>
       <c r="C9" t="str">
-        <v>SB #6</v>
+        <v>CRENSHAW CRAVOR #2</v>
       </c>
       <c r="E9">
-        <v>1940</v>
+        <v>2780</v>
       </c>
       <c r="F9" t="str">
         <v>T</v>
       </c>
       <c r="I9" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+        <v>ATM Inactive greater than 48 minutes</v>
       </c>
       <c r="J9" t="str">
-        <v>04/06/23 22:10</v>
+        <v>01/23/20 08:24</v>
       </c>
       <c r="K9" t="str">
-        <v>04/06/23 22:05</v>
+        <v>01/23/20 08:24</v>
       </c>
       <c r="L9">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M9" t="str">
-        <v>$1,940 as of 4/6/2023 8:05:45 PM</v>
+        <v>$2,780 as of 1/23/2020 6:24:32 AM</v>
       </c>
       <c r="N9">
-        <v>1960</v>
+        <v>2800</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -680,34 +686,34 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>L474792</v>
+        <v>L678988</v>
       </c>
       <c r="C10" t="str">
-        <v>NICK SHELL SERVICE</v>
+        <v>PAYELESS MARKET</v>
       </c>
       <c r="E10">
-        <v>2240</v>
+        <v>3000</v>
       </c>
       <c r="F10" t="str">
         <v>T</v>
       </c>
       <c r="H10">
-        <v>45099.04184097222</v>
+        <v>45105.04187195602</v>
       </c>
       <c r="J10" t="str">
-        <v>06/06/23 14:52</v>
+        <v>06/12/23 15:37</v>
       </c>
       <c r="K10" t="str">
-        <v>06/06/23 14:52</v>
+        <v>06/12/23 15:37</v>
       </c>
       <c r="L10">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="M10" t="str">
-        <v>$2,400 as of 6/2/2023 10:58:37 AM</v>
+        <v>$3,000 as of 6/12/2023 1:37:03 PM</v>
       </c>
       <c r="N10">
-        <v>2300</v>
+        <v>3000</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -721,34 +727,34 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>L476340</v>
+        <v>L475182</v>
       </c>
       <c r="C11" t="str">
-        <v>DONUT &amp; SANDWICH</v>
+        <v>LA ESQUINA DE ORO</v>
       </c>
       <c r="E11">
-        <v>2400</v>
+        <v>3800</v>
       </c>
       <c r="F11" t="str">
         <v>T</v>
       </c>
-      <c r="H11">
-        <v>45091.04184097222</v>
+      <c r="I11" t="str">
+        <v>ATM Inactive greater than 48 minutes</v>
       </c>
       <c r="J11" t="str">
-        <v>06/06/23 18:24</v>
+        <v>09/16/20 16:57</v>
       </c>
       <c r="K11" t="str">
-        <v>06/06/23 18:24</v>
+        <v>09/15/20 23:38</v>
       </c>
       <c r="L11">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M11" t="str">
-        <v>$2,440 as of 6/5/2023 3:15:01 PM</v>
+        <v>$3,800 as of 9/16/2020 1:28:00 PM</v>
       </c>
       <c r="N11">
-        <v>2400</v>
+        <v>3800</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -762,34 +768,34 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>L474746</v>
+        <v>L682801</v>
       </c>
       <c r="C12" t="str">
-        <v>ZACATES MARKET</v>
+        <v>SB#5</v>
       </c>
       <c r="E12">
-        <v>2460</v>
+        <v>3880</v>
       </c>
       <c r="F12" t="str">
         <v>T</v>
       </c>
       <c r="H12">
-        <v>45089.04184097222</v>
+        <v>45106.04187195602</v>
       </c>
       <c r="J12" t="str">
-        <v>06/06/23 17:07</v>
+        <v>06/13/23 16:25</v>
       </c>
       <c r="K12" t="str">
-        <v>06/06/23 17:07</v>
+        <v>06/13/23 16:25</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12" t="str">
-        <v>$2,660 as of 6/6/2023 11:30:18 AM</v>
+        <v>$4,020 as of 6/12/2023 6:05:36 PM</v>
       </c>
       <c r="N12">
-        <v>2500</v>
+        <v>3920</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -803,34 +809,34 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>LK561655</v>
+        <v>LK236828</v>
       </c>
       <c r="C13" t="str">
-        <v>CRENSHAW CRAVOR #2</v>
+        <v>WORLDWIDE AUTOMOTIVE</v>
       </c>
       <c r="E13">
-        <v>2780</v>
+        <v>5320</v>
       </c>
       <c r="F13" t="str">
         <v>T</v>
       </c>
-      <c r="I13" t="str">
-        <v>ATM Inactive greater than 48 minutes</v>
+      <c r="H13">
+        <v>45113.04187195602</v>
       </c>
       <c r="J13" t="str">
-        <v>01/23/20 08:24</v>
+        <v>06/12/23 20:28</v>
       </c>
       <c r="K13" t="str">
-        <v>01/23/20 08:24</v>
+        <v>06/12/23 20:28</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="M13" t="str">
-        <v>$2,780 as of 1/23/2020 6:24:32 AM</v>
+        <v>$5,320 as of 6/12/2023 6:28:00 PM</v>
       </c>
       <c r="N13">
-        <v>2800</v>
+        <v>5360</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -844,37 +850,34 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>L688961</v>
+        <v>L662336</v>
       </c>
       <c r="C14" t="str">
-        <v>MONA MART</v>
+        <v>SB#4 MONA MARKET</v>
       </c>
       <c r="E14">
-        <v>2880</v>
+        <v>6080</v>
       </c>
       <c r="F14" t="str">
         <v>T</v>
       </c>
       <c r="H14">
-        <v>45127.04184097222</v>
-      </c>
-      <c r="I14" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+        <v>45117.04187195602</v>
       </c>
       <c r="J14" t="str">
-        <v>06/06/23 16:03</v>
+        <v>06/13/23 16:48</v>
       </c>
       <c r="K14" t="str">
-        <v>06/04/23 21:44</v>
+        <v>06/13/23 15:07</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14" t="str">
-        <v>$2,880 as of 6/4/2023 7:44:47 PM</v>
+        <v>$6,220 as of 6/13/2023 8:24:02 AM</v>
       </c>
       <c r="N14">
-        <v>2880</v>
+        <v>6080</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -888,34 +891,34 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>L678988</v>
+        <v>L474817</v>
       </c>
       <c r="C15" t="str">
-        <v>PAYELESS MARKET</v>
+        <v>SAFETY MARKET</v>
       </c>
       <c r="E15">
-        <v>3520</v>
+        <v>6320</v>
       </c>
       <c r="F15" t="str">
         <v>T</v>
       </c>
       <c r="H15">
-        <v>45095.04184097222</v>
+        <v>45099.04187195602</v>
       </c>
       <c r="J15" t="str">
-        <v>06/06/23 15:00</v>
+        <v>06/13/23 16:26</v>
       </c>
       <c r="K15" t="str">
-        <v>06/06/23 15:00</v>
+        <v>06/13/23 15:26</v>
       </c>
       <c r="L15">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M15" t="str">
-        <v>$3,840 as of 6/5/2023 6:33:06 PM</v>
+        <v>$6,440 as of 6/13/2023 7:36:23 AM</v>
       </c>
       <c r="N15">
-        <v>3720</v>
+        <v>6320</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -929,34 +932,37 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>LK236828</v>
+        <v>L488595</v>
       </c>
       <c r="C16" t="str">
-        <v>WORLDWIDE AUTOMOTIVE</v>
+        <v>N S MART</v>
       </c>
       <c r="E16">
-        <v>3620</v>
+        <v>6480</v>
       </c>
       <c r="F16" t="str">
         <v>T</v>
       </c>
       <c r="H16">
-        <v>45098.04184097222</v>
+        <v>45128.04187195602</v>
+      </c>
+      <c r="I16" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J16" t="str">
-        <v>06/06/23 10:23</v>
+        <v>06/12/23 15:05</v>
       </c>
       <c r="K16" t="str">
-        <v>06/05/23 17:41</v>
+        <v>06/11/23 21:53</v>
       </c>
       <c r="L16">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="M16" t="str">
-        <v>$3,620 as of 6/6/2023 8:23:22 AM</v>
+        <v>$6,480 as of 6/11/2023 7:53:56 PM</v>
       </c>
       <c r="N16">
-        <v>3620</v>
+        <v>6480</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -970,34 +976,34 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>L475182</v>
+        <v>L476340</v>
       </c>
       <c r="C17" t="str">
-        <v>LA ESQUINA DE ORO</v>
+        <v>DONUT &amp; SANDWICH</v>
       </c>
       <c r="E17">
-        <v>3800</v>
+        <v>6620</v>
       </c>
       <c r="F17" t="str">
         <v>T</v>
       </c>
-      <c r="I17" t="str">
-        <v>ATM Inactive greater than 48 minutes</v>
+      <c r="H17">
+        <v>45117.04187195602</v>
       </c>
       <c r="J17" t="str">
-        <v>09/16/20 16:57</v>
+        <v>06/13/23 14:15</v>
       </c>
       <c r="K17" t="str">
-        <v>09/15/20 23:38</v>
+        <v>06/13/23 14:15</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="M17" t="str">
-        <v>$3,800 as of 9/16/2020 1:28:00 PM</v>
+        <v>$6,660 as of 6/13/2023 5:11:45 AM</v>
       </c>
       <c r="N17">
-        <v>3800</v>
+        <v>6660</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1011,34 +1017,34 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>L662336</v>
+        <v>L474746</v>
       </c>
       <c r="C18" t="str">
-        <v>SB#4 MONA MARKET</v>
+        <v>ZACATES MARKET</v>
       </c>
       <c r="E18">
-        <v>3960</v>
+        <v>6780</v>
       </c>
       <c r="F18" t="str">
         <v>T</v>
       </c>
       <c r="H18">
-        <v>45090.04184097222</v>
+        <v>45115.04187195602</v>
       </c>
       <c r="J18" t="str">
-        <v>06/06/23 18:32</v>
+        <v>06/12/23 19:10</v>
       </c>
       <c r="K18" t="str">
-        <v>06/06/23 18:32</v>
+        <v>06/12/23 19:10</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18" t="str">
-        <v>$4,020 as of 6/6/2023 11:34:08 AM</v>
+        <v>$6,780 as of 6/12/2023 5:10:31 PM</v>
       </c>
       <c r="N18">
-        <v>4020</v>
+        <v>6840</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -1052,34 +1058,34 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>L474817</v>
+        <v>L697590</v>
       </c>
       <c r="C19" t="str">
-        <v>SAFETY MARKET</v>
+        <v>S B MARKET ST</v>
       </c>
       <c r="E19">
-        <v>4720</v>
+        <v>6900</v>
       </c>
       <c r="F19" t="str">
         <v>T</v>
       </c>
       <c r="H19">
-        <v>45095.04184097222</v>
+        <v>45103.04187195602</v>
       </c>
       <c r="J19" t="str">
-        <v>06/06/23 16:00</v>
+        <v>06/13/23 16:35</v>
       </c>
       <c r="K19" t="str">
-        <v>06/06/23 16:00</v>
+        <v>06/13/23 16:35</v>
       </c>
       <c r="L19">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M19" t="str">
-        <v>$4,740 as of 6/6/2023 9:34:47 AM</v>
+        <v>$7,060 as of 6/13/2023 4:03:51 AM</v>
       </c>
       <c r="N19">
-        <v>4740</v>
+        <v>6920</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1093,34 +1099,34 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>L475090</v>
+        <v>LK864765</v>
       </c>
       <c r="C20" t="str">
-        <v>S.B. 2</v>
+        <v>SKY LIQUOR</v>
       </c>
       <c r="E20">
-        <v>5020</v>
+        <v>7120</v>
       </c>
       <c r="F20" t="str">
         <v>T</v>
       </c>
       <c r="H20">
-        <v>45090.04184097222</v>
+        <v>45103.04187195602</v>
       </c>
       <c r="J20" t="str">
-        <v>06/06/23 17:58</v>
+        <v>06/13/23 16:41</v>
       </c>
       <c r="K20" t="str">
-        <v>06/06/23 17:58</v>
+        <v>06/13/23 16:41</v>
       </c>
       <c r="L20">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M20" t="str">
-        <v>$5,960 as of 6/6/2023 10:27:47 AM</v>
+        <v>$7,340 as of 6/13/2023 11:29:34 AM</v>
       </c>
       <c r="N20">
-        <v>5000</v>
+        <v>7120</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -1134,34 +1140,34 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>LK864765</v>
+        <v>L474761</v>
       </c>
       <c r="C21" t="str">
-        <v>SKY LIQUOR</v>
+        <v>BABS MARKET</v>
       </c>
       <c r="E21">
-        <v>5460</v>
+        <v>7180</v>
       </c>
       <c r="F21" t="str">
         <v>T</v>
       </c>
       <c r="H21">
-        <v>45091.04184097222</v>
+        <v>45156.04187195602</v>
       </c>
       <c r="J21" t="str">
-        <v>06/06/23 18:24</v>
+        <v>06/12/23 20:20</v>
       </c>
       <c r="K21" t="str">
-        <v>06/06/23 15:55</v>
+        <v>06/12/23 20:20</v>
       </c>
       <c r="L21">
-        <v>700</v>
+        <v>40</v>
       </c>
       <c r="M21" t="str">
-        <v>$6,300 as of 6/6/2023 10:20:08 AM</v>
+        <v>$7,180 as of 6/12/2023 6:20:05 PM</v>
       </c>
       <c r="N21">
-        <v>6160</v>
+        <v>7220</v>
       </c>
       <c r="O21">
         <v>0</v>
@@ -1175,34 +1181,37 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>L697589</v>
+        <v>L688966</v>
       </c>
       <c r="C22" t="str">
-        <v>S B DISCOUNT MART</v>
+        <v>LACON MINI MART</v>
       </c>
       <c r="E22">
-        <v>6220</v>
+        <v>7300</v>
       </c>
       <c r="F22" t="str">
         <v>T</v>
       </c>
       <c r="H22">
-        <v>45088.04184097222</v>
+        <v>45165.04187195602</v>
+      </c>
+      <c r="I22" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J22" t="str">
-        <v>06/06/23 13:18</v>
+        <v>06/11/23 15:48</v>
       </c>
       <c r="K22" t="str">
-        <v>06/06/23 13:18</v>
+        <v>06/11/23 15:48</v>
       </c>
       <c r="L22">
         <v>20</v>
       </c>
       <c r="M22" t="str">
-        <v>$6,220 as of 6/6/2023 11:18:17 AM</v>
+        <v>$7,300 as of 6/11/2023 1:48:15 PM</v>
       </c>
       <c r="N22">
-        <v>6220</v>
+        <v>7400</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -1216,34 +1225,34 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>LK923383</v>
+        <v>L697589</v>
       </c>
       <c r="C23" t="str">
-        <v>SAMYS PHONE CARDS</v>
+        <v>S B DISCOUNT MART</v>
       </c>
       <c r="E23">
-        <v>7820</v>
+        <v>7740</v>
       </c>
       <c r="F23" t="str">
         <v>T</v>
       </c>
       <c r="H23">
-        <v>45092.04184097222</v>
+        <v>45096.04187195602</v>
       </c>
       <c r="J23" t="str">
-        <v>06/06/23 15:58</v>
+        <v>06/13/23 10:33</v>
       </c>
       <c r="K23" t="str">
-        <v>06/05/23 22:17</v>
+        <v>06/13/23 10:33</v>
       </c>
       <c r="L23">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="M23" t="str">
-        <v>$7,820 as of 6/5/2023 8:17:28 PM</v>
+        <v>$7,740 as of 6/13/2023 8:33:20 AM</v>
       </c>
       <c r="N23">
-        <v>7820</v>
+        <v>7780</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -1257,37 +1266,34 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>L688966</v>
+        <v>LK923383</v>
       </c>
       <c r="C24" t="str">
-        <v>LACON MINI MART</v>
+        <v>SAMYS PHONE CARDS</v>
       </c>
       <c r="E24">
-        <v>7980</v>
+        <v>10220</v>
       </c>
       <c r="F24" t="str">
         <v>T</v>
       </c>
       <c r="H24">
-        <v>45210.04184097222</v>
-      </c>
-      <c r="I24" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+        <v>45104.04187195602</v>
       </c>
       <c r="J24" t="str">
-        <v>06/04/23 22:12</v>
+        <v>06/12/23 22:27</v>
       </c>
       <c r="K24" t="str">
-        <v>06/04/23 22:12</v>
+        <v>06/12/23 22:27</v>
       </c>
       <c r="L24">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="M24" t="str">
-        <v>$7,980 as of 6/4/2023 8:12:54 PM</v>
+        <v>$10,220 as of 6/12/2023 8:27:39 PM</v>
       </c>
       <c r="N24">
-        <v>8000</v>
+        <v>10320</v>
       </c>
       <c r="O24">
         <v>0</v>
@@ -1301,34 +1307,34 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>L697590</v>
+        <v>L475090</v>
       </c>
       <c r="C25" t="str">
-        <v>S B MARKET ST</v>
+        <v>S.B. 2</v>
       </c>
       <c r="E25">
-        <v>10240</v>
+        <v>13420</v>
       </c>
       <c r="F25" t="str">
         <v>T</v>
       </c>
       <c r="H25">
-        <v>45101.04184097222</v>
+        <v>45107.04187195602</v>
       </c>
       <c r="J25" t="str">
-        <v>06/06/23 12:36</v>
+        <v>06/13/23 16:30</v>
       </c>
       <c r="K25" t="str">
-        <v>06/06/23 12:36</v>
+        <v>06/13/23 14:25</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25" t="str">
-        <v>$10,240 as of 6/6/2023 10:36:31 AM</v>
+        <v>$13,620 as of 6/13/2023 11:54:34 AM</v>
       </c>
       <c r="N25">
-        <v>10240</v>
+        <v>13320</v>
       </c>
       <c r="O25">
         <v>0</v>
@@ -1348,28 +1354,28 @@
         <v>98 DISCOUNT STORE</v>
       </c>
       <c r="E26">
-        <v>17940</v>
+        <v>23220</v>
       </c>
       <c r="F26" t="str">
         <v>T</v>
       </c>
       <c r="H26">
-        <v>45090.04184097222</v>
+        <v>45103.04187195602</v>
       </c>
       <c r="J26" t="str">
-        <v>06/06/23 18:29</v>
+        <v>06/13/23 16:38</v>
       </c>
       <c r="K26" t="str">
-        <v>06/06/23 18:05</v>
+        <v>06/13/23 16:38</v>
       </c>
       <c r="L26">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="M26" t="str">
-        <v>$18,640 as of 6/6/2023 11:32:33 AM</v>
+        <v>$23,440 as of 6/13/2023 11:03:04 AM</v>
       </c>
       <c r="N26">
-        <v>17960</v>
+        <v>23420</v>
       </c>
       <c r="O26">
         <v>0</v>
@@ -1386,7 +1392,7 @@
         <v>Total Outstanding Cash Balance:</v>
       </c>
       <c r="E27">
-        <v>101060</v>
+        <v>140180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
show previous values while updates process
</commit_message>
<xml_diff>
--- a/rptTerminalStatusCassetteBalances.xlsx
+++ b/rptTerminalStatusCassetteBalances.xlsx
@@ -478,34 +478,37 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>L474792</v>
+        <v>LK644532</v>
       </c>
       <c r="C5" t="str">
-        <v>NICK SHELL SERVICE</v>
+        <v>SCL ENTERPRISES LAUNDRY</v>
       </c>
       <c r="E5">
-        <v>560</v>
+        <v>880</v>
       </c>
       <c r="F5" t="str">
         <v>T</v>
       </c>
       <c r="H5">
-        <v>45095.04187195602</v>
+        <v>45118.04186157407</v>
+      </c>
+      <c r="I5" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J5" t="str">
-        <v>06/13/23 11:00</v>
+        <v>06/15/23 13:10</v>
       </c>
       <c r="K5" t="str">
-        <v>06/13/23 11:00</v>
+        <v>06/12/23 19:34</v>
       </c>
       <c r="L5">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="M5" t="str">
-        <v>$560 as of 6/13/2023 9:00:01 AM</v>
+        <v>$880 as of 6/15/2023 11:10:11 AM</v>
       </c>
       <c r="N5">
-        <v>700</v>
+        <v>880</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -519,34 +522,34 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>LK644532</v>
+        <v>L647934</v>
       </c>
       <c r="C6" t="str">
-        <v>SCL ENTERPRISES LAUNDRY</v>
+        <v>SB #6</v>
       </c>
       <c r="E6">
-        <v>880</v>
+        <v>1940</v>
       </c>
       <c r="F6" t="str">
         <v>T</v>
       </c>
-      <c r="H6">
-        <v>45106.04187195602</v>
+      <c r="I6" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J6" t="str">
-        <v>06/12/23 19:34</v>
+        <v>04/06/23 22:10</v>
       </c>
       <c r="K6" t="str">
-        <v>06/12/23 19:34</v>
+        <v>04/06/23 22:05</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M6" t="str">
-        <v>$880 as of 6/12/2023 5:34:00 PM</v>
+        <v>$1,940 as of 4/6/2023 8:05:45 PM</v>
       </c>
       <c r="N6">
-        <v>920</v>
+        <v>1960</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -560,34 +563,34 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>L647934</v>
+        <v>L678988</v>
       </c>
       <c r="C7" t="str">
-        <v>SB #6</v>
+        <v>PAYELESS MARKET</v>
       </c>
       <c r="E7">
-        <v>1940</v>
+        <v>2440</v>
       </c>
       <c r="F7" t="str">
         <v>T</v>
       </c>
-      <c r="I7" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+      <c r="H7">
+        <v>45137.04186157407</v>
       </c>
       <c r="J7" t="str">
-        <v>04/06/23 22:10</v>
+        <v>06/15/23 14:31</v>
       </c>
       <c r="K7" t="str">
-        <v>04/06/23 22:05</v>
+        <v>06/14/23 20:13</v>
       </c>
       <c r="L7">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M7" t="str">
-        <v>$1,940 as of 4/6/2023 8:05:45 PM</v>
+        <v>$2,440 as of 6/14/2023 6:13:48 PM</v>
       </c>
       <c r="N7">
-        <v>1960</v>
+        <v>2440</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -607,31 +610,28 @@
         <v>MONA MART</v>
       </c>
       <c r="E8">
-        <v>2640</v>
+        <v>2600</v>
       </c>
       <c r="F8" t="str">
         <v>T</v>
       </c>
       <c r="H8">
-        <v>45167.04187195602</v>
-      </c>
-      <c r="I8" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+        <v>45157.04186157407</v>
       </c>
       <c r="J8" t="str">
-        <v>06/13/23 14:33</v>
+        <v>06/15/23 13:15</v>
       </c>
       <c r="K8" t="str">
-        <v>06/09/23 16:00</v>
+        <v>06/14/23 12:41</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8" t="str">
-        <v>$2,640 as of 6/9/2023 2:00:40 PM</v>
+        <v>$2,600 as of 6/15/2023 11:15:09 AM</v>
       </c>
       <c r="N8">
-        <v>2640</v>
+        <v>2600</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -686,34 +686,34 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>L678988</v>
+        <v>L682801</v>
       </c>
       <c r="C10" t="str">
-        <v>PAYELESS MARKET</v>
+        <v>SB#5</v>
       </c>
       <c r="E10">
-        <v>3000</v>
+        <v>3440</v>
       </c>
       <c r="F10" t="str">
         <v>T</v>
       </c>
       <c r="H10">
-        <v>45105.04187195602</v>
+        <v>45107.04186157407</v>
       </c>
       <c r="J10" t="str">
-        <v>06/12/23 15:37</v>
+        <v>06/15/23 15:26</v>
       </c>
       <c r="K10" t="str">
-        <v>06/12/23 15:37</v>
+        <v>06/15/23 15:26</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10" t="str">
-        <v>$3,000 as of 6/12/2023 1:37:03 PM</v>
+        <v>$3,560 as of 6/14/2023 9:52:10 AM</v>
       </c>
       <c r="N10">
-        <v>3000</v>
+        <v>3540</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -768,34 +768,37 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>L682801</v>
+        <v>L474792</v>
       </c>
       <c r="C12" t="str">
-        <v>SB#5</v>
+        <v>NICK SHELL SERVICE</v>
       </c>
       <c r="E12">
-        <v>3880</v>
+        <v>4500</v>
       </c>
       <c r="F12" t="str">
         <v>T</v>
       </c>
       <c r="H12">
-        <v>45106.04187195602</v>
+        <v>45111.04186157407</v>
+      </c>
+      <c r="I12" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J12" t="str">
-        <v>06/13/23 16:25</v>
+        <v>06/14/23 12:44</v>
       </c>
       <c r="K12" t="str">
-        <v>06/13/23 16:25</v>
+        <v>06/13/23 11:00</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12" t="str">
-        <v>$4,020 as of 6/12/2023 6:05:36 PM</v>
+        <v>$4,500 as of 6/13/2023 9:00:01 AM</v>
       </c>
       <c r="N12">
-        <v>3920</v>
+        <v>4500</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -815,28 +818,28 @@
         <v>WORLDWIDE AUTOMOTIVE</v>
       </c>
       <c r="E13">
-        <v>5320</v>
+        <v>5140</v>
       </c>
       <c r="F13" t="str">
         <v>T</v>
       </c>
       <c r="H13">
-        <v>45113.04187195602</v>
+        <v>45109.04186157407</v>
       </c>
       <c r="J13" t="str">
-        <v>06/12/23 20:28</v>
+        <v>06/14/23 20:04</v>
       </c>
       <c r="K13" t="str">
-        <v>06/12/23 20:28</v>
+        <v>06/14/23 20:04</v>
       </c>
       <c r="L13">
         <v>80</v>
       </c>
       <c r="M13" t="str">
-        <v>$5,320 as of 6/12/2023 6:28:00 PM</v>
+        <v>$5,140 as of 6/14/2023 6:04:04 PM</v>
       </c>
       <c r="N13">
-        <v>5360</v>
+        <v>5180</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -850,34 +853,34 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>L662336</v>
+        <v>L474817</v>
       </c>
       <c r="C14" t="str">
-        <v>SB#4 MONA MARKET</v>
+        <v>SAFETY MARKET</v>
       </c>
       <c r="E14">
-        <v>6080</v>
+        <v>5320</v>
       </c>
       <c r="F14" t="str">
         <v>T</v>
       </c>
       <c r="H14">
-        <v>45117.04187195602</v>
+        <v>45100.04186157407</v>
       </c>
       <c r="J14" t="str">
-        <v>06/13/23 16:48</v>
+        <v>06/15/23 10:14</v>
       </c>
       <c r="K14" t="str">
-        <v>06/13/23 15:07</v>
+        <v>06/15/23 00:10</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M14" t="str">
-        <v>$6,220 as of 6/13/2023 8:24:02 AM</v>
+        <v>$5,320 as of 6/15/2023 8:14:03 AM</v>
       </c>
       <c r="N14">
-        <v>6080</v>
+        <v>5320</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -891,34 +894,34 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>L474817</v>
+        <v>L662336</v>
       </c>
       <c r="C15" t="str">
-        <v>SAFETY MARKET</v>
+        <v>SB#4 MONA MARKET</v>
       </c>
       <c r="E15">
-        <v>6320</v>
+        <v>5700</v>
       </c>
       <c r="F15" t="str">
         <v>T</v>
       </c>
       <c r="H15">
-        <v>45099.04187195602</v>
+        <v>45117.04186157407</v>
       </c>
       <c r="J15" t="str">
-        <v>06/13/23 16:26</v>
+        <v>06/15/23 09:34</v>
       </c>
       <c r="K15" t="str">
-        <v>06/13/23 15:26</v>
+        <v>06/15/23 09:34</v>
       </c>
       <c r="L15">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M15" t="str">
-        <v>$6,440 as of 6/13/2023 7:36:23 AM</v>
+        <v>$5,700 as of 6/15/2023 7:34:59 AM</v>
       </c>
       <c r="N15">
-        <v>6320</v>
+        <v>5780</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -932,37 +935,34 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>L488595</v>
+        <v>LK864765</v>
       </c>
       <c r="C16" t="str">
-        <v>N S MART</v>
+        <v>SKY LIQUOR</v>
       </c>
       <c r="E16">
-        <v>6480</v>
+        <v>6080</v>
       </c>
       <c r="F16" t="str">
         <v>T</v>
       </c>
       <c r="H16">
-        <v>45128.04187195602</v>
-      </c>
-      <c r="I16" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+        <v>45102.04186157407</v>
       </c>
       <c r="J16" t="str">
-        <v>06/12/23 15:05</v>
+        <v>06/15/23 15:27</v>
       </c>
       <c r="K16" t="str">
-        <v>06/11/23 21:53</v>
+        <v>06/15/23 01:51</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16" t="str">
-        <v>$6,480 as of 6/11/2023 7:53:56 PM</v>
+        <v>$6,080 as of 6/14/2023 11:51:34 PM</v>
       </c>
       <c r="N16">
-        <v>6480</v>
+        <v>6080</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -976,34 +976,34 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>L476340</v>
+        <v>L697589</v>
       </c>
       <c r="C17" t="str">
-        <v>DONUT &amp; SANDWICH</v>
+        <v>S B DISCOUNT MART</v>
       </c>
       <c r="E17">
-        <v>6620</v>
+        <v>6120</v>
       </c>
       <c r="F17" t="str">
         <v>T</v>
       </c>
       <c r="H17">
-        <v>45117.04187195602</v>
+        <v>45097.04186157407</v>
       </c>
       <c r="J17" t="str">
-        <v>06/13/23 14:15</v>
+        <v>06/15/23 12:55</v>
       </c>
       <c r="K17" t="str">
-        <v>06/13/23 14:15</v>
+        <v>06/15/23 12:55</v>
       </c>
       <c r="L17">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="M17" t="str">
-        <v>$6,660 as of 6/13/2023 5:11:45 AM</v>
+        <v>$6,120 as of 6/15/2023 10:55:35 AM</v>
       </c>
       <c r="N17">
-        <v>6660</v>
+        <v>6220</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1017,34 +1017,34 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>L474746</v>
+        <v>L697590</v>
       </c>
       <c r="C18" t="str">
-        <v>ZACATES MARKET</v>
+        <v>S B MARKET ST</v>
       </c>
       <c r="E18">
-        <v>6780</v>
+        <v>6320</v>
       </c>
       <c r="F18" t="str">
         <v>T</v>
       </c>
       <c r="H18">
-        <v>45115.04187195602</v>
+        <v>45108.04186157407</v>
       </c>
       <c r="J18" t="str">
-        <v>06/12/23 19:10</v>
+        <v>06/15/23 15:25</v>
       </c>
       <c r="K18" t="str">
-        <v>06/12/23 19:10</v>
+        <v>06/15/23 15:25</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18" t="str">
-        <v>$6,780 as of 6/12/2023 5:10:31 PM</v>
+        <v>$6,440 as of 6/15/2023 8:05:20 AM</v>
       </c>
       <c r="N18">
-        <v>6840</v>
+        <v>6340</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -1058,34 +1058,34 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>L697590</v>
+        <v>L476340</v>
       </c>
       <c r="C19" t="str">
-        <v>S B MARKET ST</v>
+        <v>DONUT &amp; SANDWICH</v>
       </c>
       <c r="E19">
-        <v>6900</v>
+        <v>6360</v>
       </c>
       <c r="F19" t="str">
         <v>T</v>
       </c>
       <c r="H19">
-        <v>45103.04187195602</v>
+        <v>45121.04186157407</v>
       </c>
       <c r="J19" t="str">
-        <v>06/13/23 16:35</v>
+        <v>06/15/23 15:21</v>
       </c>
       <c r="K19" t="str">
-        <v>06/13/23 16:35</v>
+        <v>06/15/23 15:21</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="M19" t="str">
-        <v>$7,060 as of 6/13/2023 4:03:51 AM</v>
+        <v>$6,540 as of 6/15/2023 9:59:33 AM</v>
       </c>
       <c r="N19">
-        <v>6920</v>
+        <v>6460</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1099,34 +1099,34 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>LK864765</v>
+        <v>L488595</v>
       </c>
       <c r="C20" t="str">
-        <v>SKY LIQUOR</v>
+        <v>N S MART</v>
       </c>
       <c r="E20">
-        <v>7120</v>
+        <v>6360</v>
       </c>
       <c r="F20" t="str">
         <v>T</v>
       </c>
       <c r="H20">
-        <v>45103.04187195602</v>
+        <v>45132.04186157407</v>
       </c>
       <c r="J20" t="str">
-        <v>06/13/23 16:41</v>
+        <v>06/14/23 22:03</v>
       </c>
       <c r="K20" t="str">
-        <v>06/13/23 16:41</v>
+        <v>06/14/23 22:03</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20" t="str">
-        <v>$7,340 as of 6/13/2023 11:29:34 AM</v>
+        <v>$6,360 as of 6/14/2023 8:03:30 PM</v>
       </c>
       <c r="N20">
-        <v>7120</v>
+        <v>6420</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -1140,34 +1140,34 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>L474761</v>
+        <v>L474746</v>
       </c>
       <c r="C21" t="str">
-        <v>BABS MARKET</v>
+        <v>ZACATES MARKET</v>
       </c>
       <c r="E21">
-        <v>7180</v>
+        <v>6620</v>
       </c>
       <c r="F21" t="str">
         <v>T</v>
       </c>
       <c r="H21">
-        <v>45156.04187195602</v>
+        <v>45121.04186157407</v>
       </c>
       <c r="J21" t="str">
-        <v>06/12/23 20:20</v>
+        <v>06/14/23 18:38</v>
       </c>
       <c r="K21" t="str">
-        <v>06/12/23 20:20</v>
+        <v>06/14/23 18:38</v>
       </c>
       <c r="L21">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M21" t="str">
-        <v>$7,180 as of 6/12/2023 6:20:05 PM</v>
+        <v>$6,620 as of 6/14/2023 4:38:13 PM</v>
       </c>
       <c r="N21">
-        <v>7220</v>
+        <v>6680</v>
       </c>
       <c r="O21">
         <v>0</v>
@@ -1181,37 +1181,34 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>L688966</v>
+        <v>L474761</v>
       </c>
       <c r="C22" t="str">
-        <v>LACON MINI MART</v>
+        <v>BABS MARKET</v>
       </c>
       <c r="E22">
-        <v>7300</v>
+        <v>6920</v>
       </c>
       <c r="F22" t="str">
         <v>T</v>
       </c>
       <c r="H22">
-        <v>45165.04187195602</v>
-      </c>
-      <c r="I22" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+        <v>45168.04186157407</v>
       </c>
       <c r="J22" t="str">
-        <v>06/11/23 15:48</v>
+        <v>06/15/23 13:03</v>
       </c>
       <c r="K22" t="str">
-        <v>06/11/23 15:48</v>
+        <v>06/15/23 13:03</v>
       </c>
       <c r="L22">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="M22" t="str">
-        <v>$7,300 as of 6/11/2023 1:48:15 PM</v>
+        <v>$6,920 as of 6/15/2023 11:03:17 AM</v>
       </c>
       <c r="N22">
-        <v>7400</v>
+        <v>6980</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -1225,34 +1222,34 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>L697589</v>
+        <v>L688966</v>
       </c>
       <c r="C23" t="str">
-        <v>S B DISCOUNT MART</v>
+        <v>LACON MINI MART</v>
       </c>
       <c r="E23">
-        <v>7740</v>
+        <v>7260</v>
       </c>
       <c r="F23" t="str">
         <v>T</v>
       </c>
       <c r="H23">
-        <v>45096.04187195602</v>
+        <v>45180.04186157407</v>
       </c>
       <c r="J23" t="str">
-        <v>06/13/23 10:33</v>
+        <v>06/15/23 15:31</v>
       </c>
       <c r="K23" t="str">
-        <v>06/13/23 10:33</v>
+        <v>06/15/23 12:37</v>
       </c>
       <c r="L23">
         <v>20</v>
       </c>
       <c r="M23" t="str">
-        <v>$7,740 as of 6/13/2023 8:33:20 AM</v>
+        <v>$7,260 as of 6/15/2023 10:37:22 AM</v>
       </c>
       <c r="N23">
-        <v>7780</v>
+        <v>7260</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -1272,16 +1269,19 @@
         <v>SAMYS PHONE CARDS</v>
       </c>
       <c r="E24">
-        <v>10220</v>
+        <v>10120</v>
       </c>
       <c r="F24" t="str">
         <v>T</v>
       </c>
       <c r="H24">
-        <v>45104.04187195602</v>
+        <v>45106.04186157407</v>
+      </c>
+      <c r="I24" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J24" t="str">
-        <v>06/12/23 22:27</v>
+        <v>06/14/23 14:05</v>
       </c>
       <c r="K24" t="str">
         <v>06/12/23 22:27</v>
@@ -1290,10 +1290,10 @@
         <v>100</v>
       </c>
       <c r="M24" t="str">
-        <v>$10,220 as of 6/12/2023 8:27:39 PM</v>
+        <v>$10,120 as of 6/12/2023 8:27:39 PM</v>
       </c>
       <c r="N24">
-        <v>10320</v>
+        <v>10220</v>
       </c>
       <c r="O24">
         <v>0</v>
@@ -1313,28 +1313,28 @@
         <v>S.B. 2</v>
       </c>
       <c r="E25">
-        <v>13420</v>
+        <v>12260</v>
       </c>
       <c r="F25" t="str">
         <v>T</v>
       </c>
       <c r="H25">
-        <v>45107.04187195602</v>
+        <v>45114.04186157407</v>
       </c>
       <c r="J25" t="str">
-        <v>06/13/23 16:30</v>
+        <v>06/15/23 15:37</v>
       </c>
       <c r="K25" t="str">
-        <v>06/13/23 14:25</v>
+        <v>06/15/23 15:37</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25" t="str">
-        <v>$13,620 as of 6/13/2023 11:54:34 AM</v>
+        <v>$12,300 as of 6/15/2023 9:19:46 AM</v>
       </c>
       <c r="N25">
-        <v>13320</v>
+        <v>12280</v>
       </c>
       <c r="O25">
         <v>0</v>
@@ -1354,28 +1354,28 @@
         <v>98 DISCOUNT STORE</v>
       </c>
       <c r="E26">
-        <v>23220</v>
+        <v>21180</v>
       </c>
       <c r="F26" t="str">
         <v>T</v>
       </c>
       <c r="H26">
-        <v>45103.04187195602</v>
+        <v>45107.04186157407</v>
       </c>
       <c r="J26" t="str">
-        <v>06/13/23 16:38</v>
+        <v>06/15/23 15:30</v>
       </c>
       <c r="K26" t="str">
-        <v>06/13/23 16:38</v>
+        <v>06/15/23 13:08</v>
       </c>
       <c r="L26">
         <v>60</v>
       </c>
       <c r="M26" t="str">
-        <v>$23,440 as of 6/13/2023 11:03:04 AM</v>
+        <v>$21,180 as of 6/15/2023 11:08:55 AM</v>
       </c>
       <c r="N26">
-        <v>23420</v>
+        <v>21180</v>
       </c>
       <c r="O26">
         <v>0</v>
@@ -1392,7 +1392,7 @@
         <v>Total Outstanding Cash Balance:</v>
       </c>
       <c r="E27">
-        <v>140180</v>
+        <v>134140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed rerendering and calling of square components
</commit_message>
<xml_diff>
--- a/rptTerminalStatusCassetteBalances.xlsx
+++ b/rptTerminalStatusCassetteBalances.xlsx
@@ -44,8 +44,8 @@
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
     <numFmt numFmtId="164" formatCode="[$-010409]#,###"/>
     <numFmt numFmtId="165" formatCode="[$-010409]&quot;$&quot;#,##0.00;(&quot;$&quot;#,##0.00)"/>
-    <numFmt numFmtId="166" formatCode="[$-010409]$#,##0"/>
-    <numFmt numFmtId="167" formatCode="[$-010409]m/d/yyyy"/>
+    <numFmt numFmtId="166" formatCode="[$-010409]m/d/yyyy"/>
+    <numFmt numFmtId="167" formatCode="[$-010409]$#,##0"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -409,7 +409,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -419,7 +419,7 @@
         <v>Active Terminals:</v>
       </c>
       <c r="D1">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" ht="9" customHeight="1"/>
@@ -478,34 +478,34 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>L647934</v>
+        <v>LK644532</v>
       </c>
       <c r="C5" t="str">
-        <v>SB #6</v>
+        <v>SCL ENTERPRISES LAUNDRY</v>
       </c>
       <c r="E5">
-        <v>1940</v>
+        <v>1880</v>
       </c>
       <c r="F5" t="str">
         <v>T</v>
       </c>
-      <c r="I5" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+      <c r="H5">
+        <v>45127.042061423606</v>
       </c>
       <c r="J5" t="str">
-        <v>04/06/23 22:10</v>
+        <v>06/28/23 15:33</v>
       </c>
       <c r="K5" t="str">
-        <v>04/06/23 22:05</v>
+        <v>06/28/23 15:33</v>
       </c>
       <c r="L5">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M5" t="str">
-        <v>$1,940 as of 4/6/2023 8:05:45 PM</v>
+        <v>$1,880 as of 6/28/2023 1:33:05 PM</v>
       </c>
       <c r="N5">
-        <v>1960</v>
+        <v>1980</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -519,34 +519,34 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>LK644532</v>
+        <v>L647934</v>
       </c>
       <c r="C6" t="str">
-        <v>SCL ENTERPRISES LAUNDRY</v>
+        <v>SB #6</v>
       </c>
       <c r="E6">
-        <v>1980</v>
+        <v>1940</v>
       </c>
       <c r="F6" t="str">
         <v>T</v>
       </c>
-      <c r="H6">
-        <v>45136.0418568287</v>
+      <c r="I6" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J6" t="str">
-        <v>06/26/23 14:42</v>
+        <v>04/06/23 22:10</v>
       </c>
       <c r="K6" t="str">
-        <v>06/26/23 14:42</v>
+        <v>04/06/23 22:05</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M6" t="str">
-        <v>$2,200 as of 6/25/2023 7:05:25 PM</v>
+        <v>$1,940 as of 4/6/2023 8:05:45 PM</v>
       </c>
       <c r="N6">
-        <v>2180</v>
+        <v>1960</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -560,37 +560,37 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>L688961</v>
+        <v>L662336</v>
       </c>
       <c r="C7" t="str">
-        <v>MONA MART</v>
+        <v>SB#4 MONA MARKET</v>
       </c>
       <c r="E7">
-        <v>2040</v>
+        <v>2240</v>
       </c>
       <c r="F7" t="str">
         <v>T</v>
       </c>
       <c r="H7">
-        <v>45151.0418568287</v>
+        <v>45114.042061423606</v>
       </c>
       <c r="I7" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+        <v>The Triton ATM reported error code 35: Mistracked Note at Double Detec</v>
       </c>
       <c r="J7" t="str">
-        <v>06/23/23 17:14</v>
+        <v>06/29/23 15:48</v>
       </c>
       <c r="K7" t="str">
-        <v>06/21/23 22:48</v>
+        <v>06/29/23 15:48</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7" t="str">
-        <v>$2,040 as of 6/23/2023 3:14:18 PM</v>
+        <v>$2,300 as of 6/29/2023 8:00:28 AM</v>
       </c>
       <c r="N7">
-        <v>2080</v>
+        <v>2240</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -604,37 +604,34 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>L682801</v>
+        <v>L474746</v>
       </c>
       <c r="C8" t="str">
-        <v>SB#5</v>
+        <v>ZACATES MARKET</v>
       </c>
       <c r="E8">
-        <v>2640</v>
+        <v>2360</v>
       </c>
       <c r="F8" t="str">
         <v>T</v>
       </c>
       <c r="H8">
-        <v>45137.0418568287</v>
-      </c>
-      <c r="I8" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+        <v>45114.042061423606</v>
       </c>
       <c r="J8" t="str">
-        <v>06/25/23 14:06</v>
+        <v>06/29/23 19:45</v>
       </c>
       <c r="K8" t="str">
-        <v>06/23/23 10:36</v>
+        <v>06/29/23 19:45</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8" t="str">
-        <v>$2,640 as of 6/25/2023 12:06:15 PM</v>
+        <v>$2,480 as of 6/29/2023 9:34:21 AM</v>
       </c>
       <c r="N8">
-        <v>2740</v>
+        <v>2480</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -648,34 +645,34 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>LK561655</v>
+        <v>L682801</v>
       </c>
       <c r="C9" t="str">
-        <v>CRENSHAW CRAVOR #2</v>
+        <v>SB#5</v>
       </c>
       <c r="E9">
-        <v>2780</v>
+        <v>2520</v>
       </c>
       <c r="F9" t="str">
         <v>T</v>
       </c>
-      <c r="I9" t="str">
-        <v>ATM Inactive greater than 48 minutes</v>
+      <c r="H9">
+        <v>45155.042061423606</v>
       </c>
       <c r="J9" t="str">
-        <v>01/23/20 08:24</v>
+        <v>06/28/23 18:23</v>
       </c>
       <c r="K9" t="str">
-        <v>01/23/20 08:24</v>
+        <v>06/28/23 18:23</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9" t="str">
-        <v>$2,780 as of 1/23/2020 6:24:32 AM</v>
+        <v>$2,520 as of 6/28/2023 4:23:23 PM</v>
       </c>
       <c r="N9">
-        <v>2800</v>
+        <v>2560</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -689,34 +686,34 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>L662336</v>
+        <v>LK561655</v>
       </c>
       <c r="C10" t="str">
-        <v>SB#4 MONA MARKET</v>
+        <v>CRENSHAW CRAVOR #2</v>
       </c>
       <c r="E10">
-        <v>2880</v>
+        <v>2780</v>
       </c>
       <c r="F10" t="str">
         <v>T</v>
       </c>
-      <c r="H10">
-        <v>45124.0418568287</v>
+      <c r="I10" t="str">
+        <v>ATM Inactive greater than 48 minutes</v>
       </c>
       <c r="J10" t="str">
-        <v>06/26/23 19:07</v>
+        <v>01/23/20 08:24</v>
       </c>
       <c r="K10" t="str">
-        <v>06/26/23 19:07</v>
+        <v>01/23/20 08:24</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10" t="str">
-        <v>$3,440 as of 6/26/2023 11:45:13 AM</v>
+        <v>$2,780 as of 1/23/2020 6:24:32 AM</v>
       </c>
       <c r="N10">
-        <v>2900</v>
+        <v>2800</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -730,34 +727,34 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>L474746</v>
+        <v>L474792</v>
       </c>
       <c r="C11" t="str">
-        <v>ZACATES MARKET</v>
+        <v>NICK SHELL SERVICE</v>
       </c>
       <c r="E11">
-        <v>3500</v>
+        <v>3440</v>
       </c>
       <c r="F11" t="str">
         <v>T</v>
       </c>
       <c r="H11">
-        <v>45116.0418568287</v>
+        <v>45142.042061423606</v>
       </c>
       <c r="J11" t="str">
-        <v>06/26/23 19:29</v>
+        <v>06/29/23 17:17</v>
       </c>
       <c r="K11" t="str">
-        <v>06/26/23 19:29</v>
+        <v>06/29/23 17:17</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11" t="str">
-        <v>$3,560 as of 6/25/2023 2:44:11 PM</v>
+        <v>$3,500 as of 6/28/2023 5:44:16 PM</v>
       </c>
       <c r="N11">
-        <v>3560</v>
+        <v>3460</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -771,34 +768,34 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>L474792</v>
+        <v>L475182</v>
       </c>
       <c r="C12" t="str">
-        <v>NICK SHELL SERVICE</v>
+        <v>LA ESQUINA DE ORO</v>
       </c>
       <c r="E12">
-        <v>3540</v>
+        <v>3800</v>
       </c>
       <c r="F12" t="str">
         <v>T</v>
       </c>
-      <c r="H12">
-        <v>45132.0418568287</v>
+      <c r="I12" t="str">
+        <v>ATM Inactive greater than 48 minutes</v>
       </c>
       <c r="J12" t="str">
-        <v>06/25/23 19:27</v>
+        <v>09/16/20 16:57</v>
       </c>
       <c r="K12" t="str">
-        <v>06/25/23 19:27</v>
+        <v>09/15/20 23:38</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12" t="str">
-        <v>$3,540 as of 6/25/2023 5:27:23 PM</v>
+        <v>$3,800 as of 9/16/2020 1:28:00 PM</v>
       </c>
       <c r="N12">
-        <v>3560</v>
+        <v>3800</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -812,34 +809,34 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>L475182</v>
+        <v>L688961</v>
       </c>
       <c r="C13" t="str">
-        <v>LA ESQUINA DE ORO</v>
+        <v>MONA MART</v>
       </c>
       <c r="E13">
-        <v>3800</v>
+        <v>3900</v>
       </c>
       <c r="F13" t="str">
         <v>T</v>
       </c>
-      <c r="I13" t="str">
-        <v>ATM Inactive greater than 48 minutes</v>
+      <c r="H13">
+        <v>45140.042061423606</v>
       </c>
       <c r="J13" t="str">
-        <v>09/16/20 16:57</v>
+        <v>06/29/23 16:20</v>
       </c>
       <c r="K13" t="str">
-        <v>09/15/20 23:38</v>
+        <v>06/29/23 16:20</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13" t="str">
-        <v>$3,800 as of 9/16/2020 1:28:00 PM</v>
+        <v>$1,940 as of 6/28/2023 4:57:51 PM</v>
       </c>
       <c r="N13">
-        <v>3800</v>
+        <v>3940</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -853,37 +850,34 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>L476340</v>
+        <v>L475090</v>
       </c>
       <c r="C14" t="str">
-        <v>DONUT &amp; SANDWICH</v>
+        <v>S.B. 2</v>
       </c>
       <c r="E14">
-        <v>4300</v>
+        <v>4680</v>
       </c>
       <c r="F14" t="str">
         <v>T</v>
       </c>
       <c r="H14">
-        <v>45125.0418568287</v>
-      </c>
-      <c r="I14" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+        <v>45115.042061423606</v>
       </c>
       <c r="J14" t="str">
-        <v>06/24/23 13:23</v>
+        <v>06/29/23 19:04</v>
       </c>
       <c r="K14" t="str">
-        <v>06/24/23 13:23</v>
+        <v>06/29/23 19:04</v>
       </c>
       <c r="L14">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M14" t="str">
-        <v>$4,300 as of 6/24/2023 11:23:13 AM</v>
+        <v>$4,900 as of 6/29/2023 11:52:24 AM</v>
       </c>
       <c r="N14">
-        <v>4500</v>
+        <v>4720</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -897,34 +891,34 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>LK891176</v>
+        <v>LK923383</v>
       </c>
       <c r="C15" t="str">
-        <v>98 DISCOUNT STORE</v>
+        <v>SAMYS PHONE CARDS</v>
       </c>
       <c r="E15">
-        <v>5340</v>
+        <v>4860</v>
       </c>
       <c r="F15" t="str">
         <v>T</v>
       </c>
       <c r="H15">
-        <v>45107.0418568287</v>
+        <v>45112.042061423606</v>
       </c>
       <c r="J15" t="str">
-        <v>06/26/23 19:10</v>
+        <v>06/29/23 18:34</v>
       </c>
       <c r="K15" t="str">
-        <v>06/26/23 19:10</v>
+        <v>06/29/23 18:34</v>
       </c>
       <c r="L15">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="M15" t="str">
-        <v>$6,000 as of 6/26/2023 11:50:43 AM</v>
+        <v>$5,680 as of 6/28/2023 8:26:26 PM</v>
       </c>
       <c r="N15">
-        <v>5540</v>
+        <v>4900</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -938,34 +932,34 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>L474761</v>
+        <v>L476340</v>
       </c>
       <c r="C16" t="str">
-        <v>BABS MARKET</v>
+        <v>DONUT &amp; SANDWICH</v>
       </c>
       <c r="E16">
-        <v>5720</v>
+        <v>4940</v>
       </c>
       <c r="F16" t="str">
         <v>T</v>
       </c>
       <c r="H16">
-        <v>45151.0418568287</v>
+        <v>45139.042061423606</v>
       </c>
       <c r="J16" t="str">
-        <v>06/26/23 15:25</v>
+        <v>06/29/23 16:45</v>
       </c>
       <c r="K16" t="str">
-        <v>06/26/23 15:25</v>
+        <v>06/29/23 16:45</v>
       </c>
       <c r="L16">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M16" t="str">
-        <v>$5,740 as of 6/25/2023 3:40:16 PM</v>
+        <v>$4,300 as of 6/24/2023 11:23:13 AM</v>
       </c>
       <c r="N16">
-        <v>5740</v>
+        <v>4960</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -985,28 +979,28 @@
         <v>WORLDWIDE AUTOMOTIVE</v>
       </c>
       <c r="E17">
-        <v>5840</v>
+        <v>4940</v>
       </c>
       <c r="F17" t="str">
         <v>T</v>
       </c>
       <c r="H17">
-        <v>45111.0418568287</v>
+        <v>45129.042061423606</v>
       </c>
       <c r="J17" t="str">
-        <v>06/26/23 19:45</v>
+        <v>06/29/23 12:32</v>
       </c>
       <c r="K17" t="str">
-        <v>06/26/23 19:45</v>
+        <v>06/29/23 11:23</v>
       </c>
       <c r="L17">
         <v>80</v>
       </c>
       <c r="M17" t="str">
-        <v>$2,320 as of 6/25/2023 12:54:04 PM</v>
+        <v>$4,940 as of 6/29/2023 10:32:07 AM</v>
       </c>
       <c r="N17">
-        <v>5920</v>
+        <v>5140</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1020,37 +1014,34 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>L488595</v>
+        <v>L474761</v>
       </c>
       <c r="C18" t="str">
-        <v>N S MART</v>
+        <v>BABS MARKET</v>
       </c>
       <c r="E18">
-        <v>6200</v>
+        <v>5160</v>
       </c>
       <c r="F18" t="str">
         <v>T</v>
       </c>
       <c r="H18">
-        <v>45374.0418568287</v>
-      </c>
-      <c r="I18" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+        <v>45168.042061423606</v>
       </c>
       <c r="J18" t="str">
-        <v>06/23/23 19:40</v>
+        <v>06/29/23 19:19</v>
       </c>
       <c r="K18" t="str">
-        <v>06/23/23 19:40</v>
+        <v>06/29/23 19:19</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="M18" t="str">
-        <v>$6,200 as of 6/23/2023 5:40:14 PM</v>
+        <v>$5,300 as of 6/29/2023 10:52:54 AM</v>
       </c>
       <c r="N18">
-        <v>6280</v>
+        <v>5260</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -1064,34 +1055,34 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>L475090</v>
+        <v>L697589</v>
       </c>
       <c r="C19" t="str">
-        <v>S.B. 2</v>
+        <v>S B DISCOUNT MART</v>
       </c>
       <c r="E19">
-        <v>6260</v>
+        <v>5780</v>
       </c>
       <c r="F19" t="str">
         <v>T</v>
       </c>
       <c r="H19">
-        <v>45116.0418568287</v>
+        <v>45114.042061423606</v>
       </c>
       <c r="J19" t="str">
-        <v>06/26/23 15:53</v>
+        <v>06/29/23 19:31</v>
       </c>
       <c r="K19" t="str">
-        <v>06/26/23 15:53</v>
+        <v>06/29/23 19:31</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M19" t="str">
-        <v>$6,500 as of 6/26/2023 11:22:59 AM</v>
+        <v>$7,180 as of 6/29/2023 11:54:34 AM</v>
       </c>
       <c r="N19">
-        <v>6260</v>
+        <v>5880</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1105,34 +1096,34 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>L474817</v>
+        <v>LK864765</v>
       </c>
       <c r="C20" t="str">
-        <v>SAFETY MARKET</v>
+        <v>SKY LIQUOR</v>
       </c>
       <c r="E20">
-        <v>6880</v>
+        <v>5940</v>
       </c>
       <c r="F20" t="str">
         <v>T</v>
       </c>
       <c r="H20">
-        <v>45119.0418568287</v>
+        <v>45121.042061423606</v>
       </c>
       <c r="J20" t="str">
-        <v>06/26/23 19:49</v>
+        <v>06/29/23 19:02</v>
       </c>
       <c r="K20" t="str">
-        <v>06/26/23 19:49</v>
+        <v>06/29/23 11:48</v>
       </c>
       <c r="L20">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M20" t="str">
-        <v>$7,000 as of 6/25/2023 7:01:23 PM</v>
+        <v>$5,960 as of 6/29/2023 9:48:28 AM</v>
       </c>
       <c r="N20">
-        <v>7000</v>
+        <v>5940</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -1146,37 +1137,34 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>L688966</v>
+        <v>L488595</v>
       </c>
       <c r="C21" t="str">
-        <v>LACON MINI MART</v>
+        <v>N S MART</v>
       </c>
       <c r="E21">
-        <v>6900</v>
+        <v>6020</v>
       </c>
       <c r="F21" t="str">
         <v>T</v>
       </c>
       <c r="H21">
-        <v>45276.0418568287</v>
-      </c>
-      <c r="I21" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+        <v>45407.042061423606</v>
       </c>
       <c r="J21" t="str">
-        <v>06/25/23 11:10</v>
+        <v>06/28/23 19:23</v>
       </c>
       <c r="K21" t="str">
-        <v>06/22/23 16:56</v>
+        <v>06/28/23 19:23</v>
       </c>
       <c r="L21">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M21" t="str">
-        <v>$6,900 as of 6/22/2023 2:56:56 PM</v>
+        <v>$6,020 as of 6/28/2023 5:23:06 PM</v>
       </c>
       <c r="N21">
-        <v>6920</v>
+        <v>6180</v>
       </c>
       <c r="O21">
         <v>0</v>
@@ -1190,34 +1178,34 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>LK923383</v>
+        <v>L474817</v>
       </c>
       <c r="C22" t="str">
-        <v>SAMYS PHONE CARDS</v>
+        <v>SAFETY MARKET</v>
       </c>
       <c r="E22">
-        <v>7180</v>
+        <v>6440</v>
       </c>
       <c r="F22" t="str">
         <v>T</v>
       </c>
       <c r="H22">
-        <v>45111.0418568287</v>
+        <v>45123.042061423606</v>
       </c>
       <c r="J22" t="str">
-        <v>06/26/23 18:58</v>
+        <v>06/29/23 17:44</v>
       </c>
       <c r="K22" t="str">
-        <v>06/26/23 18:48</v>
+        <v>06/29/23 17:44</v>
       </c>
       <c r="L22">
         <v>100</v>
       </c>
       <c r="M22" t="str">
-        <v>$7,420 as of 6/25/2023 6:34:38 PM</v>
+        <v>$6,480 as of 6/29/2023 7:54:04 AM</v>
       </c>
       <c r="N22">
-        <v>7180</v>
+        <v>6460</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -1231,34 +1219,37 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>LK864765</v>
+        <v>L688966</v>
       </c>
       <c r="C23" t="str">
-        <v>SKY LIQUOR</v>
+        <v>LACON MINI MART</v>
       </c>
       <c r="E23">
-        <v>8200</v>
+        <v>6900</v>
       </c>
       <c r="F23" t="str">
         <v>T</v>
       </c>
       <c r="H23">
-        <v>45131.0418568287</v>
+        <v>45279.042061423606</v>
+      </c>
+      <c r="I23" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J23" t="str">
-        <v>06/26/23 19:34</v>
+        <v>06/25/23 11:10</v>
       </c>
       <c r="K23" t="str">
-        <v>06/26/23 19:30</v>
+        <v>06/22/23 16:56</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M23" t="str">
-        <v>$8,240 as of 6/26/2023 11:27:52 AM</v>
+        <v>$6,900 as of 6/22/2023 2:56:56 PM</v>
       </c>
       <c r="N23">
-        <v>8200</v>
+        <v>6920</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -1272,34 +1263,31 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>L697590</v>
+        <v>L704741</v>
       </c>
       <c r="C24" t="str">
-        <v>S B MARKET ST</v>
+        <v>W ADAMS COIN LAUNDRY</v>
       </c>
       <c r="E24">
-        <v>9460</v>
+        <v>8320</v>
       </c>
       <c r="F24" t="str">
         <v>T</v>
       </c>
-      <c r="H24">
-        <v>45118.0418568287</v>
-      </c>
       <c r="J24" t="str">
-        <v>06/26/23 19:05</v>
+        <v>06/29/23 19:25</v>
       </c>
       <c r="K24" t="str">
-        <v>06/26/23 19:05</v>
+        <v>06/29/23 19:25</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
       <c r="M24" t="str">
-        <v>$9,700 as of 6/26/2023 4:54:54 AM</v>
+        <v>$8,680 as of 6/29/2023 11:29:36 AM</v>
       </c>
       <c r="N24">
-        <v>9480</v>
+        <v>8460</v>
       </c>
       <c r="O24">
         <v>0</v>
@@ -1313,34 +1301,34 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>L678988</v>
+        <v>L697590</v>
       </c>
       <c r="C25" t="str">
-        <v>PAYELESS MARKET</v>
+        <v>S B MARKET ST</v>
       </c>
       <c r="E25">
-        <v>9820</v>
+        <v>8780</v>
       </c>
       <c r="F25" t="str">
         <v>T</v>
       </c>
       <c r="H25">
-        <v>45145.0418568287</v>
+        <v>45120.042061423606</v>
       </c>
       <c r="J25" t="str">
-        <v>06/26/23 15:11</v>
+        <v>06/29/23 11:36</v>
       </c>
       <c r="K25" t="str">
-        <v>06/26/23 15:11</v>
+        <v>06/29/23 11:36</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25" t="str">
-        <v>$9,920 as of 6/26/2023 11:06:33 AM</v>
+        <v>$8,780 as of 6/29/2023 9:36:36 AM</v>
       </c>
       <c r="N25">
-        <v>9920</v>
+        <v>8800</v>
       </c>
       <c r="O25">
         <v>0</v>
@@ -1354,34 +1342,34 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>L697589</v>
+        <v>L678988</v>
       </c>
       <c r="C26" t="str">
-        <v>S B DISCOUNT MART</v>
+        <v>PAYELESS MARKET</v>
       </c>
       <c r="E26">
-        <v>10300</v>
+        <v>9040</v>
       </c>
       <c r="F26" t="str">
         <v>T</v>
       </c>
       <c r="H26">
-        <v>45121.0418568287</v>
+        <v>45140.042061423606</v>
       </c>
       <c r="J26" t="str">
-        <v>06/26/23 18:41</v>
+        <v>06/29/23 17:14</v>
       </c>
       <c r="K26" t="str">
-        <v>06/26/23 18:21</v>
+        <v>06/29/23 14:45</v>
       </c>
       <c r="L26">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M26" t="str">
-        <v>$11,140 as of 6/26/2023 10:23:56 AM</v>
+        <v>$9,240 as of 6/29/2023 10:47:16 AM</v>
       </c>
       <c r="N26">
-        <v>10300</v>
+        <v>9040</v>
       </c>
       <c r="O26">
         <v>0</v>
@@ -1395,14 +1383,55 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
+        <v>LK891176</v>
+      </c>
+      <c r="C27" t="str">
+        <v>98 DISCOUNT STORE</v>
+      </c>
+      <c r="E27">
+        <v>20540</v>
+      </c>
+      <c r="F27" t="str">
+        <v>T</v>
+      </c>
+      <c r="H27">
+        <v>45122.042061423606</v>
+      </c>
+      <c r="J27" t="str">
+        <v>06/29/23 18:49</v>
+      </c>
+      <c r="K27" t="str">
+        <v>06/29/23 18:49</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27" t="str">
+        <v>$21,100 as of 6/29/2023 10:23:59 AM</v>
+      </c>
+      <c r="N27">
+        <v>20580</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
         <v>Total Outstanding Cash Balance:</v>
       </c>
-      <c r="E27">
-        <v>117500</v>
+      <c r="E28">
+        <v>127200</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="74">
+  <mergeCells count="77">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:F1"/>
     <mergeCell ref="A3:Q3"/>
@@ -1475,12 +1504,15 @@
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="C26:D26"/>
     <mergeCell ref="F26:G26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="E27:H27"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="E28:H28"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0.5" header="0" footer="0"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:Q27"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:Q28"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed encryption and added decryption
</commit_message>
<xml_diff>
--- a/rptTerminalStatusCassetteBalances.xlsx
+++ b/rptTerminalStatusCassetteBalances.xlsx
@@ -484,28 +484,28 @@
         <v>SCL ENTERPRISES LAUNDRY</v>
       </c>
       <c r="E5">
-        <v>1880</v>
+        <v>1540</v>
       </c>
       <c r="F5" t="str">
         <v>T</v>
       </c>
       <c r="H5">
-        <v>45127.042061423606</v>
+        <v>45141.04206952546</v>
       </c>
       <c r="J5" t="str">
-        <v>06/28/23 15:33</v>
+        <v>07/06/23 08:49</v>
       </c>
       <c r="K5" t="str">
-        <v>06/28/23 15:33</v>
+        <v>07/06/23 08:49</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5" t="str">
-        <v>$1,880 as of 6/28/2023 1:33:05 PM</v>
+        <v>$1,540 as of 7/5/2023 11:37:54 AM</v>
       </c>
       <c r="N5">
-        <v>1980</v>
+        <v>1580</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -560,37 +560,34 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>L662336</v>
+        <v>L682801</v>
       </c>
       <c r="C7" t="str">
-        <v>SB#4 MONA MARKET</v>
+        <v>SB#5</v>
       </c>
       <c r="E7">
-        <v>2240</v>
+        <v>2100</v>
       </c>
       <c r="F7" t="str">
         <v>T</v>
       </c>
       <c r="H7">
-        <v>45114.042061423606</v>
-      </c>
-      <c r="I7" t="str">
-        <v>The Triton ATM reported error code 35: Mistracked Note at Double Detec</v>
+        <v>45144.04206952546</v>
       </c>
       <c r="J7" t="str">
-        <v>06/29/23 15:48</v>
+        <v>07/05/23 15:53</v>
       </c>
       <c r="K7" t="str">
-        <v>06/29/23 15:48</v>
+        <v>07/05/23 15:53</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7" t="str">
-        <v>$2,300 as of 6/29/2023 8:00:28 AM</v>
+        <v>$2,100 as of 7/3/2023 1:33:47 PM</v>
       </c>
       <c r="N7">
-        <v>2240</v>
+        <v>2120</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -604,34 +601,34 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>L474746</v>
+        <v>L475090</v>
       </c>
       <c r="C8" t="str">
-        <v>ZACATES MARKET</v>
+        <v>S.B. 2</v>
       </c>
       <c r="E8">
-        <v>2360</v>
+        <v>2180</v>
       </c>
       <c r="F8" t="str">
         <v>T</v>
       </c>
       <c r="H8">
-        <v>45114.042061423606</v>
+        <v>45115.04206952546</v>
       </c>
       <c r="J8" t="str">
-        <v>06/29/23 19:45</v>
+        <v>07/06/23 14:19</v>
       </c>
       <c r="K8" t="str">
-        <v>06/29/23 19:45</v>
+        <v>07/06/23 13:47</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8" t="str">
-        <v>$2,480 as of 6/29/2023 9:34:21 AM</v>
+        <v>$2,260 as of 7/5/2023 11:40:47 AM</v>
       </c>
       <c r="N8">
-        <v>2480</v>
+        <v>2140</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -645,34 +642,34 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>L682801</v>
+        <v>L662336</v>
       </c>
       <c r="C9" t="str">
-        <v>SB#5</v>
+        <v>SB#4 MONA MARKET</v>
       </c>
       <c r="E9">
-        <v>2520</v>
+        <v>2620</v>
       </c>
       <c r="F9" t="str">
         <v>T</v>
       </c>
       <c r="H9">
-        <v>45155.042061423606</v>
+        <v>45119.04206952546</v>
       </c>
       <c r="J9" t="str">
-        <v>06/28/23 18:23</v>
+        <v>07/05/23 20:35</v>
       </c>
       <c r="K9" t="str">
-        <v>06/28/23 18:23</v>
+        <v>07/05/23 20:35</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M9" t="str">
-        <v>$2,520 as of 6/28/2023 4:23:23 PM</v>
+        <v>$2,620 as of 7/4/2023 6:15:15 PM</v>
       </c>
       <c r="N9">
-        <v>2560</v>
+        <v>2720</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -686,34 +683,34 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>LK561655</v>
+        <v>L474761</v>
       </c>
       <c r="C10" t="str">
-        <v>CRENSHAW CRAVOR #2</v>
+        <v>BABS MARKET</v>
       </c>
       <c r="E10">
-        <v>2780</v>
+        <v>2700</v>
       </c>
       <c r="F10" t="str">
         <v>T</v>
       </c>
-      <c r="I10" t="str">
-        <v>ATM Inactive greater than 48 minutes</v>
+      <c r="H10">
+        <v>45120.04206952546</v>
       </c>
       <c r="J10" t="str">
-        <v>01/23/20 08:24</v>
+        <v>07/05/23 21:38</v>
       </c>
       <c r="K10" t="str">
-        <v>01/23/20 08:24</v>
+        <v>07/05/23 21:38</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="M10" t="str">
-        <v>$2,780 as of 1/23/2020 6:24:32 AM</v>
+        <v>$2,700 as of 7/5/2023 9:56:34 AM</v>
       </c>
       <c r="N10">
-        <v>2800</v>
+        <v>2760</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -727,34 +724,34 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>L474792</v>
+        <v>LK561655</v>
       </c>
       <c r="C11" t="str">
-        <v>NICK SHELL SERVICE</v>
+        <v>CRENSHAW CRAVOR #2</v>
       </c>
       <c r="E11">
-        <v>3440</v>
+        <v>2780</v>
       </c>
       <c r="F11" t="str">
         <v>T</v>
       </c>
-      <c r="H11">
-        <v>45142.042061423606</v>
+      <c r="I11" t="str">
+        <v>ATM Inactive greater than 48 minutes</v>
       </c>
       <c r="J11" t="str">
-        <v>06/29/23 17:17</v>
+        <v>01/23/20 08:24</v>
       </c>
       <c r="K11" t="str">
-        <v>06/29/23 17:17</v>
+        <v>01/23/20 08:24</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11" t="str">
-        <v>$3,500 as of 6/28/2023 5:44:16 PM</v>
+        <v>$2,780 as of 1/23/2020 6:24:32 AM</v>
       </c>
       <c r="N11">
-        <v>3460</v>
+        <v>2800</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -768,34 +765,37 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>L475182</v>
+        <v>L474792</v>
       </c>
       <c r="C12" t="str">
-        <v>LA ESQUINA DE ORO</v>
+        <v>NICK SHELL SERVICE</v>
       </c>
       <c r="E12">
-        <v>3800</v>
+        <v>2900</v>
       </c>
       <c r="F12" t="str">
         <v>T</v>
       </c>
+      <c r="H12">
+        <v>45146.04206952546</v>
+      </c>
       <c r="I12" t="str">
-        <v>ATM Inactive greater than 48 minutes</v>
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J12" t="str">
-        <v>09/16/20 16:57</v>
+        <v>07/04/23 20:34</v>
       </c>
       <c r="K12" t="str">
-        <v>09/15/20 23:38</v>
+        <v>07/04/23 20:34</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12" t="str">
-        <v>$3,800 as of 9/16/2020 1:28:00 PM</v>
+        <v>$2,900 as of 7/4/2023 6:34:42 PM</v>
       </c>
       <c r="N12">
-        <v>3800</v>
+        <v>2940</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -809,34 +809,34 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>L688961</v>
+        <v>L474817</v>
       </c>
       <c r="C13" t="str">
-        <v>MONA MART</v>
+        <v>SAFETY MARKET</v>
       </c>
       <c r="E13">
-        <v>3900</v>
+        <v>3000</v>
       </c>
       <c r="F13" t="str">
         <v>T</v>
       </c>
       <c r="H13">
-        <v>45140.042061423606</v>
+        <v>45120.04206952546</v>
       </c>
       <c r="J13" t="str">
-        <v>06/29/23 16:20</v>
+        <v>07/06/23 14:23</v>
       </c>
       <c r="K13" t="str">
-        <v>06/29/23 16:20</v>
+        <v>07/06/23 12:29</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="M13" t="str">
-        <v>$1,940 as of 6/28/2023 4:57:51 PM</v>
+        <v>$3,000 as of 7/5/2023 11:46:37 AM</v>
       </c>
       <c r="N13">
-        <v>3940</v>
+        <v>3000</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -850,34 +850,34 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>L475090</v>
+        <v>L688961</v>
       </c>
       <c r="C14" t="str">
-        <v>S.B. 2</v>
+        <v>MONA MART</v>
       </c>
       <c r="E14">
-        <v>4680</v>
+        <v>3540</v>
       </c>
       <c r="F14" t="str">
         <v>T</v>
       </c>
       <c r="H14">
-        <v>45115.042061423606</v>
+        <v>45216.04206952546</v>
       </c>
       <c r="J14" t="str">
-        <v>06/29/23 19:04</v>
+        <v>07/05/23 21:26</v>
       </c>
       <c r="K14" t="str">
-        <v>06/29/23 19:04</v>
+        <v>07/05/23 21:26</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14" t="str">
-        <v>$4,900 as of 6/29/2023 11:52:24 AM</v>
+        <v>$3,540 as of 7/4/2023 1:55:10 PM</v>
       </c>
       <c r="N14">
-        <v>4720</v>
+        <v>3620</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -891,34 +891,34 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>LK923383</v>
+        <v>L475182</v>
       </c>
       <c r="C15" t="str">
-        <v>SAMYS PHONE CARDS</v>
+        <v>LA ESQUINA DE ORO</v>
       </c>
       <c r="E15">
-        <v>4860</v>
+        <v>3800</v>
       </c>
       <c r="F15" t="str">
         <v>T</v>
       </c>
-      <c r="H15">
-        <v>45112.042061423606</v>
+      <c r="I15" t="str">
+        <v>ATM Inactive greater than 48 minutes</v>
       </c>
       <c r="J15" t="str">
-        <v>06/29/23 18:34</v>
+        <v>09/16/20 16:57</v>
       </c>
       <c r="K15" t="str">
-        <v>06/29/23 18:34</v>
+        <v>09/15/20 23:38</v>
       </c>
       <c r="L15">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M15" t="str">
-        <v>$5,680 as of 6/28/2023 8:26:26 PM</v>
+        <v>$3,800 as of 9/16/2020 1:28:00 PM</v>
       </c>
       <c r="N15">
-        <v>4900</v>
+        <v>3800</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -938,28 +938,28 @@
         <v>DONUT &amp; SANDWICH</v>
       </c>
       <c r="E16">
-        <v>4940</v>
+        <v>3820</v>
       </c>
       <c r="F16" t="str">
         <v>T</v>
       </c>
       <c r="H16">
-        <v>45139.042061423606</v>
+        <v>45136.04206952546</v>
       </c>
       <c r="J16" t="str">
-        <v>06/29/23 16:45</v>
+        <v>07/05/23 15:23</v>
       </c>
       <c r="K16" t="str">
-        <v>06/29/23 16:45</v>
+        <v>07/05/23 09:07</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16" t="str">
-        <v>$4,300 as of 6/24/2023 11:23:13 AM</v>
+        <v>$3,820 as of 7/5/2023 7:07:49 AM</v>
       </c>
       <c r="N16">
-        <v>4960</v>
+        <v>3820</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -979,28 +979,31 @@
         <v>WORLDWIDE AUTOMOTIVE</v>
       </c>
       <c r="E17">
-        <v>4940</v>
+        <v>3820</v>
       </c>
       <c r="F17" t="str">
         <v>T</v>
       </c>
       <c r="H17">
-        <v>45129.042061423606</v>
+        <v>45127.04206952546</v>
+      </c>
+      <c r="I17" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J17" t="str">
-        <v>06/29/23 12:32</v>
+        <v>07/03/23 15:16</v>
       </c>
       <c r="K17" t="str">
-        <v>06/29/23 11:23</v>
+        <v>07/03/23 15:16</v>
       </c>
       <c r="L17">
         <v>80</v>
       </c>
       <c r="M17" t="str">
-        <v>$4,940 as of 6/29/2023 10:32:07 AM</v>
+        <v>$3,820 as of 7/3/2023 1:16:30 PM</v>
       </c>
       <c r="N17">
-        <v>5140</v>
+        <v>3940</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1014,34 +1017,34 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>L474761</v>
+        <v>L474746</v>
       </c>
       <c r="C18" t="str">
-        <v>BABS MARKET</v>
+        <v>ZACATES MARKET</v>
       </c>
       <c r="E18">
-        <v>5160</v>
+        <v>4320</v>
       </c>
       <c r="F18" t="str">
         <v>T</v>
       </c>
       <c r="H18">
-        <v>45168.042061423606</v>
+        <v>45126.04206952546</v>
       </c>
       <c r="J18" t="str">
-        <v>06/29/23 19:19</v>
+        <v>07/05/23 16:19</v>
       </c>
       <c r="K18" t="str">
-        <v>06/29/23 19:19</v>
+        <v>07/05/23 16:19</v>
       </c>
       <c r="L18">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M18" t="str">
-        <v>$5,300 as of 6/29/2023 10:52:54 AM</v>
+        <v>$4,320 as of 7/5/2023 11:18:44 AM</v>
       </c>
       <c r="N18">
-        <v>5260</v>
+        <v>4360</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -1055,34 +1058,34 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>L697589</v>
+        <v>L704741</v>
       </c>
       <c r="C19" t="str">
-        <v>S B DISCOUNT MART</v>
+        <v>W ADAMS COIN LAUNDRY</v>
       </c>
       <c r="E19">
-        <v>5780</v>
+        <v>4740</v>
       </c>
       <c r="F19" t="str">
         <v>T</v>
       </c>
       <c r="H19">
-        <v>45114.042061423606</v>
+        <v>45122.04206952546</v>
       </c>
       <c r="J19" t="str">
-        <v>06/29/23 19:31</v>
+        <v>07/06/23 14:09</v>
       </c>
       <c r="K19" t="str">
-        <v>06/29/23 19:31</v>
+        <v>07/06/23 11:36</v>
       </c>
       <c r="L19">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M19" t="str">
-        <v>$7,180 as of 6/29/2023 11:54:34 AM</v>
+        <v>$4,740 as of 7/5/2023 3:58:45 AM</v>
       </c>
       <c r="N19">
-        <v>5880</v>
+        <v>4700</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1102,28 +1105,28 @@
         <v>SKY LIQUOR</v>
       </c>
       <c r="E20">
-        <v>5940</v>
+        <v>5880</v>
       </c>
       <c r="F20" t="str">
         <v>T</v>
       </c>
       <c r="H20">
-        <v>45121.042061423606</v>
+        <v>45119.04206952546</v>
       </c>
       <c r="J20" t="str">
-        <v>06/29/23 19:02</v>
+        <v>07/06/23 14:22</v>
       </c>
       <c r="K20" t="str">
-        <v>06/29/23 11:48</v>
+        <v>07/06/23 13:10</v>
       </c>
       <c r="L20">
         <v>0</v>
       </c>
       <c r="M20" t="str">
-        <v>$5,960 as of 6/29/2023 9:48:28 AM</v>
+        <v>$5,880 as of 7/5/2023 10:41:48 AM</v>
       </c>
       <c r="N20">
-        <v>5940</v>
+        <v>5880</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -1143,28 +1146,31 @@
         <v>N S MART</v>
       </c>
       <c r="E21">
-        <v>6020</v>
+        <v>5960</v>
       </c>
       <c r="F21" t="str">
         <v>T</v>
       </c>
       <c r="H21">
-        <v>45407.042061423606</v>
+        <v>45303.04206952546</v>
+      </c>
+      <c r="I21" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J21" t="str">
-        <v>06/28/23 19:23</v>
+        <v>07/04/23 22:16</v>
       </c>
       <c r="K21" t="str">
-        <v>06/28/23 19:23</v>
+        <v>07/04/23 22:16</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21" t="str">
-        <v>$6,020 as of 6/28/2023 5:23:06 PM</v>
+        <v>$5,960 as of 7/4/2023 8:16:31 PM</v>
       </c>
       <c r="N21">
-        <v>6180</v>
+        <v>6000</v>
       </c>
       <c r="O21">
         <v>0</v>
@@ -1178,34 +1184,37 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>L474817</v>
+        <v>L688966</v>
       </c>
       <c r="C22" t="str">
-        <v>SAFETY MARKET</v>
+        <v>LACON MINI MART</v>
       </c>
       <c r="E22">
-        <v>6440</v>
+        <v>6520</v>
       </c>
       <c r="F22" t="str">
         <v>T</v>
       </c>
       <c r="H22">
-        <v>45123.042061423606</v>
+        <v>45227.04206952546</v>
+      </c>
+      <c r="I22" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J22" t="str">
-        <v>06/29/23 17:44</v>
+        <v>07/04/23 16:10</v>
       </c>
       <c r="K22" t="str">
-        <v>06/29/23 17:44</v>
+        <v>07/04/23 16:10</v>
       </c>
       <c r="L22">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="M22" t="str">
-        <v>$6,480 as of 6/29/2023 7:54:04 AM</v>
+        <v>$6,520 as of 7/4/2023 2:10:50 PM</v>
       </c>
       <c r="N22">
-        <v>6460</v>
+        <v>6620</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -1219,37 +1228,34 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>L688966</v>
+        <v>L678988</v>
       </c>
       <c r="C23" t="str">
-        <v>LACON MINI MART</v>
+        <v>PAYELESS MARKET</v>
       </c>
       <c r="E23">
-        <v>6900</v>
+        <v>7000</v>
       </c>
       <c r="F23" t="str">
         <v>T</v>
       </c>
       <c r="H23">
-        <v>45279.042061423606</v>
-      </c>
-      <c r="I23" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+        <v>45134.04206952546</v>
       </c>
       <c r="J23" t="str">
-        <v>06/25/23 11:10</v>
+        <v>07/05/23 19:44</v>
       </c>
       <c r="K23" t="str">
-        <v>06/22/23 16:56</v>
+        <v>07/05/23 19:44</v>
       </c>
       <c r="L23">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M23" t="str">
-        <v>$6,900 as of 6/22/2023 2:56:56 PM</v>
+        <v>$7,000 as of 7/3/2023 4:44:25 PM</v>
       </c>
       <c r="N23">
-        <v>6920</v>
+        <v>7160</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -1263,31 +1269,37 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>L704741</v>
+        <v>L697590</v>
       </c>
       <c r="C24" t="str">
-        <v>W ADAMS COIN LAUNDRY</v>
+        <v>S B MARKET ST</v>
       </c>
       <c r="E24">
-        <v>8320</v>
+        <v>8780</v>
       </c>
       <c r="F24" t="str">
         <v>T</v>
       </c>
+      <c r="H24">
+        <v>45369.04206952546</v>
+      </c>
+      <c r="I24" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
+      </c>
       <c r="J24" t="str">
-        <v>06/29/23 19:25</v>
+        <v>06/29/23 11:36</v>
       </c>
       <c r="K24" t="str">
-        <v>06/29/23 19:25</v>
+        <v>06/29/23 11:36</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
       <c r="M24" t="str">
-        <v>$8,680 as of 6/29/2023 11:29:36 AM</v>
+        <v>$8,780 as of 6/29/2023 9:36:36 AM</v>
       </c>
       <c r="N24">
-        <v>8460</v>
+        <v>8800</v>
       </c>
       <c r="O24">
         <v>0</v>
@@ -1301,34 +1313,34 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>L697590</v>
+        <v>L697589</v>
       </c>
       <c r="C25" t="str">
-        <v>S B MARKET ST</v>
+        <v>S B DISCOUNT MART</v>
       </c>
       <c r="E25">
-        <v>8780</v>
+        <v>9420</v>
       </c>
       <c r="F25" t="str">
         <v>T</v>
       </c>
       <c r="H25">
-        <v>45120.042061423606</v>
+        <v>45119.04206952546</v>
       </c>
       <c r="J25" t="str">
-        <v>06/29/23 11:36</v>
+        <v>07/06/23 13:51</v>
       </c>
       <c r="K25" t="str">
-        <v>06/29/23 11:36</v>
+        <v>07/06/23 13:51</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="M25" t="str">
-        <v>$8,780 as of 6/29/2023 9:36:36 AM</v>
+        <v>$9,440 as of 7/5/2023 11:48:53 AM</v>
       </c>
       <c r="N25">
-        <v>8800</v>
+        <v>9440</v>
       </c>
       <c r="O25">
         <v>0</v>
@@ -1342,34 +1354,34 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>L678988</v>
+        <v>LK923383</v>
       </c>
       <c r="C26" t="str">
-        <v>PAYELESS MARKET</v>
+        <v>SAMYS PHONE CARDS</v>
       </c>
       <c r="E26">
-        <v>9040</v>
+        <v>10460</v>
       </c>
       <c r="F26" t="str">
         <v>T</v>
       </c>
       <c r="H26">
-        <v>45140.042061423606</v>
+        <v>45127.04206952546</v>
       </c>
       <c r="J26" t="str">
-        <v>06/29/23 17:14</v>
+        <v>07/06/23 13:59</v>
       </c>
       <c r="K26" t="str">
-        <v>06/29/23 14:45</v>
+        <v>07/06/23 13:59</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M26" t="str">
-        <v>$9,240 as of 6/29/2023 10:47:16 AM</v>
+        <v>$10,540 as of 7/3/2023 7:51:00 PM</v>
       </c>
       <c r="N26">
-        <v>9040</v>
+        <v>10540</v>
       </c>
       <c r="O26">
         <v>0</v>
@@ -1389,28 +1401,28 @@
         <v>98 DISCOUNT STORE</v>
       </c>
       <c r="E27">
-        <v>20540</v>
+        <v>21380</v>
       </c>
       <c r="F27" t="str">
         <v>T</v>
       </c>
       <c r="H27">
-        <v>45122.042061423606</v>
+        <v>45121.04206952546</v>
       </c>
       <c r="J27" t="str">
-        <v>06/29/23 18:49</v>
+        <v>07/06/23 13:57</v>
       </c>
       <c r="K27" t="str">
-        <v>06/29/23 18:49</v>
+        <v>07/06/23 13:57</v>
       </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27" t="str">
-        <v>$21,100 as of 6/29/2023 10:23:59 AM</v>
+        <v>$21,400 as of 7/5/2023 11:17:32 AM</v>
       </c>
       <c r="N27">
-        <v>20580</v>
+        <v>21400</v>
       </c>
       <c r="O27">
         <v>0</v>
@@ -1427,7 +1439,7 @@
         <v>Total Outstanding Cash Balance:</v>
       </c>
       <c r="E28">
-        <v>127200</v>
+        <v>121200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set up the error state for user info
</commit_message>
<xml_diff>
--- a/rptTerminalStatusCassetteBalances.xlsx
+++ b/rptTerminalStatusCassetteBalances.xlsx
@@ -478,34 +478,34 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>LK644532</v>
+        <v>L682801</v>
       </c>
       <c r="C5" t="str">
-        <v>SCL ENTERPRISES LAUNDRY</v>
+        <v>SB#5</v>
       </c>
       <c r="E5">
-        <v>1360</v>
+        <v>1260</v>
       </c>
       <c r="F5" t="str">
         <v>T</v>
       </c>
       <c r="H5">
-        <v>45146.042102430554</v>
+        <v>45130.041998113426</v>
       </c>
       <c r="J5" t="str">
-        <v>07/08/23 21:29</v>
+        <v>07/11/23 17:56</v>
       </c>
       <c r="K5" t="str">
-        <v>07/08/23 21:29</v>
+        <v>07/11/23 17:56</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5" t="str">
-        <v>$1,360 as of 7/8/2023 7:29:51 PM</v>
+        <v>$1,280 as of 7/11/2023 11:50:37 AM</v>
       </c>
       <c r="N5">
-        <v>1460</v>
+        <v>1280</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -519,34 +519,34 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>L474761</v>
+        <v>LK644532</v>
       </c>
       <c r="C6" t="str">
-        <v>BABS MARKET</v>
+        <v>SCL ENTERPRISES LAUNDRY</v>
       </c>
       <c r="E6">
-        <v>1680</v>
+        <v>1320</v>
       </c>
       <c r="F6" t="str">
         <v>T</v>
       </c>
       <c r="H6">
-        <v>45121.042102430554</v>
+        <v>45155.041998113426</v>
       </c>
       <c r="J6" t="str">
-        <v>07/09/23 17:18</v>
+        <v>07/11/23 21:44</v>
       </c>
       <c r="K6" t="str">
-        <v>07/09/23 17:18</v>
+        <v>07/11/23 21:44</v>
       </c>
       <c r="L6">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M6" t="str">
-        <v>$1,780 as of 7/9/2023 11:13:41 AM</v>
+        <v>$1,360 as of 7/8/2023 7:29:51 PM</v>
       </c>
       <c r="N6">
-        <v>1780</v>
+        <v>1360</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -560,34 +560,34 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>L682801</v>
+        <v>L474761</v>
       </c>
       <c r="C7" t="str">
-        <v>SB#5</v>
+        <v>BABS MARKET</v>
       </c>
       <c r="E7">
-        <v>1700</v>
+        <v>1520</v>
       </c>
       <c r="F7" t="str">
         <v>T</v>
       </c>
       <c r="H7">
-        <v>45133.042102430554</v>
+        <v>45126.041998113426</v>
       </c>
       <c r="J7" t="str">
-        <v>07/09/23 15:30</v>
+        <v>07/11/23 12:57</v>
       </c>
       <c r="K7" t="str">
-        <v>07/09/23 15:30</v>
+        <v>07/11/23 12:57</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="M7" t="str">
-        <v>$1,760 as of 7/7/2023 11:33:51 AM</v>
+        <v>$1,520 as of 7/11/2023 10:57:39 AM</v>
       </c>
       <c r="N7">
-        <v>1740</v>
+        <v>1600</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -648,28 +648,28 @@
         <v>DONUT &amp; SANDWICH</v>
       </c>
       <c r="E9">
-        <v>2600</v>
+        <v>2420</v>
       </c>
       <c r="F9" t="str">
         <v>T</v>
       </c>
       <c r="H9">
-        <v>45141.042102430554</v>
+        <v>45131.041998113426</v>
       </c>
       <c r="J9" t="str">
-        <v>07/09/23 14:18</v>
+        <v>07/11/23 16:50</v>
       </c>
       <c r="K9" t="str">
-        <v>07/09/23 14:18</v>
+        <v>07/11/23 16:50</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9" t="str">
-        <v>$2,700 as of 7/9/2023 11:41:10 AM</v>
+        <v>$2,440 as of 7/11/2023 11:25:19 AM</v>
       </c>
       <c r="N9">
-        <v>2700</v>
+        <v>2440</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -683,34 +683,34 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>LK561655</v>
+        <v>L474792</v>
       </c>
       <c r="C10" t="str">
-        <v>CRENSHAW CRAVOR #2</v>
+        <v>NICK SHELL SERVICE</v>
       </c>
       <c r="E10">
-        <v>2780</v>
+        <v>2580</v>
       </c>
       <c r="F10" t="str">
         <v>T</v>
       </c>
-      <c r="I10" t="str">
-        <v>ATM Inactive greater than 48 minutes</v>
+      <c r="H10">
+        <v>45164.041998113426</v>
       </c>
       <c r="J10" t="str">
-        <v>01/23/20 08:24</v>
+        <v>07/10/23 22:05</v>
       </c>
       <c r="K10" t="str">
-        <v>01/23/20 08:24</v>
+        <v>07/10/23 22:05</v>
       </c>
       <c r="L10">
         <v>0</v>
       </c>
       <c r="M10" t="str">
-        <v>$2,780 as of 1/23/2020 6:24:32 AM</v>
+        <v>$2,580 as of 7/10/2023 8:05:11 PM</v>
       </c>
       <c r="N10">
-        <v>2800</v>
+        <v>2600</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -724,34 +724,34 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>L474792</v>
+        <v>LK236828</v>
       </c>
       <c r="C11" t="str">
-        <v>NICK SHELL SERVICE</v>
+        <v>WORLDWIDE AUTOMOTIVE</v>
       </c>
       <c r="E11">
-        <v>2800</v>
+        <v>2640</v>
       </c>
       <c r="F11" t="str">
         <v>T</v>
       </c>
       <c r="H11">
-        <v>45156.042102430554</v>
+        <v>45135.041998113426</v>
       </c>
       <c r="J11" t="str">
-        <v>07/09/23 01:48</v>
+        <v>07/11/23 13:12</v>
       </c>
       <c r="K11" t="str">
-        <v>07/09/23 01:48</v>
+        <v>07/11/23 13:12</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="M11" t="str">
-        <v>$2,800 as of 7/8/2023 11:48:15 PM</v>
+        <v>$2,640 as of 7/11/2023 11:12:32 AM</v>
       </c>
       <c r="N11">
-        <v>2840</v>
+        <v>2660</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -765,34 +765,34 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>L688961</v>
+        <v>L474746</v>
       </c>
       <c r="C12" t="str">
-        <v>MONA MART</v>
+        <v>ZACATES MARKET</v>
       </c>
       <c r="E12">
-        <v>2920</v>
+        <v>2680</v>
       </c>
       <c r="F12" t="str">
         <v>T</v>
       </c>
       <c r="H12">
-        <v>45144.042102430554</v>
+        <v>45129.041998113426</v>
       </c>
       <c r="J12" t="str">
-        <v>07/08/23 22:16</v>
+        <v>07/11/23 21:00</v>
       </c>
       <c r="K12" t="str">
-        <v>07/08/23 22:16</v>
+        <v>07/11/23 15:31</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12" t="str">
-        <v>$2,920 as of 7/8/2023 8:16:27 PM</v>
+        <v>$2,780 as of 7/10/2023 5:55:27 PM</v>
       </c>
       <c r="N12">
-        <v>3000</v>
+        <v>2680</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -806,34 +806,34 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>L474746</v>
+        <v>LK561655</v>
       </c>
       <c r="C13" t="str">
-        <v>ZACATES MARKET</v>
+        <v>CRENSHAW CRAVOR #2</v>
       </c>
       <c r="E13">
-        <v>3120</v>
+        <v>2780</v>
       </c>
       <c r="F13" t="str">
         <v>T</v>
       </c>
-      <c r="H13">
-        <v>45127.042102430554</v>
+      <c r="I13" t="str">
+        <v>ATM Inactive greater than 48 minutes</v>
       </c>
       <c r="J13" t="str">
-        <v>07/09/23 14:22</v>
+        <v>01/23/20 08:24</v>
       </c>
       <c r="K13" t="str">
-        <v>07/09/23 14:22</v>
+        <v>01/23/20 08:24</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13" t="str">
-        <v>$3,180 as of 7/9/2023 9:36:25 AM</v>
+        <v>$2,780 as of 1/23/2020 6:24:32 AM</v>
       </c>
       <c r="N13">
-        <v>3180</v>
+        <v>2800</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -847,34 +847,37 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>LK236828</v>
+        <v>L688961</v>
       </c>
       <c r="C14" t="str">
-        <v>WORLDWIDE AUTOMOTIVE</v>
+        <v>MONA MART</v>
       </c>
       <c r="E14">
-        <v>3420</v>
+        <v>2860</v>
       </c>
       <c r="F14" t="str">
         <v>T</v>
       </c>
       <c r="H14">
-        <v>45173.042102430554</v>
+        <v>45143.041998113426</v>
+      </c>
+      <c r="I14" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J14" t="str">
-        <v>07/08/23 19:06</v>
+        <v>07/09/23 19:27</v>
       </c>
       <c r="K14" t="str">
-        <v>07/08/23 19:06</v>
+        <v>07/09/23 19:27</v>
       </c>
       <c r="L14">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="M14" t="str">
-        <v>$3,420 as of 7/8/2023 5:06:45 PM</v>
+        <v>$2,860 as of 7/9/2023 5:27:48 PM</v>
       </c>
       <c r="N14">
-        <v>3520</v>
+        <v>2920</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -935,28 +938,28 @@
         <v>SB#4 MONA MARKET</v>
       </c>
       <c r="E16">
-        <v>4820</v>
+        <v>3980</v>
       </c>
       <c r="F16" t="str">
         <v>T</v>
       </c>
       <c r="H16">
-        <v>45125.042102430554</v>
+        <v>45127.041998113426</v>
       </c>
       <c r="J16" t="str">
-        <v>07/09/23 16:27</v>
+        <v>07/11/23 21:55</v>
       </c>
       <c r="K16" t="str">
-        <v>07/09/23 16:27</v>
+        <v>07/11/23 19:13</v>
       </c>
       <c r="L16">
         <v>100</v>
       </c>
       <c r="M16" t="str">
-        <v>$4,900 as of 7/9/2023 10:56:39 AM</v>
+        <v>$4,040 as of 7/11/2023 11:33:08 AM</v>
       </c>
       <c r="N16">
-        <v>4840</v>
+        <v>3980</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -970,34 +973,34 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>L488595</v>
+        <v>L475090</v>
       </c>
       <c r="C17" t="str">
-        <v>N S MART</v>
+        <v>S.B. 2</v>
       </c>
       <c r="E17">
-        <v>5820</v>
+        <v>4960</v>
       </c>
       <c r="F17" t="str">
         <v>T</v>
       </c>
       <c r="H17">
-        <v>45460.042102430554</v>
+        <v>45123.041998113426</v>
       </c>
       <c r="J17" t="str">
-        <v>07/09/23 15:57</v>
+        <v>07/11/23 21:37</v>
       </c>
       <c r="K17" t="str">
-        <v>07/09/23 15:57</v>
+        <v>07/11/23 21:25</v>
       </c>
       <c r="L17">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="M17" t="str">
-        <v>$5,900 as of 7/7/2023 11:38:03 AM</v>
+        <v>$5,580 as of 7/11/2023 9:25:53 AM</v>
       </c>
       <c r="N17">
-        <v>5860</v>
+        <v>4960</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1011,34 +1014,34 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>L678988</v>
+        <v>L704741</v>
       </c>
       <c r="C18" t="str">
-        <v>PAYELESS MARKET</v>
+        <v>W ADAMS COIN LAUNDRY</v>
       </c>
       <c r="E18">
-        <v>6260</v>
+        <v>4980</v>
       </c>
       <c r="F18" t="str">
         <v>T</v>
       </c>
       <c r="H18">
-        <v>45143.042102430554</v>
+        <v>45125.041998113426</v>
       </c>
       <c r="J18" t="str">
-        <v>07/09/23 14:04</v>
+        <v>07/12/23 00:25</v>
       </c>
       <c r="K18" t="str">
-        <v>07/09/23 14:04</v>
+        <v>07/12/23 00:25</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18" t="str">
-        <v>$6,320 as of 7/9/2023 11:27:08 AM</v>
+        <v>$5,740 as of 7/11/2023 11:50:13 AM</v>
       </c>
       <c r="N18">
-        <v>6320</v>
+        <v>5000</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -1052,34 +1055,34 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>L688966</v>
+        <v>L678988</v>
       </c>
       <c r="C19" t="str">
-        <v>LACON MINI MART</v>
+        <v>PAYELESS MARKET</v>
       </c>
       <c r="E19">
-        <v>6420</v>
+        <v>5560</v>
       </c>
       <c r="F19" t="str">
         <v>T</v>
       </c>
       <c r="H19">
-        <v>45230.042102430554</v>
+        <v>45142.041998113426</v>
       </c>
       <c r="J19" t="str">
-        <v>07/09/23 15:28</v>
+        <v>07/11/23 19:48</v>
       </c>
       <c r="K19" t="str">
-        <v>07/09/23 15:28</v>
+        <v>07/11/23 19:48</v>
       </c>
       <c r="L19">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M19" t="str">
-        <v>$6,500 as of 7/4/2023 2:10:50 PM</v>
+        <v>$5,720 as of 7/11/2023 11:38:49 AM</v>
       </c>
       <c r="N19">
-        <v>6520</v>
+        <v>5660</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1093,34 +1096,34 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>LK864765</v>
+        <v>L488595</v>
       </c>
       <c r="C20" t="str">
-        <v>SKY LIQUOR</v>
+        <v>N S MART</v>
       </c>
       <c r="E20">
-        <v>6700</v>
+        <v>5600</v>
       </c>
       <c r="F20" t="str">
         <v>T</v>
       </c>
       <c r="H20">
-        <v>45125.042102430554</v>
+        <v>45259.041998113426</v>
       </c>
       <c r="J20" t="str">
-        <v>07/09/23 15:49</v>
+        <v>07/11/23 22:35</v>
       </c>
       <c r="K20" t="str">
-        <v>07/09/23 10:02</v>
+        <v>07/11/23 22:35</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="M20" t="str">
-        <v>$6,700 as of 7/9/2023 9:11:23 AM</v>
+        <v>$5,720 as of 7/9/2023 9:11:13 PM</v>
       </c>
       <c r="N20">
-        <v>6700</v>
+        <v>5700</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -1134,34 +1137,34 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>L704741</v>
+        <v>LK864765</v>
       </c>
       <c r="C21" t="str">
-        <v>W ADAMS COIN LAUNDRY</v>
+        <v>SKY LIQUOR</v>
       </c>
       <c r="E21">
-        <v>6720</v>
+        <v>5860</v>
       </c>
       <c r="F21" t="str">
         <v>T</v>
       </c>
       <c r="H21">
-        <v>45126.042102430554</v>
+        <v>45128.041998113426</v>
       </c>
       <c r="J21" t="str">
-        <v>07/09/23 17:15</v>
+        <v>07/11/23 23:52</v>
       </c>
       <c r="K21" t="str">
-        <v>07/09/23 17:15</v>
+        <v>07/11/23 21:55</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21" t="str">
-        <v>$6,840 as of 7/9/2023 11:26:34 AM</v>
+        <v>$6,200 as of 7/10/2023 7:01:11 PM</v>
       </c>
       <c r="N21">
-        <v>6760</v>
+        <v>5860</v>
       </c>
       <c r="O21">
         <v>0</v>
@@ -1175,34 +1178,37 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>L475090</v>
+        <v>L688966</v>
       </c>
       <c r="C22" t="str">
-        <v>S.B. 2</v>
+        <v>LACON MINI MART</v>
       </c>
       <c r="E22">
-        <v>6960</v>
+        <v>6400</v>
       </c>
       <c r="F22" t="str">
         <v>T</v>
       </c>
       <c r="H22">
-        <v>45121.042102430554</v>
+        <v>45343.041998113426</v>
+      </c>
+      <c r="I22" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J22" t="str">
-        <v>07/09/23 17:12</v>
+        <v>07/09/23 22:56</v>
       </c>
       <c r="K22" t="str">
-        <v>07/09/23 17:12</v>
+        <v>07/09/23 15:28</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M22" t="str">
-        <v>$8,060 as of 7/9/2023 11:43:50 AM</v>
+        <v>$6,400 as of 7/9/2023 1:28:46 PM</v>
       </c>
       <c r="N22">
-        <v>7000</v>
+        <v>6420</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -1216,34 +1222,34 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>L474817</v>
+        <v>LK923383</v>
       </c>
       <c r="C23" t="str">
-        <v>SAFETY MARKET</v>
+        <v>SAMYS PHONE CARDS</v>
       </c>
       <c r="E23">
-        <v>8000</v>
+        <v>6480</v>
       </c>
       <c r="F23" t="str">
         <v>T</v>
       </c>
       <c r="H23">
-        <v>45134.042102430554</v>
+        <v>45131.041998113426</v>
       </c>
       <c r="J23" t="str">
-        <v>07/09/23 15:54</v>
+        <v>07/11/23 22:42</v>
       </c>
       <c r="K23" t="str">
-        <v>07/09/23 15:54</v>
+        <v>07/11/23 22:42</v>
       </c>
       <c r="L23">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="M23" t="str">
-        <v>$8,060 as of 7/9/2023 11:14:31 AM</v>
+        <v>$7,420 as of 7/11/2023 11:13:23 AM</v>
       </c>
       <c r="N23">
-        <v>8060</v>
+        <v>6680</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -1257,34 +1263,34 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>LK923383</v>
+        <v>L474817</v>
       </c>
       <c r="C24" t="str">
-        <v>SAMYS PHONE CARDS</v>
+        <v>SAFETY MARKET</v>
       </c>
       <c r="E24">
-        <v>8380</v>
+        <v>7240</v>
       </c>
       <c r="F24" t="str">
         <v>T</v>
       </c>
       <c r="H24">
-        <v>45129.042102430554</v>
+        <v>45134.041998113426</v>
       </c>
       <c r="J24" t="str">
-        <v>07/09/23 17:02</v>
+        <v>07/11/23 13:51</v>
       </c>
       <c r="K24" t="str">
-        <v>07/09/23 16:50</v>
+        <v>07/11/23 00:34</v>
       </c>
       <c r="L24">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="M24" t="str">
-        <v>$8,520 as of 7/9/2023 11:02:48 AM</v>
+        <v>$7,240 as of 7/11/2023 11:51:07 AM</v>
       </c>
       <c r="N24">
-        <v>8380</v>
+        <v>7240</v>
       </c>
       <c r="O24">
         <v>0</v>
@@ -1298,34 +1304,34 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>L697590</v>
+        <v>L697589</v>
       </c>
       <c r="C25" t="str">
-        <v>S B MARKET ST</v>
+        <v>S B DISCOUNT MART</v>
       </c>
       <c r="E25">
-        <v>8780</v>
+        <v>8380</v>
       </c>
       <c r="F25" t="str">
         <v>T</v>
       </c>
-      <c r="I25" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+      <c r="H25">
+        <v>45124.041998113426</v>
       </c>
       <c r="J25" t="str">
-        <v>06/29/23 11:36</v>
+        <v>07/11/23 22:38</v>
       </c>
       <c r="K25" t="str">
-        <v>06/29/23 11:36</v>
+        <v>07/11/23 22:38</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="M25" t="str">
-        <v>$8,780 as of 6/29/2023 9:36:36 AM</v>
+        <v>$9,200 as of 7/11/2023 11:53:30 AM</v>
       </c>
       <c r="N25">
-        <v>8800</v>
+        <v>8460</v>
       </c>
       <c r="O25">
         <v>0</v>
@@ -1339,34 +1345,34 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>L697589</v>
+        <v>L697590</v>
       </c>
       <c r="C26" t="str">
-        <v>S B DISCOUNT MART</v>
+        <v>S B MARKET ST</v>
       </c>
       <c r="E26">
-        <v>11800</v>
+        <v>8780</v>
       </c>
       <c r="F26" t="str">
         <v>T</v>
       </c>
-      <c r="H26">
-        <v>45123.042102430554</v>
+      <c r="I26" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J26" t="str">
-        <v>07/09/23 16:08</v>
+        <v>06/29/23 11:36</v>
       </c>
       <c r="K26" t="str">
-        <v>07/09/23 16:08</v>
+        <v>06/29/23 11:36</v>
       </c>
       <c r="L26">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M26" t="str">
-        <v>$12,180 as of 7/9/2023 11:20:42 AM</v>
+        <v>$8,780 as of 6/29/2023 9:36:36 AM</v>
       </c>
       <c r="N26">
-        <v>11800</v>
+        <v>8800</v>
       </c>
       <c r="O26">
         <v>0</v>
@@ -1386,28 +1392,28 @@
         <v>98 DISCOUNT STORE</v>
       </c>
       <c r="E27">
-        <v>15340</v>
+        <v>11780</v>
       </c>
       <c r="F27" t="str">
         <v>T</v>
       </c>
       <c r="H27">
-        <v>45124.042102430554</v>
+        <v>45125.041998113426</v>
       </c>
       <c r="J27" t="str">
-        <v>07/09/23 16:25</v>
+        <v>07/11/23 22:44</v>
       </c>
       <c r="K27" t="str">
-        <v>07/09/23 16:23</v>
+        <v>07/11/23 22:44</v>
       </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27" t="str">
-        <v>$15,580 as of 7/9/2023 11:23:36 AM</v>
+        <v>$12,320 as of 7/11/2023 11:23:11 AM</v>
       </c>
       <c r="N27">
-        <v>15340</v>
+        <v>11820</v>
       </c>
       <c r="O27">
         <v>0</v>
@@ -1424,7 +1430,7 @@
         <v>Total Outstanding Cash Balance:</v>
       </c>
       <c r="E28">
-        <v>124120</v>
+        <v>105800</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Fixed issues with form doubling up"
</commit_message>
<xml_diff>
--- a/rptTerminalStatusCassetteBalances.xlsx
+++ b/rptTerminalStatusCassetteBalances.xlsx
@@ -484,28 +484,28 @@
         <v>SB#5</v>
       </c>
       <c r="E5">
-        <v>1260</v>
+        <v>580</v>
       </c>
       <c r="F5" t="str">
         <v>T</v>
       </c>
       <c r="H5">
-        <v>45130.041998113426</v>
+        <v>45130.04188321759</v>
       </c>
       <c r="J5" t="str">
-        <v>07/11/23 17:56</v>
+        <v>07/17/23 18:04</v>
       </c>
       <c r="K5" t="str">
-        <v>07/11/23 17:56</v>
+        <v>07/17/23 18:04</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5" t="str">
-        <v>$1,280 as of 7/11/2023 11:50:37 AM</v>
+        <v>$580 as of 7/17/2023 4:04:56 PM</v>
       </c>
       <c r="N5">
-        <v>1280</v>
+        <v>600</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -519,34 +519,34 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>LK644532</v>
+        <v>L474746</v>
       </c>
       <c r="C6" t="str">
-        <v>SCL ENTERPRISES LAUNDRY</v>
+        <v>ZACATES MARKET</v>
       </c>
       <c r="E6">
-        <v>1320</v>
+        <v>640</v>
       </c>
       <c r="F6" t="str">
         <v>T</v>
       </c>
       <c r="H6">
-        <v>45155.041998113426</v>
+        <v>45129.04188321759</v>
       </c>
       <c r="J6" t="str">
-        <v>07/11/23 21:44</v>
+        <v>07/18/23 14:22</v>
       </c>
       <c r="K6" t="str">
-        <v>07/11/23 21:44</v>
+        <v>07/18/23 14:22</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6" t="str">
-        <v>$1,360 as of 7/8/2023 7:29:51 PM</v>
+        <v>$780 as of 7/18/2023 10:19:11 AM</v>
       </c>
       <c r="N6">
-        <v>1360</v>
+        <v>680</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -560,34 +560,37 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>L474761</v>
+        <v>LK644532</v>
       </c>
       <c r="C7" t="str">
-        <v>BABS MARKET</v>
+        <v>SCL ENTERPRISES LAUNDRY</v>
       </c>
       <c r="E7">
-        <v>1520</v>
+        <v>700</v>
       </c>
       <c r="F7" t="str">
         <v>T</v>
       </c>
       <c r="H7">
-        <v>45126.041998113426</v>
+        <v>45133.04188321759</v>
+      </c>
+      <c r="I7" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J7" t="str">
-        <v>07/11/23 12:57</v>
+        <v>07/17/23 20:34</v>
       </c>
       <c r="K7" t="str">
-        <v>07/11/23 12:57</v>
+        <v>07/17/23 20:34</v>
       </c>
       <c r="L7">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M7" t="str">
-        <v>$1,520 as of 7/11/2023 10:57:39 AM</v>
+        <v>$700 as of 7/17/2023 6:34:04 PM</v>
       </c>
       <c r="N7">
-        <v>1600</v>
+        <v>760</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -642,34 +645,34 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>L476340</v>
+        <v>L704741</v>
       </c>
       <c r="C9" t="str">
-        <v>DONUT &amp; SANDWICH</v>
+        <v>W ADAMS COIN LAUNDRY</v>
       </c>
       <c r="E9">
-        <v>2420</v>
+        <v>2100</v>
       </c>
       <c r="F9" t="str">
         <v>T</v>
       </c>
       <c r="H9">
-        <v>45131.041998113426</v>
+        <v>45129.04188321759</v>
       </c>
       <c r="J9" t="str">
-        <v>07/11/23 16:50</v>
+        <v>07/18/23 15:07</v>
       </c>
       <c r="K9" t="str">
-        <v>07/11/23 16:50</v>
+        <v>07/18/23 03:46</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9" t="str">
-        <v>$2,440 as of 7/11/2023 11:25:19 AM</v>
+        <v>$2,100 as of 7/18/2023 10:08:00 AM</v>
       </c>
       <c r="N9">
-        <v>2440</v>
+        <v>2100</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -683,34 +686,34 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>L474792</v>
+        <v>L662336</v>
       </c>
       <c r="C10" t="str">
-        <v>NICK SHELL SERVICE</v>
+        <v>SB#4 MONA MARKET</v>
       </c>
       <c r="E10">
-        <v>2580</v>
+        <v>2260</v>
       </c>
       <c r="F10" t="str">
         <v>T</v>
       </c>
       <c r="H10">
-        <v>45164.041998113426</v>
+        <v>45132.04188321759</v>
       </c>
       <c r="J10" t="str">
-        <v>07/10/23 22:05</v>
+        <v>07/17/23 17:03</v>
       </c>
       <c r="K10" t="str">
-        <v>07/10/23 22:05</v>
+        <v>07/17/23 17:03</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M10" t="str">
-        <v>$2,580 as of 7/10/2023 8:05:11 PM</v>
+        <v>$2,260 as of 7/17/2023 3:03:55 PM</v>
       </c>
       <c r="N10">
-        <v>2600</v>
+        <v>2280</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -724,34 +727,34 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>LK236828</v>
+        <v>LK864765</v>
       </c>
       <c r="C11" t="str">
-        <v>WORLDWIDE AUTOMOTIVE</v>
+        <v>SKY LIQUOR</v>
       </c>
       <c r="E11">
-        <v>2640</v>
+        <v>2340</v>
       </c>
       <c r="F11" t="str">
         <v>T</v>
       </c>
       <c r="H11">
-        <v>45135.041998113426</v>
+        <v>45130.04188321759</v>
       </c>
       <c r="J11" t="str">
-        <v>07/11/23 13:12</v>
+        <v>07/18/23 14:03</v>
       </c>
       <c r="K11" t="str">
-        <v>07/11/23 13:12</v>
+        <v>07/18/23 10:02</v>
       </c>
       <c r="L11">
         <v>80</v>
       </c>
       <c r="M11" t="str">
-        <v>$2,640 as of 7/11/2023 11:12:32 AM</v>
+        <v>$2,420 as of 7/18/2023 8:02:45 AM</v>
       </c>
       <c r="N11">
-        <v>2660</v>
+        <v>2420</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -765,34 +768,34 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>L474746</v>
+        <v>LK561655</v>
       </c>
       <c r="C12" t="str">
-        <v>ZACATES MARKET</v>
+        <v>CRENSHAW CRAVOR #2</v>
       </c>
       <c r="E12">
-        <v>2680</v>
+        <v>2780</v>
       </c>
       <c r="F12" t="str">
         <v>T</v>
       </c>
-      <c r="H12">
-        <v>45129.041998113426</v>
+      <c r="I12" t="str">
+        <v>ATM Inactive greater than 48 minutes</v>
       </c>
       <c r="J12" t="str">
-        <v>07/11/23 21:00</v>
+        <v>01/23/20 08:24</v>
       </c>
       <c r="K12" t="str">
-        <v>07/11/23 15:31</v>
+        <v>01/23/20 08:24</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12" t="str">
-        <v>$2,780 as of 7/10/2023 5:55:27 PM</v>
+        <v>$2,780 as of 1/23/2020 6:24:32 AM</v>
       </c>
       <c r="N12">
-        <v>2680</v>
+        <v>2800</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -806,34 +809,34 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>LK561655</v>
+        <v>L678988</v>
       </c>
       <c r="C13" t="str">
-        <v>CRENSHAW CRAVOR #2</v>
+        <v>PAYELESS MARKET</v>
       </c>
       <c r="E13">
-        <v>2780</v>
+        <v>2860</v>
       </c>
       <c r="F13" t="str">
         <v>T</v>
       </c>
-      <c r="I13" t="str">
-        <v>ATM Inactive greater than 48 minutes</v>
+      <c r="H13">
+        <v>45132.04188321759</v>
       </c>
       <c r="J13" t="str">
-        <v>01/23/20 08:24</v>
+        <v>07/18/23 15:33</v>
       </c>
       <c r="K13" t="str">
-        <v>01/23/20 08:24</v>
+        <v>07/18/23 15:33</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13" t="str">
-        <v>$2,780 as of 1/23/2020 6:24:32 AM</v>
+        <v>$2,880 as of 7/17/2023 5:44:43 PM</v>
       </c>
       <c r="N13">
-        <v>2800</v>
+        <v>2880</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -858,9 +861,6 @@
       <c r="F14" t="str">
         <v>T</v>
       </c>
-      <c r="H14">
-        <v>45143.041998113426</v>
-      </c>
       <c r="I14" t="str">
         <v>ATM Inactive greater than 2000 minutes</v>
       </c>
@@ -891,34 +891,34 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>L475182</v>
+        <v>L474792</v>
       </c>
       <c r="C15" t="str">
-        <v>LA ESQUINA DE ORO</v>
+        <v>NICK SHELL SERVICE</v>
       </c>
       <c r="E15">
-        <v>3800</v>
+        <v>3580</v>
       </c>
       <c r="F15" t="str">
         <v>T</v>
       </c>
-      <c r="I15" t="str">
-        <v>ATM Inactive greater than 48 minutes</v>
+      <c r="H15">
+        <v>45155.04188321759</v>
       </c>
       <c r="J15" t="str">
-        <v>09/16/20 16:57</v>
+        <v>07/18/23 08:53</v>
       </c>
       <c r="K15" t="str">
-        <v>09/15/20 23:38</v>
+        <v>07/18/23 08:53</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15" t="str">
-        <v>$3,800 as of 9/16/2020 1:28:00 PM</v>
+        <v>$3,580 as of 7/18/2023 6:53:29 AM</v>
       </c>
       <c r="N15">
-        <v>3800</v>
+        <v>3640</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -932,34 +932,34 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>L662336</v>
+        <v>L475182</v>
       </c>
       <c r="C16" t="str">
-        <v>SB#4 MONA MARKET</v>
+        <v>LA ESQUINA DE ORO</v>
       </c>
       <c r="E16">
-        <v>3980</v>
+        <v>3800</v>
       </c>
       <c r="F16" t="str">
         <v>T</v>
       </c>
-      <c r="H16">
-        <v>45127.041998113426</v>
+      <c r="I16" t="str">
+        <v>ATM Inactive greater than 48 minutes</v>
       </c>
       <c r="J16" t="str">
-        <v>07/11/23 21:55</v>
+        <v>09/16/20 16:57</v>
       </c>
       <c r="K16" t="str">
-        <v>07/11/23 19:13</v>
+        <v>09/15/20 23:38</v>
       </c>
       <c r="L16">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M16" t="str">
-        <v>$4,040 as of 7/11/2023 11:33:08 AM</v>
+        <v>$3,800 as of 9/16/2020 1:28:00 PM</v>
       </c>
       <c r="N16">
-        <v>3980</v>
+        <v>3800</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -973,34 +973,34 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>L475090</v>
+        <v>L474817</v>
       </c>
       <c r="C17" t="str">
-        <v>S.B. 2</v>
+        <v>SAFETY MARKET</v>
       </c>
       <c r="E17">
-        <v>4960</v>
+        <v>4580</v>
       </c>
       <c r="F17" t="str">
         <v>T</v>
       </c>
       <c r="H17">
-        <v>45123.041998113426</v>
+        <v>45138.04188321759</v>
       </c>
       <c r="J17" t="str">
-        <v>07/11/23 21:37</v>
+        <v>07/18/23 15:08</v>
       </c>
       <c r="K17" t="str">
-        <v>07/11/23 21:25</v>
+        <v>07/18/23 15:08</v>
       </c>
       <c r="L17">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="M17" t="str">
-        <v>$5,580 as of 7/11/2023 9:25:53 AM</v>
+        <v>$4,620 as of 7/18/2023 10:05:20 AM</v>
       </c>
       <c r="N17">
-        <v>4960</v>
+        <v>4620</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1014,34 +1014,34 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>L704741</v>
+        <v>L476340</v>
       </c>
       <c r="C18" t="str">
-        <v>W ADAMS COIN LAUNDRY</v>
+        <v>DONUT &amp; SANDWICH</v>
       </c>
       <c r="E18">
-        <v>4980</v>
+        <v>4640</v>
       </c>
       <c r="F18" t="str">
         <v>T</v>
       </c>
       <c r="H18">
-        <v>45125.041998113426</v>
+        <v>45145.04188321759</v>
       </c>
       <c r="J18" t="str">
-        <v>07/12/23 00:25</v>
+        <v>07/18/23 14:23</v>
       </c>
       <c r="K18" t="str">
-        <v>07/12/23 00:25</v>
+        <v>07/18/23 14:23</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18" t="str">
-        <v>$5,740 as of 7/11/2023 11:50:13 AM</v>
+        <v>$4,700 as of 7/18/2023 8:03:40 AM</v>
       </c>
       <c r="N18">
-        <v>5000</v>
+        <v>4700</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -1055,34 +1055,37 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>L678988</v>
+        <v>L488595</v>
       </c>
       <c r="C19" t="str">
-        <v>PAYELESS MARKET</v>
+        <v>N S MART</v>
       </c>
       <c r="E19">
-        <v>5560</v>
+        <v>5480</v>
       </c>
       <c r="F19" t="str">
         <v>T</v>
       </c>
       <c r="H19">
-        <v>45142.041998113426</v>
+        <v>45285.04188321759</v>
+      </c>
+      <c r="I19" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J19" t="str">
-        <v>07/11/23 19:48</v>
+        <v>07/16/23 01:58</v>
       </c>
       <c r="K19" t="str">
-        <v>07/11/23 19:48</v>
+        <v>07/16/23 01:58</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="M19" t="str">
-        <v>$5,720 as of 7/11/2023 11:38:49 AM</v>
+        <v>$5,480 as of 7/15/2023 11:58:38 PM</v>
       </c>
       <c r="N19">
-        <v>5660</v>
+        <v>5580</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1096,34 +1099,34 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>L488595</v>
+        <v>LK236828</v>
       </c>
       <c r="C20" t="str">
-        <v>N S MART</v>
+        <v>WORLDWIDE AUTOMOTIVE</v>
       </c>
       <c r="E20">
-        <v>5600</v>
+        <v>5480</v>
       </c>
       <c r="F20" t="str">
         <v>T</v>
       </c>
       <c r="H20">
-        <v>45259.041998113426</v>
+        <v>45151.04188321759</v>
       </c>
       <c r="J20" t="str">
-        <v>07/11/23 22:35</v>
+        <v>07/17/23 20:02</v>
       </c>
       <c r="K20" t="str">
-        <v>07/11/23 22:35</v>
+        <v>07/17/23 20:02</v>
       </c>
       <c r="L20">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="M20" t="str">
-        <v>$5,720 as of 7/9/2023 9:11:13 PM</v>
+        <v>$5,480 as of 7/17/2023 6:02:33 PM</v>
       </c>
       <c r="N20">
-        <v>5700</v>
+        <v>5500</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -1137,34 +1140,34 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>LK864765</v>
+        <v>L688966</v>
       </c>
       <c r="C21" t="str">
-        <v>SKY LIQUOR</v>
+        <v>LACON MINI MART</v>
       </c>
       <c r="E21">
-        <v>5860</v>
+        <v>6400</v>
       </c>
       <c r="F21" t="str">
         <v>T</v>
       </c>
-      <c r="H21">
-        <v>45128.041998113426</v>
+      <c r="I21" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J21" t="str">
-        <v>07/11/23 23:52</v>
+        <v>07/09/23 22:56</v>
       </c>
       <c r="K21" t="str">
-        <v>07/11/23 21:55</v>
+        <v>07/09/23 15:28</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M21" t="str">
-        <v>$6,200 as of 7/10/2023 7:01:11 PM</v>
+        <v>$6,400 as of 7/9/2023 1:28:46 PM</v>
       </c>
       <c r="N21">
-        <v>5860</v>
+        <v>6420</v>
       </c>
       <c r="O21">
         <v>0</v>
@@ -1178,37 +1181,34 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>L688966</v>
+        <v>L474761</v>
       </c>
       <c r="C22" t="str">
-        <v>LACON MINI MART</v>
+        <v>BABS MARKET</v>
       </c>
       <c r="E22">
-        <v>6400</v>
+        <v>6740</v>
       </c>
       <c r="F22" t="str">
         <v>T</v>
       </c>
       <c r="H22">
-        <v>45343.041998113426</v>
-      </c>
-      <c r="I22" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+        <v>45180.04188321759</v>
       </c>
       <c r="J22" t="str">
-        <v>07/09/23 22:56</v>
+        <v>07/18/23 14:05</v>
       </c>
       <c r="K22" t="str">
-        <v>07/09/23 15:28</v>
+        <v>07/18/23 14:05</v>
       </c>
       <c r="L22">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="M22" t="str">
-        <v>$6,400 as of 7/9/2023 1:28:46 PM</v>
+        <v>$6,780 as of 7/16/2023 9:53:05 AM</v>
       </c>
       <c r="N22">
-        <v>6420</v>
+        <v>6780</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -1222,34 +1222,34 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>LK923383</v>
+        <v>L475090</v>
       </c>
       <c r="C23" t="str">
-        <v>SAMYS PHONE CARDS</v>
+        <v>S.B. 2</v>
       </c>
       <c r="E23">
-        <v>6480</v>
+        <v>7900</v>
       </c>
       <c r="F23" t="str">
         <v>T</v>
       </c>
       <c r="H23">
-        <v>45131.041998113426</v>
+        <v>45134.04188321759</v>
       </c>
       <c r="J23" t="str">
-        <v>07/11/23 22:42</v>
+        <v>07/18/23 12:20</v>
       </c>
       <c r="K23" t="str">
-        <v>07/11/23 22:42</v>
+        <v>07/18/23 12:20</v>
       </c>
       <c r="L23">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M23" t="str">
-        <v>$7,420 as of 7/11/2023 11:13:23 AM</v>
+        <v>$7,900 as of 7/18/2023 10:20:54 AM</v>
       </c>
       <c r="N23">
-        <v>6680</v>
+        <v>8000</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -1263,34 +1263,34 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>L474817</v>
+        <v>LK923383</v>
       </c>
       <c r="C24" t="str">
-        <v>SAFETY MARKET</v>
+        <v>SAMYS PHONE CARDS</v>
       </c>
       <c r="E24">
-        <v>7240</v>
+        <v>8180</v>
       </c>
       <c r="F24" t="str">
         <v>T</v>
       </c>
       <c r="H24">
-        <v>45134.041998113426</v>
+        <v>45133.04188321759</v>
       </c>
       <c r="J24" t="str">
-        <v>07/11/23 13:51</v>
+        <v>07/18/23 15:32</v>
       </c>
       <c r="K24" t="str">
-        <v>07/11/23 00:34</v>
+        <v>07/18/23 15:32</v>
       </c>
       <c r="L24">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="M24" t="str">
-        <v>$7,240 as of 7/11/2023 11:51:07 AM</v>
+        <v>$8,200 as of 7/17/2023 8:23:28 PM</v>
       </c>
       <c r="N24">
-        <v>7240</v>
+        <v>8200</v>
       </c>
       <c r="O24">
         <v>0</v>
@@ -1304,34 +1304,34 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>L697589</v>
+        <v>L697590</v>
       </c>
       <c r="C25" t="str">
-        <v>S B DISCOUNT MART</v>
+        <v>S B MARKET ST</v>
       </c>
       <c r="E25">
-        <v>8380</v>
+        <v>8780</v>
       </c>
       <c r="F25" t="str">
         <v>T</v>
       </c>
-      <c r="H25">
-        <v>45124.041998113426</v>
+      <c r="I25" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J25" t="str">
-        <v>07/11/23 22:38</v>
+        <v>06/29/23 11:36</v>
       </c>
       <c r="K25" t="str">
-        <v>07/11/23 22:38</v>
+        <v>06/29/23 11:36</v>
       </c>
       <c r="L25">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M25" t="str">
-        <v>$9,200 as of 7/11/2023 11:53:30 AM</v>
+        <v>$8,780 as of 6/29/2023 9:36:36 AM</v>
       </c>
       <c r="N25">
-        <v>8460</v>
+        <v>8800</v>
       </c>
       <c r="O25">
         <v>0</v>
@@ -1345,34 +1345,34 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>L697590</v>
+        <v>L697589</v>
       </c>
       <c r="C26" t="str">
-        <v>S B MARKET ST</v>
+        <v>S B DISCOUNT MART</v>
       </c>
       <c r="E26">
-        <v>8780</v>
+        <v>11360</v>
       </c>
       <c r="F26" t="str">
         <v>T</v>
       </c>
-      <c r="I26" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+      <c r="H26">
+        <v>45131.04188321759</v>
       </c>
       <c r="J26" t="str">
-        <v>06/29/23 11:36</v>
+        <v>07/18/23 15:06</v>
       </c>
       <c r="K26" t="str">
-        <v>06/29/23 11:36</v>
+        <v>07/18/23 15:06</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="M26" t="str">
-        <v>$8,780 as of 6/29/2023 9:36:36 AM</v>
+        <v>$11,680 as of 7/18/2023 10:57:39 AM</v>
       </c>
       <c r="N26">
-        <v>8800</v>
+        <v>11540</v>
       </c>
       <c r="O26">
         <v>0</v>
@@ -1392,28 +1392,28 @@
         <v>98 DISCOUNT STORE</v>
       </c>
       <c r="E27">
-        <v>11780</v>
+        <v>16320</v>
       </c>
       <c r="F27" t="str">
         <v>T</v>
       </c>
       <c r="H27">
-        <v>45125.041998113426</v>
+        <v>45129.04188321759</v>
       </c>
       <c r="J27" t="str">
-        <v>07/11/23 22:44</v>
+        <v>07/18/23 15:45</v>
       </c>
       <c r="K27" t="str">
-        <v>07/11/23 22:44</v>
+        <v>07/18/23 15:45</v>
       </c>
       <c r="L27">
         <v>0</v>
       </c>
       <c r="M27" t="str">
-        <v>$12,320 as of 7/11/2023 11:23:11 AM</v>
+        <v>$16,600 as of 7/18/2023 11:33:29 AM</v>
       </c>
       <c r="N27">
-        <v>11820</v>
+        <v>16360</v>
       </c>
       <c r="O27">
         <v>0</v>
@@ -1430,7 +1430,7 @@
         <v>Total Outstanding Cash Balance:</v>
       </c>
       <c r="E28">
-        <v>105800</v>
+        <v>112300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
making fixes to allow building
</commit_message>
<xml_diff>
--- a/rptTerminalStatusCassetteBalances.xlsx
+++ b/rptTerminalStatusCassetteBalances.xlsx
@@ -534,7 +534,7 @@
         <v>45129.04188321759</v>
       </c>
       <c r="J6" t="str">
-        <v>07/18/23 14:22</v>
+        <v>07/18/23 17:59</v>
       </c>
       <c r="K6" t="str">
         <v>07/18/23 14:22</v>
@@ -546,7 +546,7 @@
         <v>$780 as of 7/18/2023 10:19:11 AM</v>
       </c>
       <c r="N6">
-        <v>680</v>
+        <v>640</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -604,34 +604,34 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>L647934</v>
+        <v>LK864765</v>
       </c>
       <c r="C8" t="str">
-        <v>SB #6</v>
+        <v>SKY LIQUOR</v>
       </c>
       <c r="E8">
-        <v>1940</v>
+        <v>1560</v>
       </c>
       <c r="F8" t="str">
         <v>T</v>
       </c>
-      <c r="I8" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+      <c r="H8">
+        <v>45130.04188321759</v>
       </c>
       <c r="J8" t="str">
-        <v>04/06/23 22:10</v>
+        <v>07/18/23 18:03</v>
       </c>
       <c r="K8" t="str">
-        <v>04/06/23 22:05</v>
+        <v>07/18/23 17:46</v>
       </c>
       <c r="L8">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="M8" t="str">
-        <v>$1,940 as of 4/6/2023 8:05:45 PM</v>
+        <v>$2,420 as of 7/18/2023 8:02:45 AM</v>
       </c>
       <c r="N8">
-        <v>1960</v>
+        <v>1640</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -645,34 +645,34 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>L704741</v>
+        <v>L647934</v>
       </c>
       <c r="C9" t="str">
-        <v>W ADAMS COIN LAUNDRY</v>
+        <v>SB #6</v>
       </c>
       <c r="E9">
-        <v>2100</v>
+        <v>1940</v>
       </c>
       <c r="F9" t="str">
         <v>T</v>
       </c>
-      <c r="H9">
-        <v>45129.04188321759</v>
+      <c r="I9" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J9" t="str">
-        <v>07/18/23 15:07</v>
+        <v>04/06/23 22:10</v>
       </c>
       <c r="K9" t="str">
-        <v>07/18/23 03:46</v>
+        <v>04/06/23 22:05</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M9" t="str">
-        <v>$2,100 as of 7/18/2023 10:08:00 AM</v>
+        <v>$1,940 as of 4/6/2023 8:05:45 PM</v>
       </c>
       <c r="N9">
-        <v>2100</v>
+        <v>1960</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -686,34 +686,34 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>L662336</v>
+        <v>L704741</v>
       </c>
       <c r="C10" t="str">
-        <v>SB#4 MONA MARKET</v>
+        <v>W ADAMS COIN LAUNDRY</v>
       </c>
       <c r="E10">
-        <v>2260</v>
+        <v>2020</v>
       </c>
       <c r="F10" t="str">
         <v>T</v>
       </c>
       <c r="H10">
-        <v>45132.04188321759</v>
+        <v>45129.04188321759</v>
       </c>
       <c r="J10" t="str">
-        <v>07/17/23 17:03</v>
+        <v>07/18/23 18:59</v>
       </c>
       <c r="K10" t="str">
-        <v>07/17/23 17:03</v>
+        <v>07/18/23 18:59</v>
       </c>
       <c r="L10">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M10" t="str">
-        <v>$2,260 as of 7/17/2023 3:03:55 PM</v>
+        <v>$2,100 as of 7/18/2023 10:08:00 AM</v>
       </c>
       <c r="N10">
-        <v>2280</v>
+        <v>2080</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -727,34 +727,34 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>LK864765</v>
+        <v>L662336</v>
       </c>
       <c r="C11" t="str">
-        <v>SKY LIQUOR</v>
+        <v>SB#4 MONA MARKET</v>
       </c>
       <c r="E11">
-        <v>2340</v>
+        <v>2260</v>
       </c>
       <c r="F11" t="str">
         <v>T</v>
       </c>
       <c r="H11">
-        <v>45130.04188321759</v>
+        <v>45132.04188321759</v>
       </c>
       <c r="J11" t="str">
-        <v>07/18/23 14:03</v>
+        <v>07/18/23 17:18</v>
       </c>
       <c r="K11" t="str">
-        <v>07/18/23 10:02</v>
+        <v>07/17/23 17:03</v>
       </c>
       <c r="L11">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="M11" t="str">
-        <v>$2,420 as of 7/18/2023 8:02:45 AM</v>
+        <v>$2,260 as of 7/17/2023 3:03:55 PM</v>
       </c>
       <c r="N11">
-        <v>2420</v>
+        <v>2260</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -897,7 +897,7 @@
         <v>NICK SHELL SERVICE</v>
       </c>
       <c r="E15">
-        <v>3580</v>
+        <v>3540</v>
       </c>
       <c r="F15" t="str">
         <v>T</v>
@@ -906,10 +906,10 @@
         <v>45155.04188321759</v>
       </c>
       <c r="J15" t="str">
-        <v>07/18/23 08:53</v>
+        <v>07/18/23 16:42</v>
       </c>
       <c r="K15" t="str">
-        <v>07/18/23 08:53</v>
+        <v>07/18/23 16:42</v>
       </c>
       <c r="L15">
         <v>0</v>
@@ -918,7 +918,7 @@
         <v>$3,580 as of 7/18/2023 6:53:29 AM</v>
       </c>
       <c r="N15">
-        <v>3640</v>
+        <v>3580</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -979,7 +979,7 @@
         <v>SAFETY MARKET</v>
       </c>
       <c r="E17">
-        <v>4580</v>
+        <v>4480</v>
       </c>
       <c r="F17" t="str">
         <v>T</v>
@@ -988,10 +988,10 @@
         <v>45138.04188321759</v>
       </c>
       <c r="J17" t="str">
-        <v>07/18/23 15:08</v>
+        <v>07/18/23 17:49</v>
       </c>
       <c r="K17" t="str">
-        <v>07/18/23 15:08</v>
+        <v>07/18/23 17:28</v>
       </c>
       <c r="L17">
         <v>120</v>
@@ -1000,7 +1000,7 @@
         <v>$4,620 as of 7/18/2023 10:05:20 AM</v>
       </c>
       <c r="N17">
-        <v>4620</v>
+        <v>4480</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1020,7 +1020,7 @@
         <v>DONUT &amp; SANDWICH</v>
       </c>
       <c r="E18">
-        <v>4640</v>
+        <v>4960</v>
       </c>
       <c r="F18" t="str">
         <v>T</v>
@@ -1029,19 +1029,19 @@
         <v>45145.04188321759</v>
       </c>
       <c r="J18" t="str">
-        <v>07/18/23 14:23</v>
+        <v>07/18/23 17:43</v>
       </c>
       <c r="K18" t="str">
-        <v>07/18/23 14:23</v>
+        <v>07/18/23 17:43</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M18" t="str">
         <v>$4,700 as of 7/18/2023 8:03:40 AM</v>
       </c>
       <c r="N18">
-        <v>4700</v>
+        <v>5000</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -1055,37 +1055,34 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>L488595</v>
+        <v>LK236828</v>
       </c>
       <c r="C19" t="str">
-        <v>N S MART</v>
+        <v>WORLDWIDE AUTOMOTIVE</v>
       </c>
       <c r="E19">
+        <v>5380</v>
+      </c>
+      <c r="F19" t="str">
+        <v>T</v>
+      </c>
+      <c r="H19">
+        <v>45151.04188321759</v>
+      </c>
+      <c r="J19" t="str">
+        <v>07/18/23 17:06</v>
+      </c>
+      <c r="K19" t="str">
+        <v>07/18/23 17:06</v>
+      </c>
+      <c r="L19">
+        <v>80</v>
+      </c>
+      <c r="M19" t="str">
+        <v>$5,480 as of 7/17/2023 6:02:33 PM</v>
+      </c>
+      <c r="N19">
         <v>5480</v>
-      </c>
-      <c r="F19" t="str">
-        <v>T</v>
-      </c>
-      <c r="H19">
-        <v>45285.04188321759</v>
-      </c>
-      <c r="I19" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
-      </c>
-      <c r="J19" t="str">
-        <v>07/16/23 01:58</v>
-      </c>
-      <c r="K19" t="str">
-        <v>07/16/23 01:58</v>
-      </c>
-      <c r="L19">
-        <v>60</v>
-      </c>
-      <c r="M19" t="str">
-        <v>$5,480 as of 7/15/2023 11:58:38 PM</v>
-      </c>
-      <c r="N19">
-        <v>5580</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1099,10 +1096,10 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>LK236828</v>
+        <v>L488595</v>
       </c>
       <c r="C20" t="str">
-        <v>WORLDWIDE AUTOMOTIVE</v>
+        <v>N S MART</v>
       </c>
       <c r="E20">
         <v>5480</v>
@@ -1111,22 +1108,25 @@
         <v>T</v>
       </c>
       <c r="H20">
-        <v>45151.04188321759</v>
+        <v>45285.04188321759</v>
+      </c>
+      <c r="I20" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J20" t="str">
-        <v>07/17/23 20:02</v>
+        <v>07/16/23 01:58</v>
       </c>
       <c r="K20" t="str">
-        <v>07/17/23 20:02</v>
+        <v>07/16/23 01:58</v>
       </c>
       <c r="L20">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="M20" t="str">
-        <v>$5,480 as of 7/17/2023 6:02:33 PM</v>
+        <v>$5,480 as of 7/15/2023 11:58:38 PM</v>
       </c>
       <c r="N20">
-        <v>5500</v>
+        <v>5580</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -1228,7 +1228,7 @@
         <v>S.B. 2</v>
       </c>
       <c r="E23">
-        <v>7900</v>
+        <v>7400</v>
       </c>
       <c r="F23" t="str">
         <v>T</v>
@@ -1237,10 +1237,10 @@
         <v>45134.04188321759</v>
       </c>
       <c r="J23" t="str">
-        <v>07/18/23 12:20</v>
+        <v>07/18/23 19:24</v>
       </c>
       <c r="K23" t="str">
-        <v>07/18/23 12:20</v>
+        <v>07/18/23 19:24</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -1249,7 +1249,7 @@
         <v>$7,900 as of 7/18/2023 10:20:54 AM</v>
       </c>
       <c r="N23">
-        <v>8000</v>
+        <v>7600</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -1269,7 +1269,7 @@
         <v>SAMYS PHONE CARDS</v>
       </c>
       <c r="E24">
-        <v>8180</v>
+        <v>7960</v>
       </c>
       <c r="F24" t="str">
         <v>T</v>
@@ -1278,10 +1278,10 @@
         <v>45133.04188321759</v>
       </c>
       <c r="J24" t="str">
-        <v>07/18/23 15:32</v>
+        <v>07/18/23 18:58</v>
       </c>
       <c r="K24" t="str">
-        <v>07/18/23 15:32</v>
+        <v>07/18/23 18:58</v>
       </c>
       <c r="L24">
         <v>100</v>
@@ -1290,7 +1290,7 @@
         <v>$8,200 as of 7/17/2023 8:23:28 PM</v>
       </c>
       <c r="N24">
-        <v>8200</v>
+        <v>8160</v>
       </c>
       <c r="O24">
         <v>0</v>
@@ -1351,7 +1351,7 @@
         <v>S B DISCOUNT MART</v>
       </c>
       <c r="E26">
-        <v>11360</v>
+        <v>11260</v>
       </c>
       <c r="F26" t="str">
         <v>T</v>
@@ -1360,10 +1360,10 @@
         <v>45131.04188321759</v>
       </c>
       <c r="J26" t="str">
-        <v>07/18/23 15:06</v>
+        <v>07/18/23 17:32</v>
       </c>
       <c r="K26" t="str">
-        <v>07/18/23 15:06</v>
+        <v>07/18/23 17:32</v>
       </c>
       <c r="L26">
         <v>40</v>
@@ -1372,7 +1372,7 @@
         <v>$11,680 as of 7/18/2023 10:57:39 AM</v>
       </c>
       <c r="N26">
-        <v>11540</v>
+        <v>11360</v>
       </c>
       <c r="O26">
         <v>0</v>
@@ -1392,7 +1392,7 @@
         <v>98 DISCOUNT STORE</v>
       </c>
       <c r="E27">
-        <v>16320</v>
+        <v>16220</v>
       </c>
       <c r="F27" t="str">
         <v>T</v>
@@ -1401,10 +1401,10 @@
         <v>45129.04188321759</v>
       </c>
       <c r="J27" t="str">
-        <v>07/18/23 15:45</v>
+        <v>07/18/23 18:26</v>
       </c>
       <c r="K27" t="str">
-        <v>07/18/23 15:45</v>
+        <v>07/18/23 18:26</v>
       </c>
       <c r="L27">
         <v>0</v>
@@ -1413,7 +1413,7 @@
         <v>$16,600 as of 7/18/2023 11:33:29 AM</v>
       </c>
       <c r="N27">
-        <v>16360</v>
+        <v>16260</v>
       </c>
       <c r="O27">
         <v>0</v>
@@ -1430,7 +1430,7 @@
         <v>Total Outstanding Cash Balance:</v>
       </c>
       <c r="E28">
-        <v>112300</v>
+        <v>110600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added splash page and adjusted login
</commit_message>
<xml_diff>
--- a/rptTerminalStatusCassetteBalances.xlsx
+++ b/rptTerminalStatusCassetteBalances.xlsx
@@ -478,34 +478,34 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>LK644532</v>
+        <v>L474792</v>
       </c>
       <c r="C5" t="str">
-        <v>SCL ENTERPRISES LAUNDRY</v>
+        <v>NICK SHELL SERVICE</v>
       </c>
       <c r="E5">
-        <v>1580</v>
+        <v>1840</v>
       </c>
       <c r="F5" t="str">
         <v>T</v>
       </c>
       <c r="H5">
-        <v>45175.04187299768</v>
+        <v>45241.0421827199</v>
       </c>
       <c r="J5" t="str">
-        <v>08/01/23 22:35</v>
+        <v>10/15/23 13:31</v>
       </c>
       <c r="K5" t="str">
-        <v>08/01/23 22:35</v>
+        <v>10/15/23 13:31</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5" t="str">
-        <v>$1,580 as of 8/1/2023 8:35:31 PM</v>
+        <v>$1,840 as of 10/15/2023 11:31:29 AM</v>
       </c>
       <c r="N5">
-        <v>1600</v>
+        <v>1880</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -519,10 +519,10 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>L474792</v>
+        <v>L647934</v>
       </c>
       <c r="C6" t="str">
-        <v>NICK SHELL SERVICE</v>
+        <v>SB #6</v>
       </c>
       <c r="E6">
         <v>1940</v>
@@ -530,23 +530,23 @@
       <c r="F6" t="str">
         <v>T</v>
       </c>
-      <c r="H6">
-        <v>45173.04187299768</v>
+      <c r="I6" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J6" t="str">
-        <v>08/02/23 09:56</v>
+        <v>04/06/23 22:10</v>
       </c>
       <c r="K6" t="str">
-        <v>08/02/23 09:56</v>
+        <v>04/06/23 22:05</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M6" t="str">
-        <v>$1,940 as of 8/2/2023 7:56:10 AM</v>
+        <v>$1,940 as of 4/6/2023 8:05:45 PM</v>
       </c>
       <c r="N6">
-        <v>2140</v>
+        <v>1960</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -560,34 +560,34 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>L647934</v>
+        <v>LK644532</v>
       </c>
       <c r="C7" t="str">
-        <v>SB #6</v>
+        <v>SCL ENTERPRISES LAUNDRY</v>
       </c>
       <c r="E7">
-        <v>1940</v>
+        <v>2320</v>
       </c>
       <c r="F7" t="str">
         <v>T</v>
       </c>
-      <c r="I7" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+      <c r="H7">
+        <v>45283.0421827199</v>
       </c>
       <c r="J7" t="str">
-        <v>04/06/23 22:10</v>
+        <v>10/16/23 15:08</v>
       </c>
       <c r="K7" t="str">
-        <v>04/06/23 22:05</v>
+        <v>10/16/23 15:08</v>
       </c>
       <c r="L7">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M7" t="str">
-        <v>$1,940 as of 4/6/2023 8:05:45 PM</v>
+        <v>$2,340 as of 10/15/2023 8:14:28 PM</v>
       </c>
       <c r="N7">
-        <v>1960</v>
+        <v>2340</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -601,34 +601,34 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>L697590</v>
+        <v>L678988</v>
       </c>
       <c r="C8" t="str">
-        <v>S B MARKET ST</v>
+        <v>PAYELESS MARKET</v>
       </c>
       <c r="E8">
-        <v>2100</v>
+        <v>2400</v>
       </c>
       <c r="F8" t="str">
         <v>T</v>
       </c>
-      <c r="H8">
-        <v>45154.04187299768</v>
+      <c r="I8" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J8" t="str">
-        <v>08/01/23 19:51</v>
+        <v>07/20/23 20:09</v>
       </c>
       <c r="K8" t="str">
-        <v>08/01/23 17:38</v>
+        <v>07/20/23 20:09</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8" t="str">
-        <v>$2,100 as of 8/1/2023 5:51:56 PM</v>
+        <v>$2,400 as of 7/20/2023 6:09:40 PM</v>
       </c>
       <c r="N8">
-        <v>2100</v>
+        <v>2500</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -642,34 +642,34 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>L678988</v>
+        <v>L688966</v>
       </c>
       <c r="C9" t="str">
-        <v>PAYELESS MARKET</v>
+        <v>S B WESTERN 108TH MARKET</v>
       </c>
       <c r="E9">
-        <v>2400</v>
+        <v>2580</v>
       </c>
       <c r="F9" t="str">
         <v>T</v>
       </c>
-      <c r="I9" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+      <c r="H9">
+        <v>45224.0421827199</v>
       </c>
       <c r="J9" t="str">
-        <v>07/20/23 20:09</v>
+        <v>10/16/23 18:43</v>
       </c>
       <c r="K9" t="str">
-        <v>07/20/23 20:09</v>
+        <v>10/16/23 18:43</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="M9" t="str">
-        <v>$2,400 as of 7/20/2023 6:09:40 PM</v>
+        <v>$2,600 as of 10/16/2023 10:06:02 AM</v>
       </c>
       <c r="N9">
-        <v>2500</v>
+        <v>2600</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -724,34 +724,34 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>L688961</v>
+        <v>L474761</v>
       </c>
       <c r="C11" t="str">
-        <v>MONA MART</v>
+        <v>BABS MARKET</v>
       </c>
       <c r="E11">
-        <v>2860</v>
+        <v>3560</v>
       </c>
       <c r="F11" t="str">
         <v>T</v>
       </c>
-      <c r="I11" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+      <c r="H11">
+        <v>45279.0421827199</v>
       </c>
       <c r="J11" t="str">
-        <v>07/09/23 19:27</v>
+        <v>10/16/23 19:07</v>
       </c>
       <c r="K11" t="str">
-        <v>07/09/23 19:27</v>
+        <v>10/16/23 19:07</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M11" t="str">
-        <v>$2,860 as of 7/9/2023 5:27:48 PM</v>
+        <v>$3,660 as of 10/14/2023 1:54:54 PM</v>
       </c>
       <c r="N11">
-        <v>2920</v>
+        <v>3660</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -765,34 +765,34 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>L474746</v>
+        <v>L475182</v>
       </c>
       <c r="C12" t="str">
-        <v>ZACATES MARKET</v>
+        <v>LA ESQUINA DE ORO</v>
       </c>
       <c r="E12">
-        <v>2940</v>
+        <v>3800</v>
       </c>
       <c r="F12" t="str">
         <v>T</v>
       </c>
-      <c r="H12">
-        <v>45161.04187299768</v>
+      <c r="I12" t="str">
+        <v>ATM Inactive greater than 48 minutes</v>
       </c>
       <c r="J12" t="str">
-        <v>08/02/23 14:43</v>
+        <v>09/16/20 16:57</v>
       </c>
       <c r="K12" t="str">
-        <v>08/02/23 14:43</v>
+        <v>09/15/20 23:38</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12" t="str">
-        <v>$3,000 as of 8/2/2023 11:52:08 AM</v>
+        <v>$3,800 as of 9/16/2020 1:28:00 PM</v>
       </c>
       <c r="N12">
-        <v>3000</v>
+        <v>3800</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -806,34 +806,34 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>L662336</v>
+        <v>L488595</v>
       </c>
       <c r="C13" t="str">
-        <v>SB#4 MONA MARKET</v>
+        <v>N S MART</v>
       </c>
       <c r="E13">
-        <v>3580</v>
+        <v>4060</v>
       </c>
       <c r="F13" t="str">
         <v>T</v>
       </c>
       <c r="H13">
-        <v>45166.04187299768</v>
+        <v>45272.0421827199</v>
       </c>
       <c r="J13" t="str">
-        <v>08/02/23 13:33</v>
+        <v>10/15/23 22:41</v>
       </c>
       <c r="K13" t="str">
-        <v>08/01/23 13:05</v>
+        <v>10/15/23 15:07</v>
       </c>
       <c r="L13">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M13" t="str">
-        <v>$3,580 as of 8/2/2023 11:33:27 AM</v>
+        <v>$4,060 as of 10/15/2023 8:41:09 PM</v>
       </c>
       <c r="N13">
-        <v>3580</v>
+        <v>4060</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -847,34 +847,34 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>L475182</v>
+        <v>L662336</v>
       </c>
       <c r="C14" t="str">
-        <v>LA ESQUINA DE ORO</v>
+        <v>SB#4 MONA MARKET</v>
       </c>
       <c r="E14">
-        <v>3800</v>
+        <v>4580</v>
       </c>
       <c r="F14" t="str">
         <v>T</v>
       </c>
-      <c r="I14" t="str">
-        <v>ATM Inactive greater than 48 minutes</v>
+      <c r="H14">
+        <v>45232.0421827199</v>
       </c>
       <c r="J14" t="str">
-        <v>09/16/20 16:57</v>
+        <v>10/15/23 14:42</v>
       </c>
       <c r="K14" t="str">
-        <v>09/15/20 23:38</v>
+        <v>10/15/23 14:42</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="M14" t="str">
-        <v>$3,800 as of 9/16/2020 1:28:00 PM</v>
+        <v>$4,580 as of 10/15/2023 12:42:04 PM</v>
       </c>
       <c r="N14">
-        <v>3800</v>
+        <v>4580</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -888,34 +888,34 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>LK236828</v>
+        <v>L697590</v>
       </c>
       <c r="C15" t="str">
-        <v>WORLDWIDE AUTOMOTIVE</v>
+        <v>S B MARKET ST</v>
       </c>
       <c r="E15">
-        <v>4140</v>
+        <v>5400</v>
       </c>
       <c r="F15" t="str">
         <v>T</v>
       </c>
       <c r="H15">
-        <v>45152.04187299768</v>
+        <v>45274.0421827199</v>
       </c>
       <c r="J15" t="str">
-        <v>08/02/23 13:31</v>
+        <v>10/16/23 15:58</v>
       </c>
       <c r="K15" t="str">
-        <v>08/02/23 13:31</v>
+        <v>10/16/23 15:58</v>
       </c>
       <c r="L15">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="M15" t="str">
-        <v>$4,140 as of 8/2/2023 11:31:23 AM</v>
+        <v>$5,600 as of 10/15/2023 7:53:24 PM</v>
       </c>
       <c r="N15">
-        <v>4340</v>
+        <v>5600</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -929,34 +929,34 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>L474761</v>
+        <v>LK864765</v>
       </c>
       <c r="C16" t="str">
-        <v>BABS MARKET</v>
+        <v>SKY LIQUOR</v>
       </c>
       <c r="E16">
-        <v>4540</v>
+        <v>5560</v>
       </c>
       <c r="F16" t="str">
         <v>T</v>
       </c>
       <c r="H16">
-        <v>45166.04187299768</v>
+        <v>45230.0421827199</v>
       </c>
       <c r="J16" t="str">
-        <v>08/01/23 21:38</v>
+        <v>10/16/23 18:47</v>
       </c>
       <c r="K16" t="str">
-        <v>08/01/23 19:03</v>
+        <v>10/16/23 15:18</v>
       </c>
       <c r="L16">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="M16" t="str">
-        <v>$4,540 as of 8/1/2023 7:38:26 PM</v>
+        <v>$5,720 as of 10/16/2023 1:38:43 AM</v>
       </c>
       <c r="N16">
-        <v>4540</v>
+        <v>5620</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -970,34 +970,34 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>L474817</v>
+        <v>LK236828</v>
       </c>
       <c r="C17" t="str">
-        <v>SAFETY MARKET</v>
+        <v>WORLDWIDE AUTOMOTIVE</v>
       </c>
       <c r="E17">
-        <v>4560</v>
+        <v>5760</v>
       </c>
       <c r="F17" t="str">
         <v>T</v>
       </c>
       <c r="H17">
-        <v>45146.04187299768</v>
+        <v>45241.0421827199</v>
       </c>
       <c r="J17" t="str">
-        <v>08/02/23 14:41</v>
+        <v>10/16/23 17:49</v>
       </c>
       <c r="K17" t="str">
-        <v>08/02/23 14:41</v>
+        <v>10/16/23 17:49</v>
       </c>
       <c r="L17">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="M17" t="str">
-        <v>$4,760 as of 8/2/2023 10:42:43 AM</v>
+        <v>$6,100 as of 10/14/2023 5:10:56 PM</v>
       </c>
       <c r="N17">
-        <v>4660</v>
+        <v>5860</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1011,34 +1011,34 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>L488595</v>
+        <v>L476340</v>
       </c>
       <c r="C18" t="str">
-        <v>N S MART</v>
+        <v>DONUT &amp; SANDWICH</v>
       </c>
       <c r="E18">
-        <v>5160</v>
+        <v>5800</v>
       </c>
       <c r="F18" t="str">
         <v>T</v>
       </c>
       <c r="H18">
-        <v>45592.04187299768</v>
+        <v>45237.0421827199</v>
       </c>
       <c r="J18" t="str">
-        <v>08/01/23 15:17</v>
+        <v>10/16/23 15:35</v>
       </c>
       <c r="K18" t="str">
-        <v>08/01/23 15:17</v>
+        <v>10/16/23 11:14</v>
       </c>
       <c r="L18">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="M18" t="str">
-        <v>$5,160 as of 8/1/2023 1:17:29 PM</v>
+        <v>$5,800 as of 10/16/2023 9:14:56 AM</v>
       </c>
       <c r="N18">
-        <v>5260</v>
+        <v>5800</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -1052,37 +1052,34 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>L682801</v>
+        <v>L704741</v>
       </c>
       <c r="C19" t="str">
-        <v>SB#5</v>
+        <v>W ADAMS COIN LAUNDRY</v>
       </c>
       <c r="E19">
-        <v>5980</v>
+        <v>6140</v>
       </c>
       <c r="F19" t="str">
         <v>T</v>
       </c>
       <c r="H19">
-        <v>47233.04187299768</v>
-      </c>
-      <c r="I19" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+        <v>45222.0421827199</v>
       </c>
       <c r="J19" t="str">
-        <v>07/27/23 15:18</v>
+        <v>10/16/23 17:46</v>
       </c>
       <c r="K19" t="str">
-        <v>07/27/23 15:18</v>
+        <v>10/16/23 17:46</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19" t="str">
-        <v>$5,980 as of 7/27/2023 1:18:45 PM</v>
+        <v>$6,300 as of 10/16/2023 11:08:11 AM</v>
       </c>
       <c r="N19">
-        <v>6000</v>
+        <v>6160</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1096,34 +1093,34 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>L688966</v>
+        <v>L474817</v>
       </c>
       <c r="C20" t="str">
-        <v>LACON MINI MART</v>
+        <v>SAFETY MARKET</v>
       </c>
       <c r="E20">
-        <v>6400</v>
+        <v>6660</v>
       </c>
       <c r="F20" t="str">
         <v>T</v>
       </c>
-      <c r="I20" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+      <c r="H20">
+        <v>45229.0421827199</v>
       </c>
       <c r="J20" t="str">
-        <v>07/09/23 22:56</v>
+        <v>10/16/23 18:28</v>
       </c>
       <c r="K20" t="str">
-        <v>07/09/23 15:28</v>
+        <v>10/16/23 18:28</v>
       </c>
       <c r="L20">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="M20" t="str">
-        <v>$6,400 as of 7/9/2023 1:28:46 PM</v>
+        <v>$6,720 as of 10/16/2023 10:06:34 AM</v>
       </c>
       <c r="N20">
-        <v>6420</v>
+        <v>6660</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -1137,37 +1134,34 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>L476340</v>
+        <v>L682801</v>
       </c>
       <c r="C21" t="str">
-        <v>DONUT &amp; SANDWICH</v>
+        <v>SB#5</v>
       </c>
       <c r="E21">
-        <v>7860</v>
+        <v>7840</v>
       </c>
       <c r="F21" t="str">
         <v>T</v>
       </c>
-      <c r="H21">
-        <v>45178.04187299768</v>
-      </c>
       <c r="I21" t="str">
-        <v xml:space="preserve">The Triton ATM reported error code 38: Blocked Exit                   </v>
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J21" t="str">
-        <v>08/02/23 10:39</v>
+        <v>09/28/23 15:22</v>
       </c>
       <c r="K21" t="str">
-        <v>08/02/23 10:39</v>
+        <v>09/28/23 12:14</v>
       </c>
       <c r="L21">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M21" t="str">
-        <v>$7,860 as of 8/2/2023 8:39:40 AM</v>
+        <v>$7,840 as of 9/28/2023 12:31:50 PM</v>
       </c>
       <c r="N21">
-        <v>7860</v>
+        <v>7840</v>
       </c>
       <c r="O21">
         <v>0</v>
@@ -1181,34 +1175,34 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>L697589</v>
+        <v>L474746</v>
       </c>
       <c r="C22" t="str">
-        <v>S B DISCOUNT MART</v>
+        <v>ZACATES MARKET</v>
       </c>
       <c r="E22">
-        <v>9340</v>
+        <v>8020</v>
       </c>
       <c r="F22" t="str">
         <v>T</v>
       </c>
       <c r="H22">
-        <v>45149.04187299768</v>
+        <v>45262.0421827199</v>
       </c>
       <c r="J22" t="str">
-        <v>08/02/23 16:04</v>
+        <v>10/16/23 14:19</v>
       </c>
       <c r="K22" t="str">
-        <v>08/02/23 16:04</v>
+        <v>10/16/23 14:19</v>
       </c>
       <c r="L22">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M22" t="str">
-        <v>$9,920 as of 8/2/2023 8:53:51 AM</v>
+        <v>$8,080 as of 10/16/2023 11:09:43 AM</v>
       </c>
       <c r="N22">
-        <v>9440</v>
+        <v>8080</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -1222,34 +1216,34 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>LK864765</v>
+        <v>L475090</v>
       </c>
       <c r="C23" t="str">
-        <v>SKY LIQUOR</v>
+        <v>S.B. 2</v>
       </c>
       <c r="E23">
-        <v>9940</v>
+        <v>9320</v>
       </c>
       <c r="F23" t="str">
         <v>T</v>
       </c>
       <c r="H23">
-        <v>45152.04187299768</v>
+        <v>45239.0421827199</v>
       </c>
       <c r="J23" t="str">
-        <v>08/02/23 16:35</v>
+        <v>10/16/23 13:40</v>
       </c>
       <c r="K23" t="str">
-        <v>08/02/23 16:35</v>
+        <v>10/16/23 13:40</v>
       </c>
       <c r="L23">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="M23" t="str">
-        <v>$10,340 as of 8/2/2023 1:01:57 AM</v>
+        <v>$9,320 as of 10/16/2023 11:40:18 AM</v>
       </c>
       <c r="N23">
-        <v>10140</v>
+        <v>9400</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -1263,34 +1257,34 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>L704741</v>
+        <v>L688961</v>
       </c>
       <c r="C24" t="str">
-        <v>W ADAMS COIN LAUNDRY</v>
+        <v>MONA MART</v>
       </c>
       <c r="E24">
-        <v>10660</v>
+        <v>9480</v>
       </c>
       <c r="F24" t="str">
         <v>T</v>
       </c>
       <c r="H24">
-        <v>45159.04187299768</v>
+        <v>46605.0421827199</v>
       </c>
       <c r="J24" t="str">
-        <v>08/02/23 15:43</v>
+        <v>10/16/23 18:29</v>
       </c>
       <c r="K24" t="str">
-        <v>08/02/23 15:43</v>
+        <v>10/16/23 16:18</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
       <c r="M24" t="str">
-        <v>$10,720 as of 8/2/2023 10:26:30 AM</v>
+        <v>$9,500 as of 10/16/2023 10:30:50 AM</v>
       </c>
       <c r="N24">
-        <v>10720</v>
+        <v>9480</v>
       </c>
       <c r="O24">
         <v>0</v>
@@ -1304,34 +1298,34 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>LK923383</v>
+        <v>L697589</v>
       </c>
       <c r="C25" t="str">
-        <v>SAMYS PHONE CARDS</v>
+        <v>S B DISCOUNT MART</v>
       </c>
       <c r="E25">
-        <v>10720</v>
+        <v>12300</v>
       </c>
       <c r="F25" t="str">
         <v>T</v>
       </c>
       <c r="H25">
-        <v>45156.04187299768</v>
+        <v>45228.0421827199</v>
       </c>
       <c r="J25" t="str">
-        <v>08/02/23 16:29</v>
+        <v>10/16/23 19:00</v>
       </c>
       <c r="K25" t="str">
-        <v>08/02/23 13:22</v>
+        <v>10/16/23 19:00</v>
       </c>
       <c r="L25">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="M25" t="str">
-        <v>$10,720 as of 8/2/2023 11:22:53 AM</v>
+        <v>$12,460 as of 10/16/2023 11:54:58 AM</v>
       </c>
       <c r="N25">
-        <v>10720</v>
+        <v>12460</v>
       </c>
       <c r="O25">
         <v>0</v>
@@ -1345,34 +1339,34 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>L475090</v>
+        <v>LK923383</v>
       </c>
       <c r="C26" t="str">
-        <v>S.B. 2</v>
+        <v>SAMYS PHONE CARDS</v>
       </c>
       <c r="E26">
-        <v>14300</v>
+        <v>12320</v>
       </c>
       <c r="F26" t="str">
         <v>T</v>
       </c>
       <c r="H26">
-        <v>45169.04187299768</v>
+        <v>45237.0421827199</v>
       </c>
       <c r="J26" t="str">
-        <v>08/02/23 16:27</v>
+        <v>10/16/23 17:53</v>
       </c>
       <c r="K26" t="str">
-        <v>08/02/23 16:27</v>
+        <v>10/16/23 17:53</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="M26" t="str">
-        <v>$14,760 as of 8/2/2023 11:27:54 AM</v>
+        <v>$12,640 as of 10/16/2023 10:57:51 AM</v>
       </c>
       <c r="N26">
-        <v>14360</v>
+        <v>12520</v>
       </c>
       <c r="O26">
         <v>0</v>
@@ -1392,28 +1386,28 @@
         <v>98 DISCOUNT STORE</v>
       </c>
       <c r="E27">
-        <v>23660</v>
+        <v>21040</v>
       </c>
       <c r="F27" t="str">
         <v>T</v>
       </c>
       <c r="H27">
-        <v>45155.04187299768</v>
+        <v>45232.0421827199</v>
       </c>
       <c r="J27" t="str">
-        <v>08/02/23 16:30</v>
+        <v>10/16/23 19:04</v>
       </c>
       <c r="K27" t="str">
-        <v>08/02/23 16:30</v>
+        <v>10/16/23 18:59</v>
       </c>
       <c r="L27">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M27" t="str">
-        <v>$24,100 as of 8/2/2023 11:42:24 AM</v>
+        <v>$21,080 as of 10/16/2023 9:46:55 AM</v>
       </c>
       <c r="N27">
-        <v>23700</v>
+        <v>21040</v>
       </c>
       <c r="O27">
         <v>0</v>
@@ -1430,7 +1424,7 @@
         <v>Total Outstanding Cash Balance:</v>
       </c>
       <c r="E28">
-        <v>143180</v>
+        <v>145500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaned up data fetching and db processing
</commit_message>
<xml_diff>
--- a/rptTerminalStatusCassetteBalances.xlsx
+++ b/rptTerminalStatusCassetteBalances.xlsx
@@ -478,34 +478,34 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>L474792</v>
+        <v>LK644532</v>
       </c>
       <c r="C5" t="str">
-        <v>NICK SHELL SERVICE</v>
+        <v>SCL ENTERPRISES LAUNDRY</v>
       </c>
       <c r="E5">
-        <v>1840</v>
+        <v>1720</v>
       </c>
       <c r="F5" t="str">
         <v>T</v>
       </c>
       <c r="H5">
-        <v>45241.0421827199</v>
+        <v>45244.04213364583</v>
       </c>
       <c r="J5" t="str">
-        <v>10/15/23 13:31</v>
+        <v>10/23/23 21:05</v>
       </c>
       <c r="K5" t="str">
-        <v>10/15/23 13:31</v>
+        <v>10/23/23 21:05</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5" t="str">
-        <v>$1,840 as of 10/15/2023 11:31:29 AM</v>
+        <v>$1,720 as of 10/23/2023 7:05:45 PM</v>
       </c>
       <c r="N5">
-        <v>1880</v>
+        <v>1660</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -560,34 +560,34 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>LK644532</v>
+        <v>L678988</v>
       </c>
       <c r="C7" t="str">
-        <v>SCL ENTERPRISES LAUNDRY</v>
+        <v>PAYELESS MARKET</v>
       </c>
       <c r="E7">
-        <v>2320</v>
+        <v>2400</v>
       </c>
       <c r="F7" t="str">
         <v>T</v>
       </c>
-      <c r="H7">
-        <v>45283.0421827199</v>
+      <c r="I7" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J7" t="str">
-        <v>10/16/23 15:08</v>
+        <v>07/20/23 20:09</v>
       </c>
       <c r="K7" t="str">
-        <v>10/16/23 15:08</v>
+        <v>07/20/23 20:09</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7" t="str">
-        <v>$2,340 as of 10/15/2023 8:14:28 PM</v>
+        <v>$2,400 as of 7/20/2023 6:09:40 PM</v>
       </c>
       <c r="N7">
-        <v>2340</v>
+        <v>2500</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -601,34 +601,34 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>L678988</v>
+        <v>LK561655</v>
       </c>
       <c r="C8" t="str">
-        <v>PAYELESS MARKET</v>
+        <v>CRENSHAW CRAVOR #2</v>
       </c>
       <c r="E8">
-        <v>2400</v>
+        <v>2780</v>
       </c>
       <c r="F8" t="str">
         <v>T</v>
       </c>
       <c r="I8" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+        <v>ATM Inactive greater than 48 minutes</v>
       </c>
       <c r="J8" t="str">
-        <v>07/20/23 20:09</v>
+        <v>01/23/20 08:24</v>
       </c>
       <c r="K8" t="str">
-        <v>07/20/23 20:09</v>
+        <v>01/23/20 08:24</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8" t="str">
-        <v>$2,400 as of 7/20/2023 6:09:40 PM</v>
+        <v>$2,780 as of 1/23/2020 6:24:32 AM</v>
       </c>
       <c r="N8">
-        <v>2500</v>
+        <v>2800</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -642,34 +642,34 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>L688966</v>
+        <v>L474792</v>
       </c>
       <c r="C9" t="str">
-        <v>S B WESTERN 108TH MARKET</v>
+        <v>NICK SHELL SERVICE</v>
       </c>
       <c r="E9">
-        <v>2580</v>
+        <v>2860</v>
       </c>
       <c r="F9" t="str">
         <v>T</v>
       </c>
       <c r="H9">
-        <v>45224.0421827199</v>
+        <v>45243.04213364583</v>
       </c>
       <c r="J9" t="str">
-        <v>10/16/23 18:43</v>
+        <v>10/23/23 13:19</v>
       </c>
       <c r="K9" t="str">
-        <v>10/16/23 18:43</v>
+        <v>10/23/23 13:19</v>
       </c>
       <c r="L9">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="M9" t="str">
-        <v>$2,600 as of 10/16/2023 10:06:02 AM</v>
+        <v>$2,860 as of 10/23/2023 11:19:13 AM</v>
       </c>
       <c r="N9">
-        <v>2600</v>
+        <v>2860</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -683,34 +683,34 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>LK561655</v>
+        <v>L662336</v>
       </c>
       <c r="C10" t="str">
-        <v>CRENSHAW CRAVOR #2</v>
+        <v>SB#4 MONA MARKET</v>
       </c>
       <c r="E10">
-        <v>2780</v>
+        <v>3120</v>
       </c>
       <c r="F10" t="str">
         <v>T</v>
       </c>
-      <c r="I10" t="str">
-        <v>ATM Inactive greater than 48 minutes</v>
+      <c r="H10">
+        <v>45239.04213364583</v>
       </c>
       <c r="J10" t="str">
-        <v>01/23/20 08:24</v>
+        <v>10/23/23 16:57</v>
       </c>
       <c r="K10" t="str">
-        <v>01/23/20 08:24</v>
+        <v>10/23/23 16:57</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="M10" t="str">
-        <v>$2,780 as of 1/23/2020 6:24:32 AM</v>
+        <v>$3,120 as of 10/23/2023 2:57:12 PM</v>
       </c>
       <c r="N10">
-        <v>2800</v>
+        <v>3120</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -724,34 +724,37 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>L474761</v>
+        <v>L488595</v>
       </c>
       <c r="C11" t="str">
-        <v>BABS MARKET</v>
+        <v>N S MART</v>
       </c>
       <c r="E11">
-        <v>3560</v>
+        <v>3460</v>
       </c>
       <c r="F11" t="str">
         <v>T</v>
       </c>
       <c r="H11">
-        <v>45279.0421827199</v>
+        <v>45263.04213364583</v>
+      </c>
+      <c r="I11" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J11" t="str">
-        <v>10/16/23 19:07</v>
+        <v>10/22/23 16:35</v>
       </c>
       <c r="K11" t="str">
-        <v>10/16/23 19:07</v>
+        <v>10/22/23 16:35</v>
       </c>
       <c r="L11">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M11" t="str">
-        <v>$3,660 as of 10/14/2023 1:54:54 PM</v>
+        <v>$3,460 as of 10/22/2023 2:35:21 PM</v>
       </c>
       <c r="N11">
-        <v>3660</v>
+        <v>3440</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -806,34 +809,37 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>L488595</v>
+        <v>L688961</v>
       </c>
       <c r="C13" t="str">
-        <v>N S MART</v>
+        <v>MONA MART</v>
       </c>
       <c r="E13">
-        <v>4060</v>
+        <v>4000</v>
       </c>
       <c r="F13" t="str">
         <v>T</v>
       </c>
       <c r="H13">
-        <v>45272.0421827199</v>
+        <v>45456.04213364583</v>
+      </c>
+      <c r="I13" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J13" t="str">
-        <v>10/15/23 22:41</v>
+        <v>10/17/23 13:26</v>
       </c>
       <c r="K13" t="str">
-        <v>10/15/23 15:07</v>
+        <v>10/17/23 13:00</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13" t="str">
-        <v>$4,060 as of 10/15/2023 8:41:09 PM</v>
+        <v>$4,000 as of 10/17/2023 11:00:09 AM</v>
       </c>
       <c r="N13">
-        <v>4060</v>
+        <v>4000</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -847,34 +853,34 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>L662336</v>
+        <v>L476340</v>
       </c>
       <c r="C14" t="str">
-        <v>SB#4 MONA MARKET</v>
+        <v>DONUT &amp; SANDWICH</v>
       </c>
       <c r="E14">
-        <v>4580</v>
+        <v>4040</v>
       </c>
       <c r="F14" t="str">
         <v>T</v>
       </c>
       <c r="H14">
-        <v>45232.0421827199</v>
+        <v>45242.04213364583</v>
       </c>
       <c r="J14" t="str">
-        <v>10/15/23 14:42</v>
+        <v>10/24/23 14:06</v>
       </c>
       <c r="K14" t="str">
-        <v>10/15/23 14:42</v>
+        <v>10/24/23 14:06</v>
       </c>
       <c r="L14">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="M14" t="str">
-        <v>$4,580 as of 10/15/2023 12:42:04 PM</v>
+        <v>$4,060 as of 10/24/2023 10:00:58 AM</v>
       </c>
       <c r="N14">
-        <v>4580</v>
+        <v>3880</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -894,28 +900,28 @@
         <v>S B MARKET ST</v>
       </c>
       <c r="E15">
-        <v>5400</v>
+        <v>4140</v>
       </c>
       <c r="F15" t="str">
         <v>T</v>
       </c>
       <c r="H15">
-        <v>45274.0421827199</v>
+        <v>45249.04213364583</v>
       </c>
       <c r="J15" t="str">
-        <v>10/16/23 15:58</v>
+        <v>10/24/23 12:12</v>
       </c>
       <c r="K15" t="str">
-        <v>10/16/23 15:58</v>
+        <v>10/24/23 12:12</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15" t="str">
-        <v>$5,600 as of 10/15/2023 7:53:24 PM</v>
+        <v>$4,140 as of 10/24/2023 10:12:25 AM</v>
       </c>
       <c r="N15">
-        <v>5600</v>
+        <v>4120</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -929,34 +935,34 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>LK864765</v>
+        <v>L474817</v>
       </c>
       <c r="C16" t="str">
-        <v>SKY LIQUOR</v>
+        <v>SAFETY MARKET</v>
       </c>
       <c r="E16">
-        <v>5560</v>
+        <v>4220</v>
       </c>
       <c r="F16" t="str">
         <v>T</v>
       </c>
       <c r="H16">
-        <v>45230.0421827199</v>
+        <v>45237.04213364583</v>
       </c>
       <c r="J16" t="str">
-        <v>10/16/23 18:47</v>
+        <v>10/24/23 14:20</v>
       </c>
       <c r="K16" t="str">
-        <v>10/16/23 15:18</v>
+        <v>10/24/23 14:20</v>
       </c>
       <c r="L16">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="M16" t="str">
-        <v>$5,720 as of 10/16/2023 1:38:43 AM</v>
+        <v>$4,240 as of 10/24/2023 10:34:37 AM</v>
       </c>
       <c r="N16">
-        <v>5620</v>
+        <v>3960</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -976,28 +982,28 @@
         <v>WORLDWIDE AUTOMOTIVE</v>
       </c>
       <c r="E17">
-        <v>5760</v>
+        <v>4300</v>
       </c>
       <c r="F17" t="str">
         <v>T</v>
       </c>
       <c r="H17">
-        <v>45241.0421827199</v>
+        <v>45240.04213364583</v>
       </c>
       <c r="J17" t="str">
-        <v>10/16/23 17:49</v>
+        <v>10/23/23 10:42</v>
       </c>
       <c r="K17" t="str">
-        <v>10/16/23 17:49</v>
+        <v>10/23/23 10:42</v>
       </c>
       <c r="L17">
         <v>20</v>
       </c>
       <c r="M17" t="str">
-        <v>$6,100 as of 10/14/2023 5:10:56 PM</v>
+        <v>$4,300 as of 10/23/2023 8:42:11 AM</v>
       </c>
       <c r="N17">
-        <v>5860</v>
+        <v>4300</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1011,34 +1017,34 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>L476340</v>
+        <v>L688966</v>
       </c>
       <c r="C18" t="str">
-        <v>DONUT &amp; SANDWICH</v>
+        <v>S B WESTERN 108TH MARKET</v>
       </c>
       <c r="E18">
-        <v>5800</v>
+        <v>4680</v>
       </c>
       <c r="F18" t="str">
         <v>T</v>
       </c>
       <c r="H18">
-        <v>45237.0421827199</v>
+        <v>45240.04213364583</v>
       </c>
       <c r="J18" t="str">
-        <v>10/16/23 15:35</v>
+        <v>10/24/23 12:38</v>
       </c>
       <c r="K18" t="str">
-        <v>10/16/23 11:14</v>
+        <v>10/24/23 12:38</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="M18" t="str">
-        <v>$5,800 as of 10/16/2023 9:14:56 AM</v>
+        <v>$4,680 as of 10/24/2023 10:38:11 AM</v>
       </c>
       <c r="N18">
-        <v>5800</v>
+        <v>4620</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -1052,34 +1058,34 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>L704741</v>
+        <v>L697589</v>
       </c>
       <c r="C19" t="str">
-        <v>W ADAMS COIN LAUNDRY</v>
+        <v>S B DISCOUNT MART</v>
       </c>
       <c r="E19">
-        <v>6140</v>
+        <v>5840</v>
       </c>
       <c r="F19" t="str">
         <v>T</v>
       </c>
       <c r="H19">
-        <v>45222.0421827199</v>
+        <v>45232.04213364583</v>
       </c>
       <c r="J19" t="str">
-        <v>10/16/23 17:46</v>
+        <v>10/24/23 14:19</v>
       </c>
       <c r="K19" t="str">
-        <v>10/16/23 17:46</v>
+        <v>10/24/23 14:19</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="M19" t="str">
-        <v>$6,300 as of 10/16/2023 11:08:11 AM</v>
+        <v>$5,900 as of 10/24/2023 10:56:38 AM</v>
       </c>
       <c r="N19">
-        <v>6160</v>
+        <v>5800</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1093,34 +1099,34 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>L474817</v>
+        <v>L475090</v>
       </c>
       <c r="C20" t="str">
-        <v>SAFETY MARKET</v>
+        <v>S.B. 2</v>
       </c>
       <c r="E20">
-        <v>6660</v>
+        <v>6820</v>
       </c>
       <c r="F20" t="str">
         <v>T</v>
       </c>
       <c r="H20">
-        <v>45229.0421827199</v>
+        <v>45254.04213364583</v>
       </c>
       <c r="J20" t="str">
-        <v>10/16/23 18:28</v>
+        <v>10/24/23 10:37</v>
       </c>
       <c r="K20" t="str">
-        <v>10/16/23 18:28</v>
+        <v>10/24/23 10:37</v>
       </c>
       <c r="L20">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="M20" t="str">
-        <v>$6,720 as of 10/16/2023 10:06:34 AM</v>
+        <v>$6,820 as of 10/24/2023 8:37:49 AM</v>
       </c>
       <c r="N20">
-        <v>6660</v>
+        <v>6740</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -1134,34 +1140,34 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>L682801</v>
+        <v>L474746</v>
       </c>
       <c r="C21" t="str">
-        <v>SB#5</v>
+        <v>ZACATES MARKET</v>
       </c>
       <c r="E21">
-        <v>7840</v>
+        <v>6860</v>
       </c>
       <c r="F21" t="str">
         <v>T</v>
       </c>
-      <c r="I21" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+      <c r="H21">
+        <v>45271.04213364583</v>
       </c>
       <c r="J21" t="str">
-        <v>09/28/23 15:22</v>
+        <v>10/24/23 15:21</v>
       </c>
       <c r="K21" t="str">
-        <v>09/28/23 12:14</v>
+        <v>10/24/23 15:18</v>
       </c>
       <c r="L21">
         <v>0</v>
       </c>
       <c r="M21" t="str">
-        <v>$7,840 as of 9/28/2023 12:31:50 PM</v>
+        <v>$6,900 as of 10/24/2023 10:32:02 AM</v>
       </c>
       <c r="N21">
-        <v>7840</v>
+        <v>6840</v>
       </c>
       <c r="O21">
         <v>0</v>
@@ -1175,34 +1181,34 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>L474746</v>
+        <v>L682801</v>
       </c>
       <c r="C22" t="str">
-        <v>ZACATES MARKET</v>
+        <v>SB#5</v>
       </c>
       <c r="E22">
-        <v>8020</v>
+        <v>7840</v>
       </c>
       <c r="F22" t="str">
         <v>T</v>
       </c>
-      <c r="H22">
-        <v>45262.0421827199</v>
+      <c r="I22" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J22" t="str">
-        <v>10/16/23 14:19</v>
+        <v>09/28/23 15:22</v>
       </c>
       <c r="K22" t="str">
-        <v>10/16/23 14:19</v>
+        <v>09/28/23 12:14</v>
       </c>
       <c r="L22">
         <v>0</v>
       </c>
       <c r="M22" t="str">
-        <v>$8,080 as of 10/16/2023 11:09:43 AM</v>
+        <v>$7,840 as of 9/28/2023 12:31:50 PM</v>
       </c>
       <c r="N22">
-        <v>8080</v>
+        <v>7840</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -1216,34 +1222,34 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>L475090</v>
+        <v>L474761</v>
       </c>
       <c r="C23" t="str">
-        <v>S.B. 2</v>
+        <v>BABS MARKET</v>
       </c>
       <c r="E23">
-        <v>9320</v>
+        <v>7960</v>
       </c>
       <c r="F23" t="str">
         <v>T</v>
       </c>
       <c r="H23">
-        <v>45239.0421827199</v>
+        <v>45267.04213364583</v>
       </c>
       <c r="J23" t="str">
-        <v>10/16/23 13:40</v>
+        <v>10/23/23 20:57</v>
       </c>
       <c r="K23" t="str">
-        <v>10/16/23 13:40</v>
+        <v>10/23/23 20:57</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M23" t="str">
-        <v>$9,320 as of 10/16/2023 11:40:18 AM</v>
+        <v>$7,960 as of 10/23/2023 6:57:34 PM</v>
       </c>
       <c r="N23">
-        <v>9400</v>
+        <v>7900</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -1257,34 +1263,34 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>L688961</v>
+        <v>LK864765</v>
       </c>
       <c r="C24" t="str">
-        <v>MONA MART</v>
+        <v>SKY LIQUOR</v>
       </c>
       <c r="E24">
-        <v>9480</v>
+        <v>8740</v>
       </c>
       <c r="F24" t="str">
         <v>T</v>
       </c>
       <c r="H24">
-        <v>46605.0421827199</v>
+        <v>45237.04213364583</v>
       </c>
       <c r="J24" t="str">
-        <v>10/16/23 18:29</v>
+        <v>10/24/23 12:53</v>
       </c>
       <c r="K24" t="str">
-        <v>10/16/23 16:18</v>
+        <v>10/24/23 12:04</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="M24" t="str">
-        <v>$9,500 as of 10/16/2023 10:30:50 AM</v>
+        <v>$8,800 as of 10/24/2023 10:04:24 AM</v>
       </c>
       <c r="N24">
-        <v>9480</v>
+        <v>8780</v>
       </c>
       <c r="O24">
         <v>0</v>
@@ -1298,34 +1304,34 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>L697589</v>
+        <v>L704741</v>
       </c>
       <c r="C25" t="str">
-        <v>S B DISCOUNT MART</v>
+        <v>W ADAMS COIN LAUNDRY</v>
       </c>
       <c r="E25">
-        <v>12300</v>
+        <v>9880</v>
       </c>
       <c r="F25" t="str">
         <v>T</v>
       </c>
       <c r="H25">
-        <v>45228.0421827199</v>
+        <v>45236.04213364583</v>
       </c>
       <c r="J25" t="str">
-        <v>10/16/23 19:00</v>
+        <v>10/24/23 15:12</v>
       </c>
       <c r="K25" t="str">
-        <v>10/16/23 19:00</v>
+        <v>10/24/23 15:12</v>
       </c>
       <c r="L25">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="M25" t="str">
-        <v>$12,460 as of 10/16/2023 11:54:58 AM</v>
+        <v>$9,960 as of 10/24/2023 11:13:30 AM</v>
       </c>
       <c r="N25">
-        <v>12460</v>
+        <v>9660</v>
       </c>
       <c r="O25">
         <v>0</v>
@@ -1339,34 +1345,34 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>LK923383</v>
+        <v>LK891176</v>
       </c>
       <c r="C26" t="str">
-        <v>SAMYS PHONE CARDS</v>
+        <v>98 DISCOUNT STORE</v>
       </c>
       <c r="E26">
-        <v>12320</v>
+        <v>12000</v>
       </c>
       <c r="F26" t="str">
         <v>T</v>
       </c>
       <c r="H26">
-        <v>45237.0421827199</v>
+        <v>45234.04213364583</v>
       </c>
       <c r="J26" t="str">
-        <v>10/16/23 17:53</v>
+        <v>10/24/23 13:58</v>
       </c>
       <c r="K26" t="str">
-        <v>10/16/23 17:53</v>
+        <v>10/24/23 13:58</v>
       </c>
       <c r="L26">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="M26" t="str">
-        <v>$12,640 as of 10/16/2023 10:57:51 AM</v>
+        <v>$12,040 as of 10/24/2023 10:03:30 AM</v>
       </c>
       <c r="N26">
-        <v>12520</v>
+        <v>11720</v>
       </c>
       <c r="O26">
         <v>0</v>
@@ -1380,34 +1386,34 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>LK891176</v>
+        <v>LK923383</v>
       </c>
       <c r="C27" t="str">
-        <v>98 DISCOUNT STORE</v>
+        <v>SAMYS PHONE CARDS</v>
       </c>
       <c r="E27">
-        <v>21040</v>
+        <v>17020</v>
       </c>
       <c r="F27" t="str">
         <v>T</v>
       </c>
       <c r="H27">
-        <v>45232.0421827199</v>
+        <v>45247.04213364583</v>
       </c>
       <c r="J27" t="str">
-        <v>10/16/23 19:04</v>
+        <v>10/24/23 14:43</v>
       </c>
       <c r="K27" t="str">
-        <v>10/16/23 18:59</v>
+        <v>10/24/23 14:43</v>
       </c>
       <c r="L27">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="M27" t="str">
-        <v>$21,080 as of 10/16/2023 9:46:55 AM</v>
+        <v>$17,120 as of 10/24/2023 10:08:28 AM</v>
       </c>
       <c r="N27">
-        <v>21040</v>
+        <v>16920</v>
       </c>
       <c r="O27">
         <v>0</v>
@@ -1424,7 +1430,7 @@
         <v>Total Outstanding Cash Balance:</v>
       </c>
       <c r="E28">
-        <v>145500</v>
+        <v>130420</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
redoing styling and adding a sidebar
</commit_message>
<xml_diff>
--- a/rptTerminalStatusCassetteBalances.xlsx
+++ b/rptTerminalStatusCassetteBalances.xlsx
@@ -484,28 +484,28 @@
         <v>SCL ENTERPRISES LAUNDRY</v>
       </c>
       <c r="E5">
-        <v>1720</v>
+        <v>1300</v>
       </c>
       <c r="F5" t="str">
         <v>T</v>
       </c>
       <c r="H5">
-        <v>45244.04213364583</v>
+        <v>45251.04190482639</v>
       </c>
       <c r="J5" t="str">
-        <v>10/23/23 21:05</v>
+        <v>10/28/23 17:20</v>
       </c>
       <c r="K5" t="str">
-        <v>10/23/23 21:05</v>
+        <v>10/28/23 17:20</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5" t="str">
-        <v>$1,720 as of 10/23/2023 7:05:45 PM</v>
+        <v>$1,300 as of 10/28/2023 3:20:32 PM</v>
       </c>
       <c r="N5">
-        <v>1660</v>
+        <v>1500</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -519,34 +519,34 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>L647934</v>
+        <v>L662336</v>
       </c>
       <c r="C6" t="str">
-        <v>SB #6</v>
+        <v>SB#4 MONA MARKET</v>
       </c>
       <c r="E6">
-        <v>1940</v>
+        <v>1440</v>
       </c>
       <c r="F6" t="str">
         <v>T</v>
       </c>
-      <c r="I6" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+      <c r="H6">
+        <v>45234.04190482639</v>
       </c>
       <c r="J6" t="str">
-        <v>04/06/23 22:10</v>
+        <v>10/29/23 14:38</v>
       </c>
       <c r="K6" t="str">
-        <v>04/06/23 22:05</v>
+        <v>10/29/23 14:38</v>
       </c>
       <c r="L6">
-        <v>20</v>
+        <v>120</v>
       </c>
       <c r="M6" t="str">
-        <v>$1,940 as of 4/6/2023 8:05:45 PM</v>
+        <v>$1,480 as of 10/29/2023 9:25:15 AM</v>
       </c>
       <c r="N6">
-        <v>1960</v>
+        <v>1480</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -560,13 +560,13 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>L678988</v>
+        <v>L647934</v>
       </c>
       <c r="C7" t="str">
-        <v>PAYELESS MARKET</v>
+        <v>SB #6</v>
       </c>
       <c r="E7">
-        <v>2400</v>
+        <v>1940</v>
       </c>
       <c r="F7" t="str">
         <v>T</v>
@@ -575,19 +575,19 @@
         <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J7" t="str">
-        <v>07/20/23 20:09</v>
+        <v>04/06/23 22:10</v>
       </c>
       <c r="K7" t="str">
-        <v>07/20/23 20:09</v>
+        <v>04/06/23 22:05</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M7" t="str">
-        <v>$2,400 as of 7/20/2023 6:09:40 PM</v>
+        <v>$1,940 as of 4/6/2023 8:05:45 PM</v>
       </c>
       <c r="N7">
-        <v>2500</v>
+        <v>1960</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -601,34 +601,34 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>LK561655</v>
+        <v>L474792</v>
       </c>
       <c r="C8" t="str">
-        <v>CRENSHAW CRAVOR #2</v>
+        <v>NICK SHELL SERVICE</v>
       </c>
       <c r="E8">
-        <v>2780</v>
+        <v>2140</v>
       </c>
       <c r="F8" t="str">
         <v>T</v>
       </c>
-      <c r="I8" t="str">
-        <v>ATM Inactive greater than 48 minutes</v>
+      <c r="H8">
+        <v>45243.04190482639</v>
       </c>
       <c r="J8" t="str">
-        <v>01/23/20 08:24</v>
+        <v>10/29/23 09:18</v>
       </c>
       <c r="K8" t="str">
-        <v>01/23/20 08:24</v>
+        <v>10/29/23 09:18</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8" t="str">
-        <v>$2,780 as of 1/23/2020 6:24:32 AM</v>
+        <v>$2,140 as of 10/29/2023 7:18:35 AM</v>
       </c>
       <c r="N8">
-        <v>2800</v>
+        <v>2160</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -642,34 +642,34 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>L474792</v>
+        <v>L476340</v>
       </c>
       <c r="C9" t="str">
-        <v>NICK SHELL SERVICE</v>
+        <v>DONUT &amp; SANDWICH</v>
       </c>
       <c r="E9">
-        <v>2860</v>
+        <v>2360</v>
       </c>
       <c r="F9" t="str">
         <v>T</v>
       </c>
       <c r="H9">
-        <v>45243.04213364583</v>
+        <v>45236.04190482639</v>
       </c>
       <c r="J9" t="str">
-        <v>10/23/23 13:19</v>
+        <v>10/29/23 12:47</v>
       </c>
       <c r="K9" t="str">
-        <v>10/23/23 13:19</v>
+        <v>10/29/23 12:47</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9" t="str">
-        <v>$2,860 as of 10/23/2023 11:19:13 AM</v>
+        <v>$2,360 as of 10/29/2023 10:47:34 AM</v>
       </c>
       <c r="N9">
-        <v>2860</v>
+        <v>2460</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -683,34 +683,34 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>L662336</v>
+        <v>L678988</v>
       </c>
       <c r="C10" t="str">
-        <v>SB#4 MONA MARKET</v>
+        <v>PAYELESS MARKET</v>
       </c>
       <c r="E10">
-        <v>3120</v>
+        <v>2400</v>
       </c>
       <c r="F10" t="str">
         <v>T</v>
       </c>
-      <c r="H10">
-        <v>45239.04213364583</v>
+      <c r="I10" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J10" t="str">
-        <v>10/23/23 16:57</v>
+        <v>07/20/23 20:09</v>
       </c>
       <c r="K10" t="str">
-        <v>10/23/23 16:57</v>
+        <v>07/20/23 20:09</v>
       </c>
       <c r="L10">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="M10" t="str">
-        <v>$3,120 as of 10/23/2023 2:57:12 PM</v>
+        <v>$2,400 as of 7/20/2023 6:09:40 PM</v>
       </c>
       <c r="N10">
-        <v>3120</v>
+        <v>2500</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -724,37 +724,34 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>L488595</v>
+        <v>LK561655</v>
       </c>
       <c r="C11" t="str">
-        <v>N S MART</v>
+        <v>CRENSHAW CRAVOR #2</v>
       </c>
       <c r="E11">
-        <v>3460</v>
+        <v>2780</v>
       </c>
       <c r="F11" t="str">
         <v>T</v>
       </c>
-      <c r="H11">
-        <v>45263.04213364583</v>
-      </c>
       <c r="I11" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+        <v>ATM Inactive greater than 48 minutes</v>
       </c>
       <c r="J11" t="str">
-        <v>10/22/23 16:35</v>
+        <v>01/23/20 08:24</v>
       </c>
       <c r="K11" t="str">
-        <v>10/22/23 16:35</v>
+        <v>01/23/20 08:24</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11" t="str">
-        <v>$3,460 as of 10/22/2023 2:35:21 PM</v>
+        <v>$2,780 as of 1/23/2020 6:24:32 AM</v>
       </c>
       <c r="N11">
-        <v>3440</v>
+        <v>2800</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -768,34 +765,34 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>L475182</v>
+        <v>L488595</v>
       </c>
       <c r="C12" t="str">
-        <v>LA ESQUINA DE ORO</v>
+        <v>N S MART</v>
       </c>
       <c r="E12">
-        <v>3800</v>
+        <v>3140</v>
       </c>
       <c r="F12" t="str">
         <v>T</v>
       </c>
-      <c r="I12" t="str">
-        <v>ATM Inactive greater than 48 minutes</v>
+      <c r="H12">
+        <v>45307.04190482639</v>
       </c>
       <c r="J12" t="str">
-        <v>09/16/20 16:57</v>
+        <v>10/28/23 21:40</v>
       </c>
       <c r="K12" t="str">
-        <v>09/15/20 23:38</v>
+        <v>10/28/23 21:40</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12" t="str">
-        <v>$3,800 as of 9/16/2020 1:28:00 PM</v>
+        <v>$3,140 as of 10/28/2023 7:40:28 PM</v>
       </c>
       <c r="N12">
-        <v>3800</v>
+        <v>3220</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -809,37 +806,34 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>L688961</v>
+        <v>LK236828</v>
       </c>
       <c r="C13" t="str">
-        <v>MONA MART</v>
+        <v>WORLDWIDE AUTOMOTIVE</v>
       </c>
       <c r="E13">
-        <v>4000</v>
+        <v>3560</v>
       </c>
       <c r="F13" t="str">
         <v>T</v>
       </c>
       <c r="H13">
-        <v>45456.04213364583</v>
-      </c>
-      <c r="I13" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+        <v>45257.04190482639</v>
       </c>
       <c r="J13" t="str">
-        <v>10/17/23 13:26</v>
+        <v>10/29/23 16:35</v>
       </c>
       <c r="K13" t="str">
-        <v>10/17/23 13:00</v>
+        <v>10/29/23 16:35</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M13" t="str">
-        <v>$4,000 as of 10/17/2023 11:00:09 AM</v>
+        <v>$3,620 as of 10/28/2023 10:37:24 AM</v>
       </c>
       <c r="N13">
-        <v>4000</v>
+        <v>3620</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -853,34 +847,34 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>L476340</v>
+        <v>L697590</v>
       </c>
       <c r="C14" t="str">
-        <v>DONUT &amp; SANDWICH</v>
+        <v>S B MARKET ST</v>
       </c>
       <c r="E14">
-        <v>4040</v>
+        <v>3720</v>
       </c>
       <c r="F14" t="str">
         <v>T</v>
       </c>
       <c r="H14">
-        <v>45242.04213364583</v>
+        <v>45265.04190482639</v>
       </c>
       <c r="J14" t="str">
-        <v>10/24/23 14:06</v>
+        <v>10/29/23 14:07</v>
       </c>
       <c r="K14" t="str">
-        <v>10/24/23 14:06</v>
+        <v>10/29/23 14:07</v>
       </c>
       <c r="L14">
         <v>0</v>
       </c>
       <c r="M14" t="str">
-        <v>$4,060 as of 10/24/2023 10:00:58 AM</v>
+        <v>$3,740 as of 10/28/2023 2:56:53 PM</v>
       </c>
       <c r="N14">
-        <v>3880</v>
+        <v>3740</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -894,34 +888,34 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>L697590</v>
+        <v>L475182</v>
       </c>
       <c r="C15" t="str">
-        <v>S B MARKET ST</v>
+        <v>LA ESQUINA DE ORO</v>
       </c>
       <c r="E15">
-        <v>4140</v>
+        <v>3800</v>
       </c>
       <c r="F15" t="str">
         <v>T</v>
       </c>
-      <c r="H15">
-        <v>45249.04213364583</v>
+      <c r="I15" t="str">
+        <v>ATM Inactive greater than 48 minutes</v>
       </c>
       <c r="J15" t="str">
-        <v>10/24/23 12:12</v>
+        <v>09/16/20 16:57</v>
       </c>
       <c r="K15" t="str">
-        <v>10/24/23 12:12</v>
+        <v>09/15/20 23:38</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15" t="str">
-        <v>$4,140 as of 10/24/2023 10:12:25 AM</v>
+        <v>$3,800 as of 9/16/2020 1:28:00 PM</v>
       </c>
       <c r="N15">
-        <v>4120</v>
+        <v>3800</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -935,34 +929,34 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>L474817</v>
+        <v>L688966</v>
       </c>
       <c r="C16" t="str">
-        <v>SAFETY MARKET</v>
+        <v>S B WESTERN 108TH MARKET</v>
       </c>
       <c r="E16">
-        <v>4220</v>
+        <v>3980</v>
       </c>
       <c r="F16" t="str">
         <v>T</v>
       </c>
       <c r="H16">
-        <v>45237.04213364583</v>
+        <v>45272.04190482639</v>
       </c>
       <c r="J16" t="str">
-        <v>10/24/23 14:20</v>
+        <v>10/29/23 15:09</v>
       </c>
       <c r="K16" t="str">
-        <v>10/24/23 14:20</v>
+        <v>10/29/23 15:09</v>
       </c>
       <c r="L16">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="M16" t="str">
-        <v>$4,240 as of 10/24/2023 10:34:37 AM</v>
+        <v>$4,100 as of 10/29/2023 11:15:25 AM</v>
       </c>
       <c r="N16">
-        <v>3960</v>
+        <v>4080</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -976,34 +970,34 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>LK236828</v>
+        <v>L688961</v>
       </c>
       <c r="C17" t="str">
-        <v>WORLDWIDE AUTOMOTIVE</v>
+        <v>MONA MART</v>
       </c>
       <c r="E17">
-        <v>4300</v>
+        <v>4000</v>
       </c>
       <c r="F17" t="str">
         <v>T</v>
       </c>
-      <c r="H17">
-        <v>45240.04213364583</v>
+      <c r="I17" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J17" t="str">
-        <v>10/23/23 10:42</v>
+        <v>10/17/23 13:26</v>
       </c>
       <c r="K17" t="str">
-        <v>10/23/23 10:42</v>
+        <v>10/17/23 13:00</v>
       </c>
       <c r="L17">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M17" t="str">
-        <v>$4,300 as of 10/23/2023 8:42:11 AM</v>
+        <v>$4,000 as of 10/17/2023 11:00:09 AM</v>
       </c>
       <c r="N17">
-        <v>4300</v>
+        <v>4000</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1017,34 +1011,34 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>L688966</v>
+        <v>L475090</v>
       </c>
       <c r="C18" t="str">
-        <v>S B WESTERN 108TH MARKET</v>
+        <v>S.B. 2</v>
       </c>
       <c r="E18">
-        <v>4680</v>
+        <v>5000</v>
       </c>
       <c r="F18" t="str">
         <v>T</v>
       </c>
       <c r="H18">
-        <v>45240.04213364583</v>
+        <v>45238.04190482639</v>
       </c>
       <c r="J18" t="str">
-        <v>10/24/23 12:38</v>
+        <v>10/29/23 18:00</v>
       </c>
       <c r="K18" t="str">
-        <v>10/24/23 12:38</v>
+        <v>10/29/23 18:00</v>
       </c>
       <c r="L18">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="M18" t="str">
-        <v>$4,680 as of 10/24/2023 10:38:11 AM</v>
+        <v>$5,080 as of 10/28/2023 4:33:08 PM</v>
       </c>
       <c r="N18">
-        <v>4620</v>
+        <v>5020</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -1058,34 +1052,34 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>L697589</v>
+        <v>L474746</v>
       </c>
       <c r="C19" t="str">
-        <v>S B DISCOUNT MART</v>
+        <v>ZACATES MARKET</v>
       </c>
       <c r="E19">
-        <v>5840</v>
+        <v>5440</v>
       </c>
       <c r="F19" t="str">
         <v>T</v>
       </c>
       <c r="H19">
-        <v>45232.04213364583</v>
+        <v>45255.04190482639</v>
       </c>
       <c r="J19" t="str">
-        <v>10/24/23 14:19</v>
+        <v>10/29/23 17:21</v>
       </c>
       <c r="K19" t="str">
-        <v>10/24/23 14:19</v>
+        <v>10/29/23 17:21</v>
       </c>
       <c r="L19">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="M19" t="str">
-        <v>$5,900 as of 10/24/2023 10:56:38 AM</v>
+        <v>$5,620 as of 10/29/2023 11:14:47 AM</v>
       </c>
       <c r="N19">
-        <v>5800</v>
+        <v>5620</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1099,34 +1093,34 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>L475090</v>
+        <v>LK864765</v>
       </c>
       <c r="C20" t="str">
-        <v>S.B. 2</v>
+        <v>SKY LIQUOR</v>
       </c>
       <c r="E20">
-        <v>6820</v>
+        <v>5520</v>
       </c>
       <c r="F20" t="str">
         <v>T</v>
       </c>
       <c r="H20">
-        <v>45254.04213364583</v>
+        <v>45236.04190482639</v>
       </c>
       <c r="J20" t="str">
-        <v>10/24/23 10:37</v>
+        <v>10/29/23 12:55</v>
       </c>
       <c r="K20" t="str">
-        <v>10/24/23 10:37</v>
+        <v>10/29/23 02:29</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="M20" t="str">
-        <v>$6,820 as of 10/24/2023 8:37:49 AM</v>
+        <v>$5,600 as of 10/29/2023 10:00:03 AM</v>
       </c>
       <c r="N20">
-        <v>6740</v>
+        <v>5600</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -1140,34 +1134,34 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>L474746</v>
+        <v>L704741</v>
       </c>
       <c r="C21" t="str">
-        <v>ZACATES MARKET</v>
+        <v>W ADAMS COIN LAUNDRY</v>
       </c>
       <c r="E21">
-        <v>6860</v>
+        <v>5800</v>
       </c>
       <c r="F21" t="str">
         <v>T</v>
       </c>
       <c r="H21">
-        <v>45271.04213364583</v>
+        <v>45237.04190482639</v>
       </c>
       <c r="J21" t="str">
-        <v>10/24/23 15:21</v>
+        <v>10/29/23 17:36</v>
       </c>
       <c r="K21" t="str">
-        <v>10/24/23 15:18</v>
+        <v>10/29/23 17:36</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="M21" t="str">
-        <v>$6,900 as of 10/24/2023 10:32:02 AM</v>
+        <v>$5,860 as of 10/29/2023 9:54:54 AM</v>
       </c>
       <c r="N21">
-        <v>6840</v>
+        <v>5840</v>
       </c>
       <c r="O21">
         <v>0</v>
@@ -1181,34 +1175,34 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>L682801</v>
+        <v>L474817</v>
       </c>
       <c r="C22" t="str">
-        <v>SB#5</v>
+        <v>SAFETY MARKET</v>
       </c>
       <c r="E22">
-        <v>7840</v>
+        <v>6700</v>
       </c>
       <c r="F22" t="str">
         <v>T</v>
       </c>
-      <c r="I22" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+      <c r="H22">
+        <v>45244.04190482639</v>
       </c>
       <c r="J22" t="str">
-        <v>09/28/23 15:22</v>
+        <v>10/29/23 18:10</v>
       </c>
       <c r="K22" t="str">
-        <v>09/28/23 12:14</v>
+        <v>10/29/23 18:10</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="M22" t="str">
-        <v>$7,840 as of 9/28/2023 12:31:50 PM</v>
+        <v>$7,280 as of 10/29/2023 8:50:55 AM</v>
       </c>
       <c r="N22">
-        <v>7840</v>
+        <v>6800</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -1228,28 +1222,28 @@
         <v>BABS MARKET</v>
       </c>
       <c r="E23">
-        <v>7960</v>
+        <v>6860</v>
       </c>
       <c r="F23" t="str">
         <v>T</v>
       </c>
       <c r="H23">
-        <v>45267.04213364583</v>
+        <v>45268.04190482639</v>
       </c>
       <c r="J23" t="str">
-        <v>10/23/23 20:57</v>
+        <v>10/29/23 12:02</v>
       </c>
       <c r="K23" t="str">
-        <v>10/23/23 20:57</v>
+        <v>10/29/23 12:02</v>
       </c>
       <c r="L23">
         <v>100</v>
       </c>
       <c r="M23" t="str">
-        <v>$7,960 as of 10/23/2023 6:57:34 PM</v>
+        <v>$6,860 as of 10/29/2023 10:02:36 AM</v>
       </c>
       <c r="N23">
-        <v>7900</v>
+        <v>6920</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -1263,34 +1257,34 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>LK864765</v>
+        <v>LK891176</v>
       </c>
       <c r="C24" t="str">
-        <v>SKY LIQUOR</v>
+        <v>98 DISCOUNT STORE</v>
       </c>
       <c r="E24">
-        <v>8740</v>
+        <v>6920</v>
       </c>
       <c r="F24" t="str">
         <v>T</v>
       </c>
       <c r="H24">
-        <v>45237.04213364583</v>
+        <v>45236.04190482639</v>
       </c>
       <c r="J24" t="str">
-        <v>10/24/23 12:53</v>
+        <v>10/29/23 17:28</v>
       </c>
       <c r="K24" t="str">
-        <v>10/24/23 12:04</v>
+        <v>10/29/23 17:28</v>
       </c>
       <c r="L24">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="M24" t="str">
-        <v>$8,800 as of 10/24/2023 10:04:24 AM</v>
+        <v>$7,280 as of 10/29/2023 10:20:08 AM</v>
       </c>
       <c r="N24">
-        <v>8780</v>
+        <v>6960</v>
       </c>
       <c r="O24">
         <v>0</v>
@@ -1304,34 +1298,34 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>L704741</v>
+        <v>L682801</v>
       </c>
       <c r="C25" t="str">
-        <v>W ADAMS COIN LAUNDRY</v>
+        <v>SB#5</v>
       </c>
       <c r="E25">
-        <v>9880</v>
+        <v>7840</v>
       </c>
       <c r="F25" t="str">
         <v>T</v>
       </c>
-      <c r="H25">
-        <v>45236.04213364583</v>
+      <c r="I25" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J25" t="str">
-        <v>10/24/23 15:12</v>
+        <v>09/28/23 15:22</v>
       </c>
       <c r="K25" t="str">
-        <v>10/24/23 15:12</v>
+        <v>09/28/23 12:14</v>
       </c>
       <c r="L25">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M25" t="str">
-        <v>$9,960 as of 10/24/2023 11:13:30 AM</v>
+        <v>$7,840 as of 9/28/2023 12:31:50 PM</v>
       </c>
       <c r="N25">
-        <v>9660</v>
+        <v>7840</v>
       </c>
       <c r="O25">
         <v>0</v>
@@ -1345,34 +1339,34 @@
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>LK891176</v>
+        <v>L697589</v>
       </c>
       <c r="C26" t="str">
-        <v>98 DISCOUNT STORE</v>
+        <v>S B DISCOUNT MART</v>
       </c>
       <c r="E26">
-        <v>12000</v>
+        <v>13240</v>
       </c>
       <c r="F26" t="str">
         <v>T</v>
       </c>
       <c r="H26">
-        <v>45234.04213364583</v>
+        <v>45242.04190482639</v>
       </c>
       <c r="J26" t="str">
-        <v>10/24/23 13:58</v>
+        <v>10/29/23 18:14</v>
       </c>
       <c r="K26" t="str">
-        <v>10/24/23 13:58</v>
+        <v>10/29/23 17:49</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="M26" t="str">
-        <v>$12,040 as of 10/24/2023 10:03:30 AM</v>
+        <v>$13,380 as of 10/29/2023 10:17:18 AM</v>
       </c>
       <c r="N26">
-        <v>11720</v>
+        <v>13240</v>
       </c>
       <c r="O26">
         <v>0</v>
@@ -1392,28 +1386,28 @@
         <v>SAMYS PHONE CARDS</v>
       </c>
       <c r="E27">
-        <v>17020</v>
+        <v>14760</v>
       </c>
       <c r="F27" t="str">
         <v>T</v>
       </c>
       <c r="H27">
-        <v>45247.04213364583</v>
+        <v>45255.04190482639</v>
       </c>
       <c r="J27" t="str">
-        <v>10/24/23 14:43</v>
+        <v>10/29/23 15:29</v>
       </c>
       <c r="K27" t="str">
-        <v>10/24/23 14:43</v>
+        <v>10/29/23 15:29</v>
       </c>
       <c r="L27">
         <v>80</v>
       </c>
       <c r="M27" t="str">
-        <v>$17,120 as of 10/24/2023 10:08:28 AM</v>
+        <v>$14,780 as of 10/29/2023 10:00:13 AM</v>
       </c>
       <c r="N27">
-        <v>16920</v>
+        <v>14780</v>
       </c>
       <c r="O27">
         <v>0</v>
@@ -1430,7 +1424,7 @@
         <v>Total Outstanding Cash Balance:</v>
       </c>
       <c r="E28">
-        <v>130420</v>
+        <v>114640</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add back blur and sign out button
</commit_message>
<xml_diff>
--- a/rptTerminalStatusCassetteBalances.xlsx
+++ b/rptTerminalStatusCassetteBalances.xlsx
@@ -525,7 +525,7 @@
         <v>SCL ENTERPRISES LAUNDRY</v>
       </c>
       <c r="E6">
-        <v>2240</v>
+        <v>2200</v>
       </c>
       <c r="F6" t="str">
         <v>T</v>
@@ -534,19 +534,19 @@
         <v>45254.0418602662</v>
       </c>
       <c r="J6" t="str">
-        <v>11/07/23 20:44</v>
+        <v>11/08/23 09:37</v>
       </c>
       <c r="K6" t="str">
-        <v>11/07/23 20:44</v>
+        <v>11/08/23 09:37</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6" t="str">
-        <v>$2,280 as of 11/6/2023 7:45:51 PM</v>
+        <v>$2,200 as of 11/8/2023 7:37:51 AM</v>
       </c>
       <c r="N6">
-        <v>2280</v>
+        <v>2240</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -651,7 +651,7 @@
         <v>NICK SHELL SERVICE</v>
       </c>
       <c r="E9">
-        <v>2600</v>
+        <v>2540</v>
       </c>
       <c r="F9" t="str">
         <v>T</v>
@@ -660,19 +660,19 @@
         <v>45251.0418602662</v>
       </c>
       <c r="J9" t="str">
-        <v>11/07/23 11:20</v>
+        <v>11/08/23 12:46</v>
       </c>
       <c r="K9" t="str">
-        <v>11/07/23 11:20</v>
+        <v>11/08/23 12:46</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9" t="str">
-        <v>$2,600 as of 11/7/2023 9:20:27 AM</v>
+        <v>$2,540 as of 11/8/2023 10:46:48 AM</v>
       </c>
       <c r="N9">
-        <v>2720</v>
+        <v>2600</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -686,34 +686,34 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>LK561655</v>
+        <v>L662336</v>
       </c>
       <c r="C10" t="str">
-        <v>CRENSHAW CRAVOR #2</v>
+        <v>SB#4 MONA MARKET</v>
       </c>
       <c r="E10">
-        <v>2780</v>
+        <v>2560</v>
       </c>
       <c r="F10" t="str">
         <v>T</v>
       </c>
-      <c r="I10" t="str">
-        <v>ATM Inactive greater than 48 minutes</v>
+      <c r="H10">
+        <v>45250.0418602662</v>
       </c>
       <c r="J10" t="str">
-        <v>01/23/20 08:24</v>
+        <v>11/08/23 17:02</v>
       </c>
       <c r="K10" t="str">
-        <v>01/23/20 08:24</v>
+        <v>11/08/23 17:02</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="M10" t="str">
-        <v>$2,780 as of 1/23/2020 6:24:32 AM</v>
+        <v>$3,180 as of 11/8/2023 7:54:25 AM</v>
       </c>
       <c r="N10">
-        <v>2800</v>
+        <v>2640</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -727,34 +727,34 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>L474746</v>
+        <v>LK561655</v>
       </c>
       <c r="C11" t="str">
-        <v>ZACATES MARKET</v>
+        <v>CRENSHAW CRAVOR #2</v>
       </c>
       <c r="E11">
-        <v>3000</v>
+        <v>2780</v>
       </c>
       <c r="F11" t="str">
         <v>T</v>
       </c>
-      <c r="H11">
-        <v>45247.0418602662</v>
+      <c r="I11" t="str">
+        <v>ATM Inactive greater than 48 minutes</v>
       </c>
       <c r="J11" t="str">
-        <v>11/07/23 17:33</v>
+        <v>01/23/20 08:24</v>
       </c>
       <c r="K11" t="str">
-        <v>11/07/23 17:33</v>
+        <v>01/23/20 08:24</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11" t="str">
-        <v>$3,100 as of 11/7/2023 9:32:35 AM</v>
+        <v>$2,780 as of 1/23/2020 6:24:32 AM</v>
       </c>
       <c r="N11">
-        <v>3020</v>
+        <v>2800</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -768,34 +768,34 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>L662336</v>
+        <v>L475090</v>
       </c>
       <c r="C12" t="str">
-        <v>SB#4 MONA MARKET</v>
+        <v>S.B. 2</v>
       </c>
       <c r="E12">
-        <v>3220</v>
+        <v>2840</v>
       </c>
       <c r="F12" t="str">
         <v>T</v>
       </c>
       <c r="H12">
-        <v>45250.0418602662</v>
+        <v>45241.0418602662</v>
       </c>
       <c r="J12" t="str">
-        <v>11/07/23 18:55</v>
+        <v>11/08/23 19:47</v>
       </c>
       <c r="K12" t="str">
-        <v>11/07/23 17:45</v>
+        <v>11/08/23 19:03</v>
       </c>
       <c r="L12">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="M12" t="str">
-        <v>$3,320 as of 11/7/2023 11:09:06 AM</v>
+        <v>$3,220 as of 11/8/2023 9:27:02 AM</v>
       </c>
       <c r="N12">
-        <v>3220</v>
+        <v>2840</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -809,34 +809,34 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>L475090</v>
+        <v>L474746</v>
       </c>
       <c r="C13" t="str">
-        <v>S.B. 2</v>
+        <v>ZACATES MARKET</v>
       </c>
       <c r="E13">
-        <v>3520</v>
+        <v>2960</v>
       </c>
       <c r="F13" t="str">
         <v>T</v>
       </c>
       <c r="H13">
-        <v>45241.0418602662</v>
+        <v>45247.0418602662</v>
       </c>
       <c r="J13" t="str">
-        <v>11/07/23 20:55</v>
+        <v>11/08/23 13:39</v>
       </c>
       <c r="K13" t="str">
-        <v>11/07/23 20:55</v>
+        <v>11/08/23 13:36</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13" t="str">
-        <v>$4,160 as of 11/7/2023 11:46:19 AM</v>
+        <v>$2,960 as of 11/8/2023 11:36:06 AM</v>
       </c>
       <c r="N13">
-        <v>3720</v>
+        <v>2960</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -850,34 +850,34 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>L475182</v>
+        <v>LK864765</v>
       </c>
       <c r="C14" t="str">
-        <v>LA ESQUINA DE ORO</v>
+        <v>SKY LIQUOR</v>
       </c>
       <c r="E14">
-        <v>3800</v>
+        <v>3400</v>
       </c>
       <c r="F14" t="str">
         <v>T</v>
       </c>
-      <c r="I14" t="str">
-        <v>ATM Inactive greater than 48 minutes</v>
+      <c r="H14">
+        <v>45243.0418602662</v>
       </c>
       <c r="J14" t="str">
-        <v>09/16/20 16:57</v>
+        <v>11/08/23 17:12</v>
       </c>
       <c r="K14" t="str">
-        <v>09/15/20 23:38</v>
+        <v>11/08/23 17:12</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="M14" t="str">
-        <v>$3,800 as of 9/16/2020 1:28:00 PM</v>
+        <v>$3,840 as of 11/8/2023 11:37:39 AM</v>
       </c>
       <c r="N14">
-        <v>3800</v>
+        <v>3500</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -891,34 +891,34 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>L688961</v>
+        <v>L475182</v>
       </c>
       <c r="C15" t="str">
-        <v>MONA MART</v>
+        <v>LA ESQUINA DE ORO</v>
       </c>
       <c r="E15">
-        <v>4000</v>
+        <v>3800</v>
       </c>
       <c r="F15" t="str">
         <v>T</v>
       </c>
       <c r="I15" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+        <v>ATM Inactive greater than 48 minutes</v>
       </c>
       <c r="J15" t="str">
-        <v>10/17/23 13:26</v>
+        <v>09/16/20 16:57</v>
       </c>
       <c r="K15" t="str">
-        <v>10/17/23 13:00</v>
+        <v>09/15/20 23:38</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15" t="str">
-        <v>$4,000 as of 10/17/2023 11:00:09 AM</v>
+        <v>$3,800 as of 9/16/2020 1:28:00 PM</v>
       </c>
       <c r="N15">
-        <v>4000</v>
+        <v>3800</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -938,7 +938,7 @@
         <v>S B MARKET ST</v>
       </c>
       <c r="E16">
-        <v>4040</v>
+        <v>3820</v>
       </c>
       <c r="F16" t="str">
         <v>T</v>
@@ -947,19 +947,19 @@
         <v>45260.0418602662</v>
       </c>
       <c r="J16" t="str">
-        <v>11/07/23 19:56</v>
+        <v>11/08/23 19:38</v>
       </c>
       <c r="K16" t="str">
-        <v>11/07/23 19:56</v>
+        <v>11/08/23 17:11</v>
       </c>
       <c r="L16">
         <v>0</v>
       </c>
       <c r="M16" t="str">
-        <v>$4,120 as of 11/7/2023 9:21:49 AM</v>
+        <v>$4,020 as of 11/8/2023 10:06:15 AM</v>
       </c>
       <c r="N16">
-        <v>4060</v>
+        <v>4020</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -973,34 +973,34 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>LK864765</v>
+        <v>L688966</v>
       </c>
       <c r="C17" t="str">
-        <v>SKY LIQUOR</v>
+        <v>S B WESTERN 108TH MARKET</v>
       </c>
       <c r="E17">
-        <v>4520</v>
+        <v>3880</v>
       </c>
       <c r="F17" t="str">
         <v>T</v>
       </c>
       <c r="H17">
-        <v>45243.0418602662</v>
+        <v>45245.0418602662</v>
       </c>
       <c r="J17" t="str">
-        <v>11/08/23 00:44</v>
+        <v>11/08/23 19:10</v>
       </c>
       <c r="K17" t="str">
-        <v>11/08/23 00:44</v>
+        <v>11/08/23 19:10</v>
       </c>
       <c r="L17">
         <v>80</v>
       </c>
       <c r="M17" t="str">
-        <v>$4,740 as of 11/7/2023 11:15:41 AM</v>
+        <v>$4,360 as of 11/8/2023 10:31:03 AM</v>
       </c>
       <c r="N17">
-        <v>4560</v>
+        <v>3840</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1014,34 +1014,34 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>L688966</v>
+        <v>L688961</v>
       </c>
       <c r="C18" t="str">
-        <v>S B WESTERN 108TH MARKET</v>
+        <v>MONA MART</v>
       </c>
       <c r="E18">
-        <v>4680</v>
+        <v>4000</v>
       </c>
       <c r="F18" t="str">
         <v>T</v>
       </c>
-      <c r="H18">
-        <v>45245.0418602662</v>
+      <c r="I18" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J18" t="str">
-        <v>11/08/23 00:01</v>
+        <v>10/17/23 13:26</v>
       </c>
       <c r="K18" t="str">
-        <v>11/08/23 00:01</v>
+        <v>10/17/23 13:00</v>
       </c>
       <c r="L18">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="M18" t="str">
-        <v>$4,780 as of 11/7/2023 10:50:09 AM</v>
+        <v>$4,000 as of 10/17/2023 11:00:09 AM</v>
       </c>
       <c r="N18">
-        <v>4700</v>
+        <v>4000</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -1061,7 +1061,7 @@
         <v>WORLDWIDE AUTOMOTIVE</v>
       </c>
       <c r="E19">
-        <v>5040</v>
+        <v>4740</v>
       </c>
       <c r="F19" t="str">
         <v>T</v>
@@ -1070,19 +1070,19 @@
         <v>45260.0418602662</v>
       </c>
       <c r="J19" t="str">
-        <v>11/07/23 19:02</v>
+        <v>11/08/23 17:48</v>
       </c>
       <c r="K19" t="str">
-        <v>11/07/23 19:02</v>
+        <v>11/08/23 17:48</v>
       </c>
       <c r="L19">
         <v>20</v>
       </c>
       <c r="M19" t="str">
-        <v>$5,120 as of 11/7/2023 9:56:30 AM</v>
+        <v>$4,840 as of 11/8/2023 10:15:56 AM</v>
       </c>
       <c r="N19">
-        <v>5100</v>
+        <v>4840</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1102,7 +1102,7 @@
         <v>BABS MARKET</v>
       </c>
       <c r="E20">
-        <v>5160</v>
+        <v>4960</v>
       </c>
       <c r="F20" t="str">
         <v>T</v>
@@ -1111,10 +1111,10 @@
         <v>45261.0418602662</v>
       </c>
       <c r="J20" t="str">
-        <v>11/07/23 13:51</v>
+        <v>11/08/23 17:33</v>
       </c>
       <c r="K20" t="str">
-        <v>11/07/23 13:51</v>
+        <v>11/08/23 17:33</v>
       </c>
       <c r="L20">
         <v>100</v>
@@ -1123,7 +1123,7 @@
         <v>$5,160 as of 11/7/2023 11:51:10 AM</v>
       </c>
       <c r="N20">
-        <v>5240</v>
+        <v>5120</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -1143,7 +1143,7 @@
         <v>SAFETY MARKET</v>
       </c>
       <c r="E21">
-        <v>6020</v>
+        <v>5660</v>
       </c>
       <c r="F21" t="str">
         <v>T</v>
@@ -1152,19 +1152,19 @@
         <v>45245.0418602662</v>
       </c>
       <c r="J21" t="str">
-        <v>11/07/23 21:43</v>
+        <v>11/08/23 18:26</v>
       </c>
       <c r="K21" t="str">
-        <v>11/07/23 21:43</v>
+        <v>11/08/23 18:26</v>
       </c>
       <c r="L21">
         <v>120</v>
       </c>
       <c r="M21" t="str">
-        <v>$6,620 as of 11/7/2023 7:59:42 AM</v>
+        <v>$5,820 as of 11/8/2023 10:55:36 AM</v>
       </c>
       <c r="N21">
-        <v>6040</v>
+        <v>5760</v>
       </c>
       <c r="O21">
         <v>0</v>
@@ -1178,34 +1178,34 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>L682801</v>
+        <v>L704741</v>
       </c>
       <c r="C22" t="str">
-        <v>SB#5</v>
+        <v>W ADAMS COIN LAUNDRY</v>
       </c>
       <c r="E22">
-        <v>7840</v>
+        <v>7780</v>
       </c>
       <c r="F22" t="str">
         <v>T</v>
       </c>
-      <c r="I22" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+      <c r="H22">
+        <v>45248.0418602662</v>
       </c>
       <c r="J22" t="str">
-        <v>09/28/23 15:22</v>
+        <v>11/08/23 17:29</v>
       </c>
       <c r="K22" t="str">
-        <v>09/28/23 12:14</v>
+        <v>11/08/23 17:29</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="M22" t="str">
-        <v>$7,840 as of 9/28/2023 12:31:50 PM</v>
+        <v>$8,040 as of 11/8/2023 11:37:41 AM</v>
       </c>
       <c r="N22">
-        <v>7840</v>
+        <v>7800</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -1225,7 +1225,7 @@
         <v>DONUT &amp; SANDWICH</v>
       </c>
       <c r="E23">
-        <v>7900</v>
+        <v>7840</v>
       </c>
       <c r="F23" t="str">
         <v>T</v>
@@ -1234,19 +1234,19 @@
         <v>45265.0418602662</v>
       </c>
       <c r="J23" t="str">
-        <v>11/07/23 10:39</v>
+        <v>11/08/23 11:55</v>
       </c>
       <c r="K23" t="str">
-        <v>11/06/23 18:53</v>
+        <v>11/08/23 11:55</v>
       </c>
       <c r="L23">
         <v>0</v>
       </c>
       <c r="M23" t="str">
-        <v>$7,900 as of 11/7/2023 8:39:34 AM</v>
+        <v>$7,840 as of 11/8/2023 9:55:43 AM</v>
       </c>
       <c r="N23">
-        <v>7900</v>
+        <v>7860</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -1260,34 +1260,34 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>L704741</v>
+        <v>L682801</v>
       </c>
       <c r="C24" t="str">
-        <v>W ADAMS COIN LAUNDRY</v>
+        <v>SB#5</v>
       </c>
       <c r="E24">
-        <v>8260</v>
+        <v>7840</v>
       </c>
       <c r="F24" t="str">
         <v>T</v>
       </c>
-      <c r="H24">
-        <v>45248.0418602662</v>
+      <c r="I24" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J24" t="str">
-        <v>11/08/23 01:44</v>
+        <v>09/28/23 15:22</v>
       </c>
       <c r="K24" t="str">
-        <v>11/08/23 01:44</v>
+        <v>09/28/23 12:14</v>
       </c>
       <c r="L24">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M24" t="str">
-        <v>$8,400 as of 11/7/2023 11:35:46 AM</v>
+        <v>$7,840 as of 9/28/2023 12:31:50 PM</v>
       </c>
       <c r="N24">
-        <v>8280</v>
+        <v>7840</v>
       </c>
       <c r="O24">
         <v>0</v>
@@ -1307,7 +1307,7 @@
         <v>SAMYS PHONE CARDS</v>
       </c>
       <c r="E25">
-        <v>10580</v>
+        <v>10460</v>
       </c>
       <c r="F25" t="str">
         <v>T</v>
@@ -1316,19 +1316,19 @@
         <v>45261.0418602662</v>
       </c>
       <c r="J25" t="str">
-        <v>11/07/23 20:56</v>
+        <v>11/08/23 17:39</v>
       </c>
       <c r="K25" t="str">
-        <v>11/07/23 20:56</v>
+        <v>11/08/23 17:39</v>
       </c>
       <c r="L25">
         <v>80</v>
       </c>
       <c r="M25" t="str">
-        <v>$10,920 as of 11/6/2023 7:47:12 PM</v>
+        <v>$10,520 as of 11/8/2023 11:38:10 AM</v>
       </c>
       <c r="N25">
-        <v>10600</v>
+        <v>10500</v>
       </c>
       <c r="O25">
         <v>0</v>
@@ -1348,7 +1348,7 @@
         <v>98 DISCOUNT STORE</v>
       </c>
       <c r="E26">
-        <v>11740</v>
+        <v>10920</v>
       </c>
       <c r="F26" t="str">
         <v>T</v>
@@ -1357,19 +1357,19 @@
         <v>45245.0418602662</v>
       </c>
       <c r="J26" t="str">
-        <v>11/08/23 01:34</v>
+        <v>11/08/23 19:37</v>
       </c>
       <c r="K26" t="str">
-        <v>11/08/23 01:34</v>
+        <v>11/08/23 19:14</v>
       </c>
       <c r="L26">
         <v>0</v>
       </c>
       <c r="M26" t="str">
-        <v>$12,980 as of 11/7/2023 11:00:55 AM</v>
+        <v>$11,360 as of 11/8/2023 11:41:50 AM</v>
       </c>
       <c r="N26">
-        <v>11920</v>
+        <v>10920</v>
       </c>
       <c r="O26">
         <v>0</v>
@@ -1389,7 +1389,7 @@
         <v>S B DISCOUNT MART</v>
       </c>
       <c r="E27">
-        <v>14720</v>
+        <v>13920</v>
       </c>
       <c r="F27" t="str">
         <v>T</v>
@@ -1398,19 +1398,19 @@
         <v>45246.0418602662</v>
       </c>
       <c r="J27" t="str">
-        <v>11/07/23 23:06</v>
+        <v>11/08/23 19:03</v>
       </c>
       <c r="K27" t="str">
-        <v>11/07/23 21:33</v>
+        <v>11/08/23 19:03</v>
       </c>
       <c r="L27">
         <v>60</v>
       </c>
       <c r="M27" t="str">
-        <v>$15,740 as of 11/7/2023 10:54:10 AM</v>
+        <v>$14,140 as of 11/8/2023 11:40:47 AM</v>
       </c>
       <c r="N27">
-        <v>14720</v>
+        <v>14120</v>
       </c>
       <c r="O27">
         <v>0</v>
@@ -1427,7 +1427,7 @@
         <v>Total Outstanding Cash Balance:</v>
       </c>
       <c r="E28">
-        <v>122300</v>
+        <v>115540</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More ui updates, mainly,  blur button rework
</commit_message>
<xml_diff>
--- a/rptTerminalStatusCassetteBalances.xlsx
+++ b/rptTerminalStatusCassetteBalances.xlsx
@@ -44,8 +44,8 @@
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
     <numFmt numFmtId="164" formatCode="[$-010409]#,###"/>
     <numFmt numFmtId="165" formatCode="[$-010409]&quot;$&quot;#,##0.00;(&quot;$&quot;#,##0.00)"/>
-    <numFmt numFmtId="166" formatCode="[$-010409]$#,##0"/>
-    <numFmt numFmtId="167" formatCode="[$-010409]m/d/yyyy"/>
+    <numFmt numFmtId="166" formatCode="[$-010409]m/d/yyyy"/>
+    <numFmt numFmtId="167" formatCode="[$-010409]$#,##0"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -478,34 +478,34 @@
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>L647934</v>
+        <v>LK644532</v>
       </c>
       <c r="C5" t="str">
-        <v>SB #6</v>
+        <v>SCL ENTERPRISES LAUNDRY</v>
       </c>
       <c r="E5">
-        <v>1940</v>
+        <v>460</v>
       </c>
       <c r="F5" t="str">
         <v>T</v>
       </c>
-      <c r="I5" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+      <c r="H5">
+        <v>45263.04188596064</v>
       </c>
       <c r="J5" t="str">
-        <v>04/06/23 22:10</v>
+        <v>11/27/23 17:36</v>
       </c>
       <c r="K5" t="str">
-        <v>04/06/23 22:05</v>
+        <v>11/27/23 17:36</v>
       </c>
       <c r="L5">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M5" t="str">
-        <v>$1,940 as of 4/6/2023 8:05:45 PM</v>
+        <v>$700 as of 11/27/2023 10:15:44 AM</v>
       </c>
       <c r="N5">
-        <v>1960</v>
+        <v>500</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -519,34 +519,37 @@
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>LK644532</v>
+        <v>L488595</v>
       </c>
       <c r="C6" t="str">
-        <v>SCL ENTERPRISES LAUNDRY</v>
+        <v>N S MART</v>
       </c>
       <c r="E6">
-        <v>2200</v>
+        <v>1700</v>
       </c>
       <c r="F6" t="str">
         <v>T</v>
       </c>
       <c r="H6">
-        <v>45254.0418602662</v>
+        <v>45324.04188596064</v>
+      </c>
+      <c r="I6" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J6" t="str">
-        <v>11/08/23 09:37</v>
+        <v>11/24/23 16:21</v>
       </c>
       <c r="K6" t="str">
-        <v>11/08/23 09:37</v>
+        <v>11/22/23 20:35</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6" t="str">
-        <v>$2,200 as of 11/8/2023 7:37:51 AM</v>
+        <v>$1,700 as of 11/24/2023 2:21:19 PM</v>
       </c>
       <c r="N6">
-        <v>2240</v>
+        <v>1700</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -560,37 +563,34 @@
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>L488595</v>
+        <v>L474817</v>
       </c>
       <c r="C7" t="str">
-        <v>N S MART</v>
+        <v>SAFETY MARKET</v>
       </c>
       <c r="E7">
-        <v>2300</v>
+        <v>1740</v>
       </c>
       <c r="F7" t="str">
         <v>T</v>
       </c>
       <c r="H7">
-        <v>45257.0418602662</v>
-      </c>
-      <c r="I7" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+        <v>45261.04188596064</v>
       </c>
       <c r="J7" t="str">
-        <v>11/06/23 16:31</v>
+        <v>11/27/23 23:21</v>
       </c>
       <c r="K7" t="str">
-        <v>11/05/23 18:07</v>
+        <v>11/27/23 22:35</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="M7" t="str">
-        <v>$2,300 as of 11/6/2023 2:31:34 PM</v>
+        <v>$2,060 as of 11/27/2023 9:29:55 AM</v>
       </c>
       <c r="N7">
-        <v>2300</v>
+        <v>1740</v>
       </c>
       <c r="O7">
         <v>0</v>
@@ -604,13 +604,13 @@
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>L678988</v>
+        <v>L647934</v>
       </c>
       <c r="C8" t="str">
-        <v>PAYELESS MARKET</v>
+        <v>SB #6</v>
       </c>
       <c r="E8">
-        <v>2400</v>
+        <v>1940</v>
       </c>
       <c r="F8" t="str">
         <v>T</v>
@@ -619,19 +619,19 @@
         <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J8" t="str">
-        <v>07/20/23 20:09</v>
+        <v>04/06/23 22:10</v>
       </c>
       <c r="K8" t="str">
-        <v>07/20/23 20:09</v>
+        <v>04/06/23 22:05</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M8" t="str">
-        <v>$2,400 as of 7/20/2023 6:09:40 PM</v>
+        <v>$1,940 as of 4/6/2023 8:05:45 PM</v>
       </c>
       <c r="N8">
-        <v>2500</v>
+        <v>1960</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -645,34 +645,34 @@
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>L474792</v>
+        <v>L678988</v>
       </c>
       <c r="C9" t="str">
-        <v>NICK SHELL SERVICE</v>
+        <v>PAYELESS MARKET</v>
       </c>
       <c r="E9">
-        <v>2540</v>
+        <v>2400</v>
       </c>
       <c r="F9" t="str">
         <v>T</v>
       </c>
-      <c r="H9">
-        <v>45251.0418602662</v>
+      <c r="I9" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J9" t="str">
-        <v>11/08/23 12:46</v>
+        <v>07/20/23 20:09</v>
       </c>
       <c r="K9" t="str">
-        <v>11/08/23 12:46</v>
+        <v>07/20/23 20:09</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9" t="str">
-        <v>$2,540 as of 11/8/2023 10:46:48 AM</v>
+        <v>$2,400 as of 7/20/2023 6:09:40 PM</v>
       </c>
       <c r="N9">
-        <v>2600</v>
+        <v>2500</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -686,34 +686,34 @@
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>L662336</v>
+        <v>LK561655</v>
       </c>
       <c r="C10" t="str">
-        <v>SB#4 MONA MARKET</v>
+        <v>CRENSHAW CRAVOR #2</v>
       </c>
       <c r="E10">
-        <v>2560</v>
+        <v>2780</v>
       </c>
       <c r="F10" t="str">
         <v>T</v>
       </c>
-      <c r="H10">
-        <v>45250.0418602662</v>
+      <c r="I10" t="str">
+        <v>ATM Inactive greater than 48 minutes</v>
       </c>
       <c r="J10" t="str">
-        <v>11/08/23 17:02</v>
+        <v>01/23/20 08:24</v>
       </c>
       <c r="K10" t="str">
-        <v>11/08/23 17:02</v>
+        <v>01/23/20 08:24</v>
       </c>
       <c r="L10">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="M10" t="str">
-        <v>$3,180 as of 11/8/2023 7:54:25 AM</v>
+        <v>$2,780 as of 1/23/2020 6:24:32 AM</v>
       </c>
       <c r="N10">
-        <v>2640</v>
+        <v>2800</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -727,34 +727,34 @@
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>LK561655</v>
+        <v>L476340</v>
       </c>
       <c r="C11" t="str">
-        <v>CRENSHAW CRAVOR #2</v>
+        <v>DONUT &amp; SANDWICH</v>
       </c>
       <c r="E11">
-        <v>2780</v>
+        <v>2960</v>
       </c>
       <c r="F11" t="str">
         <v>T</v>
       </c>
-      <c r="I11" t="str">
-        <v>ATM Inactive greater than 48 minutes</v>
+      <c r="H11">
+        <v>45276.04188596064</v>
       </c>
       <c r="J11" t="str">
-        <v>01/23/20 08:24</v>
+        <v>11/27/23 20:17</v>
       </c>
       <c r="K11" t="str">
-        <v>01/23/20 08:24</v>
+        <v>11/27/23 20:17</v>
       </c>
       <c r="L11">
         <v>0</v>
       </c>
       <c r="M11" t="str">
-        <v>$2,780 as of 1/23/2020 6:24:32 AM</v>
+        <v>$3,360 as of 11/27/2023 10:55:14 AM</v>
       </c>
       <c r="N11">
-        <v>2800</v>
+        <v>2980</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -768,34 +768,34 @@
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>L475090</v>
+        <v>L474746</v>
       </c>
       <c r="C12" t="str">
-        <v>S.B. 2</v>
+        <v>ZACATES MARKET</v>
       </c>
       <c r="E12">
-        <v>2840</v>
+        <v>3780</v>
       </c>
       <c r="F12" t="str">
         <v>T</v>
       </c>
       <c r="H12">
-        <v>45241.0418602662</v>
+        <v>45279.04188596064</v>
       </c>
       <c r="J12" t="str">
-        <v>11/08/23 19:47</v>
+        <v>11/27/23 18:02</v>
       </c>
       <c r="K12" t="str">
-        <v>11/08/23 19:03</v>
+        <v>11/27/23 18:02</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
       <c r="M12" t="str">
-        <v>$3,220 as of 11/8/2023 9:27:02 AM</v>
+        <v>$3,920 as of 11/27/2023 11:30:17 AM</v>
       </c>
       <c r="N12">
-        <v>2840</v>
+        <v>3820</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -809,34 +809,34 @@
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>L474746</v>
+        <v>L475182</v>
       </c>
       <c r="C13" t="str">
-        <v>ZACATES MARKET</v>
+        <v>LA ESQUINA DE ORO</v>
       </c>
       <c r="E13">
-        <v>2960</v>
+        <v>3800</v>
       </c>
       <c r="F13" t="str">
         <v>T</v>
       </c>
-      <c r="H13">
-        <v>45247.0418602662</v>
+      <c r="I13" t="str">
+        <v>ATM Inactive greater than 48 minutes</v>
       </c>
       <c r="J13" t="str">
-        <v>11/08/23 13:39</v>
+        <v>09/16/20 16:57</v>
       </c>
       <c r="K13" t="str">
-        <v>11/08/23 13:36</v>
+        <v>09/15/20 23:38</v>
       </c>
       <c r="L13">
         <v>0</v>
       </c>
       <c r="M13" t="str">
-        <v>$2,960 as of 11/8/2023 11:36:06 AM</v>
+        <v>$3,800 as of 9/16/2020 1:28:00 PM</v>
       </c>
       <c r="N13">
-        <v>2960</v>
+        <v>3800</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -850,34 +850,34 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>LK864765</v>
+        <v>L688966</v>
       </c>
       <c r="C14" t="str">
-        <v>SKY LIQUOR</v>
+        <v>S B WESTERN 108TH MARKET</v>
       </c>
       <c r="E14">
-        <v>3400</v>
+        <v>3920</v>
       </c>
       <c r="F14" t="str">
         <v>T</v>
       </c>
       <c r="H14">
-        <v>45243.0418602662</v>
+        <v>45269.04188596064</v>
       </c>
       <c r="J14" t="str">
-        <v>11/08/23 17:12</v>
+        <v>11/27/23 16:46</v>
       </c>
       <c r="K14" t="str">
-        <v>11/08/23 17:12</v>
+        <v>11/27/23 16:02</v>
       </c>
       <c r="L14">
         <v>80</v>
       </c>
       <c r="M14" t="str">
-        <v>$3,840 as of 11/8/2023 11:37:39 AM</v>
+        <v>$4,080 as of 11/27/2023 10:11:00 AM</v>
       </c>
       <c r="N14">
-        <v>3500</v>
+        <v>3920</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -891,34 +891,34 @@
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>L475182</v>
+        <v>L688961</v>
       </c>
       <c r="C15" t="str">
-        <v>LA ESQUINA DE ORO</v>
+        <v>MONA MART</v>
       </c>
       <c r="E15">
-        <v>3800</v>
+        <v>4000</v>
       </c>
       <c r="F15" t="str">
         <v>T</v>
       </c>
       <c r="I15" t="str">
-        <v>ATM Inactive greater than 48 minutes</v>
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J15" t="str">
-        <v>09/16/20 16:57</v>
+        <v>10/17/23 13:26</v>
       </c>
       <c r="K15" t="str">
-        <v>09/15/20 23:38</v>
+        <v>10/17/23 13:00</v>
       </c>
       <c r="L15">
         <v>0</v>
       </c>
       <c r="M15" t="str">
-        <v>$3,800 as of 9/16/2020 1:28:00 PM</v>
+        <v>$4,000 as of 10/17/2023 11:00:09 AM</v>
       </c>
       <c r="N15">
-        <v>3800</v>
+        <v>4000</v>
       </c>
       <c r="O15">
         <v>0</v>
@@ -932,34 +932,37 @@
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>L697590</v>
+        <v>L474761</v>
       </c>
       <c r="C16" t="str">
-        <v>S B MARKET ST</v>
+        <v>BABS MARKET</v>
       </c>
       <c r="E16">
-        <v>3820</v>
+        <v>4580</v>
       </c>
       <c r="F16" t="str">
         <v>T</v>
       </c>
       <c r="H16">
-        <v>45260.0418602662</v>
+        <v>45275.04188596064</v>
+      </c>
+      <c r="I16" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J16" t="str">
-        <v>11/08/23 19:38</v>
+        <v>11/26/23 14:13</v>
       </c>
       <c r="K16" t="str">
-        <v>11/08/23 17:11</v>
+        <v>11/26/23 14:13</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M16" t="str">
-        <v>$4,020 as of 11/8/2023 10:06:15 AM</v>
+        <v>$4,580 as of 11/26/2023 12:13:41 PM</v>
       </c>
       <c r="N16">
-        <v>4020</v>
+        <v>4680</v>
       </c>
       <c r="O16">
         <v>0</v>
@@ -973,34 +976,37 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>L688966</v>
+        <v>LK236828</v>
       </c>
       <c r="C17" t="str">
-        <v>S B WESTERN 108TH MARKET</v>
+        <v>WORLDWIDE AUTOMOTIVE</v>
       </c>
       <c r="E17">
-        <v>3880</v>
+        <v>4620</v>
       </c>
       <c r="F17" t="str">
         <v>T</v>
       </c>
       <c r="H17">
-        <v>45245.0418602662</v>
+        <v>45277.04188596064</v>
+      </c>
+      <c r="I17" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J17" t="str">
-        <v>11/08/23 19:10</v>
+        <v>11/26/23 11:27</v>
       </c>
       <c r="K17" t="str">
-        <v>11/08/23 19:10</v>
+        <v>11/26/23 11:27</v>
       </c>
       <c r="L17">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="M17" t="str">
-        <v>$4,360 as of 11/8/2023 10:31:03 AM</v>
+        <v>$4,620 as of 11/26/2023 9:27:11 AM</v>
       </c>
       <c r="N17">
-        <v>3840</v>
+        <v>4820</v>
       </c>
       <c r="O17">
         <v>0</v>
@@ -1014,34 +1020,34 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>L688961</v>
+        <v>L475090</v>
       </c>
       <c r="C18" t="str">
-        <v>MONA MART</v>
+        <v>S.B. 2</v>
       </c>
       <c r="E18">
-        <v>4000</v>
+        <v>4660</v>
       </c>
       <c r="F18" t="str">
         <v>T</v>
       </c>
-      <c r="I18" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+      <c r="H18">
+        <v>45270.04188596064</v>
       </c>
       <c r="J18" t="str">
-        <v>10/17/23 13:26</v>
+        <v>11/27/23 19:46</v>
       </c>
       <c r="K18" t="str">
-        <v>10/17/23 13:00</v>
+        <v>11/27/23 19:46</v>
       </c>
       <c r="L18">
         <v>0</v>
       </c>
       <c r="M18" t="str">
-        <v>$4,000 as of 10/17/2023 11:00:09 AM</v>
+        <v>$4,900 as of 11/27/2023 10:56:51 AM</v>
       </c>
       <c r="N18">
-        <v>4000</v>
+        <v>4700</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -1055,34 +1061,37 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>LK236828</v>
+        <v>L474792</v>
       </c>
       <c r="C19" t="str">
-        <v>WORLDWIDE AUTOMOTIVE</v>
+        <v>NICK SHELL SERVICE</v>
       </c>
       <c r="E19">
-        <v>4740</v>
+        <v>4700</v>
       </c>
       <c r="F19" t="str">
         <v>T</v>
       </c>
       <c r="H19">
-        <v>45260.0418602662</v>
+        <v>45305.04188596064</v>
+      </c>
+      <c r="I19" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J19" t="str">
-        <v>11/08/23 17:48</v>
+        <v>11/26/23 15:22</v>
       </c>
       <c r="K19" t="str">
-        <v>11/08/23 17:48</v>
+        <v>11/26/23 15:22</v>
       </c>
       <c r="L19">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="M19" t="str">
-        <v>$4,840 as of 11/8/2023 10:15:56 AM</v>
+        <v>$4,700 as of 11/26/2023 1:22:02 PM</v>
       </c>
       <c r="N19">
-        <v>4840</v>
+        <v>4900</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -1096,34 +1105,34 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>L474761</v>
+        <v>L662336</v>
       </c>
       <c r="C20" t="str">
-        <v>BABS MARKET</v>
+        <v>SB#4 MONA MARKET</v>
       </c>
       <c r="E20">
-        <v>4960</v>
+        <v>6140</v>
       </c>
       <c r="F20" t="str">
         <v>T</v>
       </c>
       <c r="H20">
-        <v>45261.0418602662</v>
+        <v>45284.04188596064</v>
       </c>
       <c r="J20" t="str">
-        <v>11/08/23 17:33</v>
+        <v>11/27/23 20:55</v>
       </c>
       <c r="K20" t="str">
-        <v>11/08/23 17:33</v>
+        <v>11/27/23 20:55</v>
       </c>
       <c r="L20">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="M20" t="str">
-        <v>$5,160 as of 11/7/2023 11:51:10 AM</v>
+        <v>$6,280 as of 11/27/2023 10:48:09 AM</v>
       </c>
       <c r="N20">
-        <v>5120</v>
+        <v>6280</v>
       </c>
       <c r="O20">
         <v>0</v>
@@ -1137,34 +1146,34 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>L474817</v>
+        <v>L697590</v>
       </c>
       <c r="C21" t="str">
-        <v>SAFETY MARKET</v>
+        <v>S B MARKET ST</v>
       </c>
       <c r="E21">
-        <v>5660</v>
+        <v>6340</v>
       </c>
       <c r="F21" t="str">
         <v>T</v>
       </c>
       <c r="H21">
-        <v>45245.0418602662</v>
+        <v>45291.04188596064</v>
       </c>
       <c r="J21" t="str">
-        <v>11/08/23 18:26</v>
+        <v>11/27/23 18:33</v>
       </c>
       <c r="K21" t="str">
-        <v>11/08/23 18:26</v>
+        <v>11/27/23 13:55</v>
       </c>
       <c r="L21">
-        <v>120</v>
+        <v>20</v>
       </c>
       <c r="M21" t="str">
-        <v>$5,820 as of 11/8/2023 10:55:36 AM</v>
+        <v>$6,360 as of 11/27/2023 10:39:52 AM</v>
       </c>
       <c r="N21">
-        <v>5760</v>
+        <v>6340</v>
       </c>
       <c r="O21">
         <v>0</v>
@@ -1178,34 +1187,34 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>L704741</v>
+        <v>L682801</v>
       </c>
       <c r="C22" t="str">
-        <v>W ADAMS COIN LAUNDRY</v>
+        <v>SB#5</v>
       </c>
       <c r="E22">
-        <v>7780</v>
+        <v>7840</v>
       </c>
       <c r="F22" t="str">
         <v>T</v>
       </c>
-      <c r="H22">
-        <v>45248.0418602662</v>
+      <c r="I22" t="str">
+        <v>ATM Inactive greater than 2000 minutes</v>
       </c>
       <c r="J22" t="str">
-        <v>11/08/23 17:29</v>
+        <v>09/28/23 15:22</v>
       </c>
       <c r="K22" t="str">
-        <v>11/08/23 17:29</v>
+        <v>09/28/23 12:14</v>
       </c>
       <c r="L22">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="M22" t="str">
-        <v>$8,040 as of 11/8/2023 11:37:41 AM</v>
+        <v>$7,840 as of 9/28/2023 12:31:50 PM</v>
       </c>
       <c r="N22">
-        <v>7800</v>
+        <v>7840</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -1219,34 +1228,34 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>L476340</v>
+        <v>L704741</v>
       </c>
       <c r="C23" t="str">
-        <v>DONUT &amp; SANDWICH</v>
+        <v>W ADAMS COIN LAUNDRY</v>
       </c>
       <c r="E23">
-        <v>7840</v>
+        <v>8540</v>
       </c>
       <c r="F23" t="str">
         <v>T</v>
       </c>
       <c r="H23">
-        <v>45265.0418602662</v>
+        <v>45269.04188596064</v>
       </c>
       <c r="J23" t="str">
-        <v>11/08/23 11:55</v>
+        <v>11/28/23 01:49</v>
       </c>
       <c r="K23" t="str">
-        <v>11/08/23 11:55</v>
+        <v>11/28/23 01:49</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="M23" t="str">
-        <v>$7,840 as of 11/8/2023 9:55:43 AM</v>
+        <v>$8,820 as of 11/27/2023 10:41:06 AM</v>
       </c>
       <c r="N23">
-        <v>7860</v>
+        <v>8560</v>
       </c>
       <c r="O23">
         <v>0</v>
@@ -1260,34 +1269,34 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>L682801</v>
+        <v>LK864765</v>
       </c>
       <c r="C24" t="str">
-        <v>SB#5</v>
+        <v>SKY LIQUOR</v>
       </c>
       <c r="E24">
-        <v>7840</v>
+        <v>10200</v>
       </c>
       <c r="F24" t="str">
         <v>T</v>
       </c>
-      <c r="I24" t="str">
-        <v>ATM Inactive greater than 2000 minutes</v>
+      <c r="H24">
+        <v>45277.04188596064</v>
       </c>
       <c r="J24" t="str">
-        <v>09/28/23 15:22</v>
+        <v>11/28/23 01:48</v>
       </c>
       <c r="K24" t="str">
-        <v>09/28/23 12:14</v>
+        <v>11/28/23 01:10</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="M24" t="str">
-        <v>$7,840 as of 9/28/2023 12:31:50 PM</v>
+        <v>$10,320 as of 11/27/2023 10:17:13 AM</v>
       </c>
       <c r="N24">
-        <v>7840</v>
+        <v>10200</v>
       </c>
       <c r="O24">
         <v>0</v>
@@ -1301,34 +1310,34 @@
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>LK923383</v>
+        <v>L697589</v>
       </c>
       <c r="C25" t="str">
-        <v>SAMYS PHONE CARDS</v>
+        <v>S B DISCOUNT MART</v>
       </c>
       <c r="E25">
-        <v>10460</v>
+        <v>10880</v>
       </c>
       <c r="F25" t="str">
         <v>T</v>
       </c>
       <c r="H25">
-        <v>45261.0418602662</v>
+        <v>45271.04188596064</v>
       </c>
       <c r="J25" t="str">
-        <v>11/08/23 17:39</v>
+        <v>11/28/23 00:34</v>
       </c>
       <c r="K25" t="str">
-        <v>11/08/23 17:39</v>
+        <v>11/28/23 00:34</v>
       </c>
       <c r="L25">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="M25" t="str">
-        <v>$10,520 as of 11/8/2023 11:38:10 AM</v>
+        <v>$11,940 as of 11/27/2023 10:07:09 AM</v>
       </c>
       <c r="N25">
-        <v>10500</v>
+        <v>10920</v>
       </c>
       <c r="O25">
         <v>0</v>
@@ -1348,28 +1357,28 @@
         <v>98 DISCOUNT STORE</v>
       </c>
       <c r="E26">
-        <v>10920</v>
+        <v>11380</v>
       </c>
       <c r="F26" t="str">
         <v>T</v>
       </c>
       <c r="H26">
-        <v>45245.0418602662</v>
+        <v>45269.04188596064</v>
       </c>
       <c r="J26" t="str">
-        <v>11/08/23 19:37</v>
+        <v>11/28/23 01:37</v>
       </c>
       <c r="K26" t="str">
-        <v>11/08/23 19:14</v>
+        <v>11/28/23 01:37</v>
       </c>
       <c r="L26">
         <v>0</v>
       </c>
       <c r="M26" t="str">
-        <v>$11,360 as of 11/8/2023 11:41:50 AM</v>
+        <v>$12,560 as of 11/27/2023 10:33:36 AM</v>
       </c>
       <c r="N26">
-        <v>10920</v>
+        <v>11460</v>
       </c>
       <c r="O26">
         <v>0</v>
@@ -1383,34 +1392,34 @@
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>L697589</v>
+        <v>LK923383</v>
       </c>
       <c r="C27" t="str">
-        <v>S B DISCOUNT MART</v>
+        <v>SAMYS PHONE CARDS</v>
       </c>
       <c r="E27">
-        <v>13920</v>
+        <v>14240</v>
       </c>
       <c r="F27" t="str">
         <v>T</v>
       </c>
       <c r="H27">
-        <v>45246.0418602662</v>
+        <v>45284.04188596064</v>
       </c>
       <c r="J27" t="str">
-        <v>11/08/23 19:03</v>
+        <v>11/27/23 20:44</v>
       </c>
       <c r="K27" t="str">
-        <v>11/08/23 19:03</v>
+        <v>11/27/23 20:44</v>
       </c>
       <c r="L27">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="M27" t="str">
-        <v>$14,140 as of 11/8/2023 11:40:47 AM</v>
+        <v>$14,580 as of 11/26/2023 7:43:20 PM</v>
       </c>
       <c r="N27">
-        <v>14120</v>
+        <v>14280</v>
       </c>
       <c r="O27">
         <v>0</v>
@@ -1427,7 +1436,7 @@
         <v>Total Outstanding Cash Balance:</v>
       </c>
       <c r="E28">
-        <v>115540</v>
+        <v>123600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>